<commit_message>
Atualização de dados automática em 2024-12-16 12:30:03 (cron)
</commit_message>
<xml_diff>
--- a/public/docs/index_07_dim_CG.xlsx
+++ b/public/docs/index_07_dim_CG.xlsx
@@ -82927,98 +82927,98 @@
     </row>
     <row r="2273">
       <c r="A2273" t="s">
-        <v>623</v>
+        <v>619</v>
       </c>
       <c r="B2273" s="1" t="n">
         <v>45657</v>
       </c>
       <c r="C2273" s="1" t="n">
-        <v>45504</v>
+        <v>45636</v>
       </c>
       <c r="D2273" t="s">
-        <v>624</v>
+        <v>620</v>
       </c>
       <c r="E2273" t="n">
-        <v>0.696969696969697</v>
+        <v>0.575757575757576</v>
       </c>
       <c r="F2273" t="n">
-        <v>0.545454545454545</v>
+        <v>0.757575757575758</v>
       </c>
       <c r="G2273" t="n">
-        <v>0.5</v>
+        <v>0.541666666666667</v>
       </c>
       <c r="H2273" t="n">
         <v>0.571428571428571</v>
       </c>
       <c r="I2273" t="n">
-        <v>0.133333333333333</v>
+        <v>0.0666666666666667</v>
       </c>
       <c r="J2273" t="n">
-        <v>0.0666666666666667</v>
+        <v>0.2</v>
       </c>
       <c r="K2273" t="n">
-        <v>0.428571428571429</v>
+        <v>0.523809523809524</v>
       </c>
     </row>
     <row r="2274">
       <c r="A2274" t="s">
-        <v>627</v>
+        <v>623</v>
       </c>
       <c r="B2274" s="1" t="n">
         <v>45657</v>
       </c>
       <c r="C2274" s="1" t="n">
-        <v>45470</v>
+        <v>45504</v>
       </c>
       <c r="D2274" t="s">
-        <v>628</v>
+        <v>624</v>
       </c>
       <c r="E2274" t="n">
-        <v>0.636363636363636</v>
+        <v>0.696969696969697</v>
       </c>
       <c r="F2274" t="n">
-        <v>0.757575757575758</v>
+        <v>0.545454545454545</v>
       </c>
       <c r="G2274" t="n">
-        <v>0.541666666666667</v>
+        <v>0.5</v>
       </c>
       <c r="H2274" t="n">
-        <v>0.333333333333333</v>
+        <v>0.571428571428571</v>
       </c>
       <c r="I2274" t="n">
         <v>0.133333333333333</v>
       </c>
       <c r="J2274" t="n">
-        <v>0</v>
+        <v>0.0666666666666667</v>
       </c>
       <c r="K2274" t="n">
-        <v>0.571428571428571</v>
+        <v>0.428571428571429</v>
       </c>
     </row>
     <row r="2275">
       <c r="A2275" t="s">
-        <v>631</v>
+        <v>627</v>
       </c>
       <c r="B2275" s="1" t="n">
         <v>45657</v>
       </c>
       <c r="C2275" s="1" t="n">
-        <v>45502</v>
+        <v>45470</v>
       </c>
       <c r="D2275" t="s">
-        <v>632</v>
+        <v>628</v>
       </c>
       <c r="E2275" t="n">
-        <v>0.454545454545455</v>
+        <v>0.636363636363636</v>
       </c>
       <c r="F2275" t="n">
-        <v>0.606060606060606</v>
+        <v>0.757575757575758</v>
       </c>
       <c r="G2275" t="n">
-        <v>0.625</v>
+        <v>0.541666666666667</v>
       </c>
       <c r="H2275" t="n">
-        <v>0.571428571428571</v>
+        <v>0.333333333333333</v>
       </c>
       <c r="I2275" t="n">
         <v>0.133333333333333</v>
@@ -83027,39 +83027,39 @@
         <v>0</v>
       </c>
       <c r="K2275" t="n">
-        <v>0.285714285714286</v>
+        <v>0.571428571428571</v>
       </c>
     </row>
     <row r="2276">
       <c r="A2276" t="s">
-        <v>936</v>
+        <v>631</v>
       </c>
       <c r="B2276" s="1" t="n">
         <v>45657</v>
       </c>
       <c r="C2276" s="1" t="n">
-        <v>45504</v>
+        <v>45502</v>
       </c>
       <c r="D2276" t="s">
-        <v>937</v>
+        <v>632</v>
       </c>
       <c r="E2276" t="n">
+        <v>0.454545454545455</v>
+      </c>
+      <c r="F2276" t="n">
         <v>0.606060606060606</v>
       </c>
-      <c r="F2276" t="n">
-        <v>0.696969696969697</v>
-      </c>
       <c r="G2276" t="n">
-        <v>0.666666666666667</v>
+        <v>0.625</v>
       </c>
       <c r="H2276" t="n">
         <v>0.571428571428571</v>
       </c>
       <c r="I2276" t="n">
-        <v>0.4</v>
+        <v>0.133333333333333</v>
       </c>
       <c r="J2276" t="n">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="K2276" t="n">
         <v>0.285714285714286</v>
@@ -83067,60 +83067,60 @@
     </row>
     <row r="2277">
       <c r="A2277" t="s">
-        <v>809</v>
+        <v>936</v>
       </c>
       <c r="B2277" s="1" t="n">
-        <v>45351</v>
+        <v>45657</v>
       </c>
       <c r="C2277" s="1" t="n">
-        <v>45198</v>
+        <v>45504</v>
       </c>
       <c r="D2277" t="s">
-        <v>810</v>
+        <v>937</v>
       </c>
       <c r="E2277" t="n">
-        <v>0.666666666666667</v>
+        <v>0.606060606060606</v>
       </c>
       <c r="F2277" t="n">
         <v>0.696969696969697</v>
       </c>
       <c r="G2277" t="n">
-        <v>0.583333333333333</v>
+        <v>0.666666666666667</v>
       </c>
       <c r="H2277" t="n">
         <v>0.571428571428571</v>
       </c>
       <c r="I2277" t="n">
-        <v>0.266666666666667</v>
+        <v>0.4</v>
       </c>
       <c r="J2277" t="n">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="K2277" t="n">
-        <v>0.571428571428571</v>
+        <v>0.285714285714286</v>
       </c>
     </row>
     <row r="2278">
       <c r="A2278" t="s">
-        <v>651</v>
+        <v>809</v>
       </c>
       <c r="B2278" s="1" t="n">
-        <v>45657</v>
+        <v>45351</v>
       </c>
       <c r="C2278" s="1" t="n">
-        <v>45499</v>
+        <v>45198</v>
       </c>
       <c r="D2278" t="s">
-        <v>652</v>
+        <v>810</v>
       </c>
       <c r="E2278" t="n">
-        <v>0.636363636363636</v>
+        <v>0.666666666666667</v>
       </c>
       <c r="F2278" t="n">
-        <v>0.727272727272727</v>
+        <v>0.696969696969697</v>
       </c>
       <c r="G2278" t="n">
-        <v>0.541666666666667</v>
+        <v>0.583333333333333</v>
       </c>
       <c r="H2278" t="n">
         <v>0.571428571428571</v>
@@ -83129,7 +83129,7 @@
         <v>0.266666666666667</v>
       </c>
       <c r="J2278" t="n">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="K2278" t="n">
         <v>0.571428571428571</v>
@@ -83137,19 +83137,19 @@
     </row>
     <row r="2279">
       <c r="A2279" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="B2279" s="1" t="n">
         <v>45657</v>
       </c>
       <c r="C2279" s="1" t="n">
-        <v>45504</v>
+        <v>45499</v>
       </c>
       <c r="D2279" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="E2279" t="n">
-        <v>0.515151515151515</v>
+        <v>0.636363636363636</v>
       </c>
       <c r="F2279" t="n">
         <v>0.727272727272727</v>
@@ -83161,179 +83161,179 @@
         <v>0.571428571428571</v>
       </c>
       <c r="I2279" t="n">
-        <v>0.133333333333333</v>
+        <v>0.266666666666667</v>
       </c>
       <c r="J2279" t="n">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="K2279" t="n">
-        <v>0.619047619047619</v>
+        <v>0.571428571428571</v>
       </c>
     </row>
     <row r="2280">
       <c r="A2280" t="s">
-        <v>996</v>
+        <v>653</v>
       </c>
       <c r="B2280" s="1" t="n">
-        <v>45473</v>
+        <v>45657</v>
       </c>
       <c r="C2280" s="1" t="n">
-        <v>45322</v>
+        <v>45504</v>
       </c>
       <c r="D2280" t="s">
-        <v>997</v>
+        <v>654</v>
       </c>
       <c r="E2280" t="n">
-        <v>0.575757575757576</v>
+        <v>0.515151515151515</v>
       </c>
       <c r="F2280" t="n">
-        <v>0.696969696969697</v>
+        <v>0.727272727272727</v>
       </c>
       <c r="G2280" t="n">
-        <v>0.416666666666667</v>
+        <v>0.541666666666667</v>
       </c>
       <c r="H2280" t="n">
-        <v>0.476190476190476</v>
+        <v>0.571428571428571</v>
       </c>
       <c r="I2280" t="n">
         <v>0.133333333333333</v>
       </c>
       <c r="J2280" t="n">
-        <v>0.733333333333333</v>
+        <v>0.4</v>
       </c>
       <c r="K2280" t="n">
-        <v>0.666666666666667</v>
+        <v>0.619047619047619</v>
       </c>
     </row>
     <row r="2281">
       <c r="A2281" t="s">
-        <v>659</v>
+        <v>996</v>
       </c>
       <c r="B2281" s="1" t="n">
-        <v>45657</v>
+        <v>45473</v>
       </c>
       <c r="C2281" s="1" t="n">
-        <v>45504</v>
+        <v>45322</v>
       </c>
       <c r="D2281" t="s">
-        <v>660</v>
+        <v>997</v>
       </c>
       <c r="E2281" t="n">
-        <v>0.606060606060606</v>
+        <v>0.575757575757576</v>
       </c>
       <c r="F2281" t="n">
-        <v>0.606060606060606</v>
+        <v>0.696969696969697</v>
       </c>
       <c r="G2281" t="n">
-        <v>0.458333333333333</v>
+        <v>0.416666666666667</v>
       </c>
       <c r="H2281" t="n">
-        <v>0.571428571428571</v>
+        <v>0.476190476190476</v>
       </c>
       <c r="I2281" t="n">
-        <v>0.2</v>
+        <v>0.133333333333333</v>
       </c>
       <c r="J2281" t="n">
-        <v>0.2</v>
+        <v>0.733333333333333</v>
       </c>
       <c r="K2281" t="n">
-        <v>0.571428571428571</v>
+        <v>0.666666666666667</v>
       </c>
     </row>
     <row r="2282">
       <c r="A2282" t="s">
-        <v>669</v>
+        <v>659</v>
       </c>
       <c r="B2282" s="1" t="n">
         <v>45657</v>
       </c>
       <c r="C2282" s="1" t="n">
-        <v>45503</v>
+        <v>45504</v>
       </c>
       <c r="D2282" t="s">
-        <v>670</v>
+        <v>660</v>
       </c>
       <c r="E2282" t="n">
-        <v>0.545454545454545</v>
+        <v>0.606060606060606</v>
       </c>
       <c r="F2282" t="n">
-        <v>0.545454545454545</v>
+        <v>0.606060606060606</v>
       </c>
       <c r="G2282" t="n">
-        <v>0.375</v>
+        <v>0.458333333333333</v>
       </c>
       <c r="H2282" t="n">
-        <v>0.380952380952381</v>
+        <v>0.571428571428571</v>
       </c>
       <c r="I2282" t="n">
-        <v>0.133333333333333</v>
+        <v>0.2</v>
       </c>
       <c r="J2282" t="n">
-        <v>0.0666666666666667</v>
+        <v>0.2</v>
       </c>
       <c r="K2282" t="n">
-        <v>0.476190476190476</v>
+        <v>0.571428571428571</v>
       </c>
     </row>
     <row r="2283">
       <c r="A2283" t="s">
-        <v>675</v>
+        <v>669</v>
       </c>
       <c r="B2283" s="1" t="n">
         <v>45657</v>
       </c>
       <c r="C2283" s="1" t="n">
-        <v>45467</v>
+        <v>45503</v>
       </c>
       <c r="D2283" t="s">
-        <v>676</v>
+        <v>670</v>
       </c>
       <c r="E2283" t="n">
-        <v>0.484848484848485</v>
+        <v>0.545454545454545</v>
       </c>
       <c r="F2283" t="n">
-        <v>0.484848484848485</v>
+        <v>0.545454545454545</v>
       </c>
       <c r="G2283" t="n">
-        <v>0.458333333333333</v>
+        <v>0.375</v>
       </c>
       <c r="H2283" t="n">
+        <v>0.380952380952381</v>
+      </c>
+      <c r="I2283" t="n">
+        <v>0.133333333333333</v>
+      </c>
+      <c r="J2283" t="n">
+        <v>0.0666666666666667</v>
+      </c>
+      <c r="K2283" t="n">
         <v>0.476190476190476</v>
-      </c>
-      <c r="I2283" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="J2283" t="n">
-        <v>0.133333333333333</v>
-      </c>
-      <c r="K2283" t="n">
-        <v>0.523809523809524</v>
       </c>
     </row>
     <row r="2284">
       <c r="A2284" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
       <c r="B2284" s="1" t="n">
-        <v>45322</v>
+        <v>45657</v>
       </c>
       <c r="C2284" s="1" t="n">
-        <v>45504</v>
+        <v>45467</v>
       </c>
       <c r="D2284" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="E2284" t="n">
-        <v>0.606060606060606</v>
+        <v>0.484848484848485</v>
       </c>
       <c r="F2284" t="n">
-        <v>0.696969696969697</v>
+        <v>0.484848484848485</v>
       </c>
       <c r="G2284" t="n">
-        <v>0.5</v>
+        <v>0.458333333333333</v>
       </c>
       <c r="H2284" t="n">
-        <v>0.571428571428571</v>
+        <v>0.476190476190476</v>
       </c>
       <c r="I2284" t="n">
         <v>0.2</v>
@@ -83342,27 +83342,27 @@
         <v>0.133333333333333</v>
       </c>
       <c r="K2284" t="n">
-        <v>0.476190476190476</v>
+        <v>0.523809523809524</v>
       </c>
     </row>
     <row r="2285">
       <c r="A2285" t="s">
-        <v>679</v>
+        <v>677</v>
       </c>
       <c r="B2285" s="1" t="n">
-        <v>45657</v>
+        <v>45322</v>
       </c>
       <c r="C2285" s="1" t="n">
-        <v>45490</v>
+        <v>45504</v>
       </c>
       <c r="D2285" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="E2285" t="n">
-        <v>0.636363636363636</v>
+        <v>0.606060606060606</v>
       </c>
       <c r="F2285" t="n">
-        <v>0.666666666666667</v>
+        <v>0.696969696969697</v>
       </c>
       <c r="G2285" t="n">
         <v>0.5</v>
@@ -83371,123 +83371,123 @@
         <v>0.571428571428571</v>
       </c>
       <c r="I2285" t="n">
-        <v>0.666666666666667</v>
+        <v>0.2</v>
       </c>
       <c r="J2285" t="n">
-        <v>0.4</v>
+        <v>0.133333333333333</v>
       </c>
       <c r="K2285" t="n">
-        <v>0.619047619047619</v>
+        <v>0.476190476190476</v>
       </c>
     </row>
     <row r="2286">
       <c r="A2286" t="s">
-        <v>683</v>
+        <v>679</v>
       </c>
       <c r="B2286" s="1" t="n">
         <v>45657</v>
       </c>
       <c r="C2286" s="1" t="n">
-        <v>45503</v>
+        <v>45490</v>
       </c>
       <c r="D2286" t="s">
-        <v>684</v>
+        <v>680</v>
       </c>
       <c r="E2286" t="n">
-        <v>0.424242424242424</v>
+        <v>0.636363636363636</v>
       </c>
       <c r="F2286" t="n">
-        <v>0.545454545454545</v>
+        <v>0.666666666666667</v>
       </c>
       <c r="G2286" t="n">
-        <v>0.416666666666667</v>
+        <v>0.5</v>
       </c>
       <c r="H2286" t="n">
+        <v>0.571428571428571</v>
+      </c>
+      <c r="I2286" t="n">
+        <v>0.666666666666667</v>
+      </c>
+      <c r="J2286" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="K2286" t="n">
         <v>0.619047619047619</v>
-      </c>
-      <c r="I2286" t="n">
-        <v>0.133333333333333</v>
-      </c>
-      <c r="J2286" t="n">
-        <v>0.333333333333333</v>
-      </c>
-      <c r="K2286" t="n">
-        <v>0.380952380952381</v>
       </c>
     </row>
     <row r="2287">
       <c r="A2287" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
       <c r="B2287" s="1" t="n">
         <v>45657</v>
       </c>
       <c r="C2287" s="1" t="n">
-        <v>45504</v>
+        <v>45503</v>
       </c>
       <c r="D2287" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
       <c r="E2287" t="n">
-        <v>0.575757575757576</v>
+        <v>0.424242424242424</v>
       </c>
       <c r="F2287" t="n">
-        <v>0.454545454545455</v>
+        <v>0.545454545454545</v>
       </c>
       <c r="G2287" t="n">
         <v>0.416666666666667</v>
       </c>
       <c r="H2287" t="n">
-        <v>0.476190476190476</v>
+        <v>0.619047619047619</v>
       </c>
       <c r="I2287" t="n">
-        <v>0.2</v>
+        <v>0.133333333333333</v>
       </c>
       <c r="J2287" t="n">
-        <v>0.4</v>
+        <v>0.333333333333333</v>
       </c>
       <c r="K2287" t="n">
-        <v>0.571428571428571</v>
+        <v>0.380952380952381</v>
       </c>
     </row>
     <row r="2288">
       <c r="A2288" t="s">
-        <v>689</v>
+        <v>685</v>
       </c>
       <c r="B2288" s="1" t="n">
         <v>45657</v>
       </c>
       <c r="C2288" s="1" t="n">
-        <v>45503</v>
+        <v>45504</v>
       </c>
       <c r="D2288" t="s">
-        <v>690</v>
+        <v>686</v>
       </c>
       <c r="E2288" t="n">
-        <v>0.454545454545455</v>
+        <v>0.575757575757576</v>
       </c>
       <c r="F2288" t="n">
         <v>0.454545454545455</v>
       </c>
       <c r="G2288" t="n">
-        <v>0.333333333333333</v>
+        <v>0.416666666666667</v>
       </c>
       <c r="H2288" t="n">
-        <v>0.571428571428571</v>
+        <v>0.476190476190476</v>
       </c>
       <c r="I2288" t="n">
         <v>0.2</v>
       </c>
       <c r="J2288" t="n">
-        <v>0.266666666666667</v>
+        <v>0.4</v>
       </c>
       <c r="K2288" t="n">
-        <v>0.666666666666667</v>
+        <v>0.571428571428571</v>
       </c>
     </row>
     <row r="2289">
       <c r="A2289" t="s">
-        <v>695</v>
+        <v>689</v>
       </c>
       <c r="B2289" s="1" t="n">
         <v>45657</v>
@@ -83496,165 +83496,165 @@
         <v>45503</v>
       </c>
       <c r="D2289" t="s">
-        <v>696</v>
+        <v>690</v>
       </c>
       <c r="E2289" t="n">
-        <v>0.545454545454545</v>
+        <v>0.454545454545455</v>
       </c>
       <c r="F2289" t="n">
-        <v>0.484848484848485</v>
+        <v>0.454545454545455</v>
       </c>
       <c r="G2289" t="n">
-        <v>0.416666666666667</v>
+        <v>0.333333333333333</v>
       </c>
       <c r="H2289" t="n">
-        <v>0.380952380952381</v>
+        <v>0.571428571428571</v>
       </c>
       <c r="I2289" t="n">
-        <v>0.133333333333333</v>
+        <v>0.2</v>
       </c>
       <c r="J2289" t="n">
-        <v>0.4</v>
+        <v>0.266666666666667</v>
       </c>
       <c r="K2289" t="n">
-        <v>0.571428571428571</v>
+        <v>0.666666666666667</v>
       </c>
     </row>
     <row r="2290">
       <c r="A2290" t="s">
-        <v>233</v>
+        <v>695</v>
       </c>
       <c r="B2290" s="1" t="n">
         <v>45657</v>
       </c>
       <c r="C2290" s="1" t="n">
-        <v>45497</v>
+        <v>45503</v>
       </c>
       <c r="D2290" t="s">
-        <v>234</v>
+        <v>696</v>
       </c>
       <c r="E2290" t="n">
-        <v>0.606060606060606</v>
+        <v>0.545454545454545</v>
       </c>
       <c r="F2290" t="n">
-        <v>0.606060606060606</v>
+        <v>0.484848484848485</v>
       </c>
       <c r="G2290" t="n">
-        <v>0.583333333333333</v>
+        <v>0.416666666666667</v>
       </c>
       <c r="H2290" t="n">
-        <v>0.571428571428571</v>
+        <v>0.380952380952381</v>
       </c>
       <c r="I2290" t="n">
         <v>0.133333333333333</v>
       </c>
       <c r="J2290" t="n">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="K2290" t="n">
-        <v>0.333333333333333</v>
+        <v>0.571428571428571</v>
       </c>
     </row>
     <row r="2291">
       <c r="A2291" t="s">
-        <v>723</v>
+        <v>233</v>
       </c>
       <c r="B2291" s="1" t="n">
         <v>45657</v>
       </c>
       <c r="C2291" s="1" t="n">
-        <v>45472</v>
+        <v>45497</v>
       </c>
       <c r="D2291" t="s">
-        <v>724</v>
+        <v>234</v>
       </c>
       <c r="E2291" t="n">
-        <v>0.666666666666667</v>
+        <v>0.606060606060606</v>
       </c>
       <c r="F2291" t="n">
-        <v>0.666666666666667</v>
+        <v>0.606060606060606</v>
       </c>
       <c r="G2291" t="n">
-        <v>0.375</v>
+        <v>0.583333333333333</v>
       </c>
       <c r="H2291" t="n">
         <v>0.571428571428571</v>
       </c>
       <c r="I2291" t="n">
+        <v>0.133333333333333</v>
+      </c>
+      <c r="J2291" t="n">
+        <v>0</v>
+      </c>
+      <c r="K2291" t="n">
         <v>0.333333333333333</v>
-      </c>
-      <c r="J2291" t="n">
-        <v>0.6</v>
-      </c>
-      <c r="K2291" t="n">
-        <v>0.285714285714286</v>
       </c>
     </row>
     <row r="2292">
       <c r="A2292" t="s">
-        <v>235</v>
+        <v>723</v>
       </c>
       <c r="B2292" s="1" t="n">
         <v>45657</v>
       </c>
       <c r="C2292" s="1" t="n">
-        <v>45138</v>
+        <v>45472</v>
       </c>
       <c r="D2292" t="s">
-        <v>236</v>
+        <v>724</v>
       </c>
       <c r="E2292" t="n">
-        <v>0.636363636363636</v>
+        <v>0.666666666666667</v>
       </c>
       <c r="F2292" t="n">
-        <v>0.606060606060606</v>
+        <v>0.666666666666667</v>
       </c>
       <c r="G2292" t="n">
-        <v>0.5</v>
+        <v>0.375</v>
       </c>
       <c r="H2292" t="n">
-        <v>0.619047619047619</v>
+        <v>0.571428571428571</v>
       </c>
       <c r="I2292" t="n">
-        <v>0</v>
+        <v>0.333333333333333</v>
       </c>
       <c r="J2292" t="n">
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="K2292" t="n">
-        <v>0.571428571428571</v>
+        <v>0.285714285714286</v>
       </c>
     </row>
     <row r="2293">
       <c r="A2293" t="s">
-        <v>725</v>
+        <v>235</v>
       </c>
       <c r="B2293" s="1" t="n">
         <v>45657</v>
       </c>
       <c r="C2293" s="1" t="n">
-        <v>45490</v>
+        <v>45138</v>
       </c>
       <c r="D2293" t="s">
-        <v>726</v>
+        <v>236</v>
       </c>
       <c r="E2293" t="n">
-        <v>0.454545454545455</v>
+        <v>0.636363636363636</v>
       </c>
       <c r="F2293" t="n">
-        <v>0.454545454545455</v>
+        <v>0.606060606060606</v>
       </c>
       <c r="G2293" t="n">
-        <v>0.375</v>
+        <v>0.5</v>
       </c>
       <c r="H2293" t="n">
-        <v>0.571428571428571</v>
+        <v>0.619047619047619</v>
       </c>
       <c r="I2293" t="n">
-        <v>0.266666666666667</v>
+        <v>0</v>
       </c>
       <c r="J2293" t="n">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="K2293" t="n">
         <v>0.571428571428571</v>
@@ -83662,34 +83662,34 @@
     </row>
     <row r="2294">
       <c r="A2294" t="s">
-        <v>237</v>
+        <v>725</v>
       </c>
       <c r="B2294" s="1" t="n">
         <v>45657</v>
       </c>
       <c r="C2294" s="1" t="n">
-        <v>45489</v>
+        <v>45490</v>
       </c>
       <c r="D2294" t="s">
-        <v>238</v>
+        <v>726</v>
       </c>
       <c r="E2294" t="n">
-        <v>0.666666666666667</v>
+        <v>0.454545454545455</v>
       </c>
       <c r="F2294" t="n">
-        <v>0.636363636363636</v>
+        <v>0.454545454545455</v>
       </c>
       <c r="G2294" t="n">
-        <v>0.541666666666667</v>
+        <v>0.375</v>
       </c>
       <c r="H2294" t="n">
         <v>0.571428571428571</v>
       </c>
       <c r="I2294" t="n">
-        <v>0.666666666666667</v>
+        <v>0.266666666666667</v>
       </c>
       <c r="J2294" t="n">
-        <v>0.2</v>
+        <v>0.333333333333333</v>
       </c>
       <c r="K2294" t="n">
         <v>0.571428571428571</v>
@@ -83697,22 +83697,22 @@
     </row>
     <row r="2295">
       <c r="A2295" t="s">
-        <v>946</v>
+        <v>237</v>
       </c>
       <c r="B2295" s="1" t="n">
         <v>45657</v>
       </c>
       <c r="C2295" s="1" t="n">
-        <v>45504</v>
+        <v>45489</v>
       </c>
       <c r="D2295" t="s">
-        <v>947</v>
+        <v>238</v>
       </c>
       <c r="E2295" t="n">
-        <v>0.696969696969697</v>
+        <v>0.666666666666667</v>
       </c>
       <c r="F2295" t="n">
-        <v>0.757575757575758</v>
+        <v>0.636363636363636</v>
       </c>
       <c r="G2295" t="n">
         <v>0.541666666666667</v>
@@ -83721,18 +83721,18 @@
         <v>0.571428571428571</v>
       </c>
       <c r="I2295" t="n">
-        <v>0.266666666666667</v>
+        <v>0.666666666666667</v>
       </c>
       <c r="J2295" t="n">
         <v>0.2</v>
       </c>
       <c r="K2295" t="n">
-        <v>0.380952380952381</v>
+        <v>0.571428571428571</v>
       </c>
     </row>
     <row r="2296">
       <c r="A2296" t="s">
-        <v>948</v>
+        <v>946</v>
       </c>
       <c r="B2296" s="1" t="n">
         <v>45657</v>
@@ -83741,27 +83741,62 @@
         <v>45504</v>
       </c>
       <c r="D2296" t="s">
-        <v>949</v>
+        <v>947</v>
       </c>
       <c r="E2296" t="n">
-        <v>0.575757575757576</v>
+        <v>0.696969696969697</v>
       </c>
       <c r="F2296" t="n">
         <v>0.757575757575758</v>
       </c>
       <c r="G2296" t="n">
-        <v>0.291666666666667</v>
+        <v>0.541666666666667</v>
       </c>
       <c r="H2296" t="n">
-        <v>0.476190476190476</v>
+        <v>0.571428571428571</v>
       </c>
       <c r="I2296" t="n">
         <v>0.266666666666667</v>
       </c>
       <c r="J2296" t="n">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="K2296" t="n">
+        <v>0.380952380952381</v>
+      </c>
+    </row>
+    <row r="2297">
+      <c r="A2297" t="s">
+        <v>948</v>
+      </c>
+      <c r="B2297" s="1" t="n">
+        <v>45657</v>
+      </c>
+      <c r="C2297" s="1" t="n">
+        <v>45504</v>
+      </c>
+      <c r="D2297" t="s">
+        <v>949</v>
+      </c>
+      <c r="E2297" t="n">
+        <v>0.575757575757576</v>
+      </c>
+      <c r="F2297" t="n">
+        <v>0.757575757575758</v>
+      </c>
+      <c r="G2297" t="n">
+        <v>0.291666666666667</v>
+      </c>
+      <c r="H2297" t="n">
+        <v>0.476190476190476</v>
+      </c>
+      <c r="I2297" t="n">
+        <v>0.266666666666667</v>
+      </c>
+      <c r="J2297" t="n">
+        <v>0</v>
+      </c>
+      <c r="K2297" t="n">
         <v>0.285714285714286</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualização de dados automática em 2025-01-07 12:30:03 (cron)
</commit_message>
<xml_diff>
--- a/public/docs/index_07_dim_CG.xlsx
+++ b/public/docs/index_07_dim_CG.xlsx
@@ -2642,7 +2642,7 @@
     <t xml:space="preserve">14.127.813/0001-51</t>
   </si>
   <si>
-    <t xml:space="preserve">GETNINJAS S.A.</t>
+    <t xml:space="preserve">REAG INVESTIMENTOS S.A.</t>
   </si>
   <si>
     <t xml:space="preserve">14.776.142/0001-50</t>
@@ -83803,6 +83803,41 @@
         <v>0.285714285714286</v>
       </c>
     </row>
+    <row r="2298">
+      <c r="A2298" t="s">
+        <v>810</v>
+      </c>
+      <c r="B2298" s="1" t="n">
+        <v>45716</v>
+      </c>
+      <c r="C2298" s="1" t="n">
+        <v>45565</v>
+      </c>
+      <c r="D2298" t="s">
+        <v>811</v>
+      </c>
+      <c r="E2298" t="n">
+        <v>0.666666666666667</v>
+      </c>
+      <c r="F2298" t="n">
+        <v>0.696969696969697</v>
+      </c>
+      <c r="G2298" t="n">
+        <v>0.583333333333333</v>
+      </c>
+      <c r="H2298" t="n">
+        <v>0.571428571428571</v>
+      </c>
+      <c r="I2298" t="n">
+        <v>0.266666666666667</v>
+      </c>
+      <c r="J2298" t="n">
+        <v>0</v>
+      </c>
+      <c r="K2298" t="n">
+        <v>0.571428571428571</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>

<commit_message>
Atualização de dados automática em 2025-01-28 12:30:03 (cron)
</commit_message>
<xml_diff>
--- a/public/docs/index_07_dim_CG.xlsx
+++ b/public/docs/index_07_dim_CG.xlsx
@@ -89648,6 +89648,41 @@
         <v>0.571428571428571</v>
       </c>
     </row>
+    <row r="2465">
+      <c r="A2465" t="s">
+        <v>812</v>
+      </c>
+      <c r="B2465" s="1" t="n">
+        <v>45838</v>
+      </c>
+      <c r="C2465" s="1" t="n">
+        <v>45681</v>
+      </c>
+      <c r="D2465" t="s">
+        <v>813</v>
+      </c>
+      <c r="E2465" t="n">
+        <v>0.454545454545455</v>
+      </c>
+      <c r="F2465" t="n">
+        <v>0.575757575757576</v>
+      </c>
+      <c r="G2465" t="n">
+        <v>0.541666666666667</v>
+      </c>
+      <c r="H2465" t="n">
+        <v>0.571428571428571</v>
+      </c>
+      <c r="I2465" t="n">
+        <v>0.333333333333333</v>
+      </c>
+      <c r="J2465" t="n">
+        <v>0.133333333333333</v>
+      </c>
+      <c r="K2465" t="n">
+        <v>0.619047619047619</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>

<commit_message>
Atualização de dados automática em 2025-02-24 20:32:44 (cron)
</commit_message>
<xml_diff>
--- a/public/docs/index_07_dim_CG.xlsx
+++ b/public/docs/index_07_dim_CG.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1019" uniqueCount="1019">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1020" uniqueCount="1020">
   <si>
     <t xml:space="preserve">CNPJ_Companhia</t>
   </si>
@@ -2805,6 +2805,9 @@
   </si>
   <si>
     <t xml:space="preserve">VITTIA S.A.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BOMBRIL S.A. - EM RECUPERAÇÃO JUDICIAL</t>
   </si>
   <si>
     <t xml:space="preserve">59.418.806/0001-47</t>
@@ -44019,7 +44022,7 @@
         <v>44407</v>
       </c>
       <c r="D1161" t="s">
-        <v>570</v>
+        <v>931</v>
       </c>
       <c r="E1161" t="n">
         <v>0.575757575757576</v>
@@ -44570,7 +44573,7 @@
     </row>
     <row r="1177">
       <c r="A1177" t="s">
-        <v>931</v>
+        <v>932</v>
       </c>
       <c r="B1177" s="1" t="n">
         <v>44561</v>
@@ -44579,7 +44582,7 @@
         <v>44410</v>
       </c>
       <c r="D1177" t="s">
-        <v>932</v>
+        <v>933</v>
       </c>
       <c r="E1177" t="n">
         <v>0.575757575757576</v>
@@ -44605,7 +44608,7 @@
     </row>
     <row r="1178">
       <c r="A1178" t="s">
-        <v>933</v>
+        <v>934</v>
       </c>
       <c r="B1178" s="1" t="n">
         <v>44561</v>
@@ -44614,7 +44617,7 @@
         <v>44410</v>
       </c>
       <c r="D1178" t="s">
-        <v>934</v>
+        <v>935</v>
       </c>
       <c r="E1178" t="n">
         <v>0.575757575757576</v>
@@ -44675,7 +44678,7 @@
     </row>
     <row r="1180">
       <c r="A1180" t="s">
-        <v>935</v>
+        <v>936</v>
       </c>
       <c r="B1180" s="1" t="n">
         <v>44561</v>
@@ -44684,7 +44687,7 @@
         <v>44410</v>
       </c>
       <c r="D1180" t="s">
-        <v>936</v>
+        <v>937</v>
       </c>
       <c r="E1180" t="n">
         <v>0.666666666666667</v>
@@ -45725,7 +45728,7 @@
     </row>
     <row r="1210">
       <c r="A1210" t="s">
-        <v>937</v>
+        <v>938</v>
       </c>
       <c r="B1210" s="1" t="n">
         <v>44561</v>
@@ -45734,7 +45737,7 @@
         <v>44407</v>
       </c>
       <c r="D1210" t="s">
-        <v>938</v>
+        <v>939</v>
       </c>
       <c r="E1210" t="n">
         <v>0.606060606060606</v>
@@ -46005,7 +46008,7 @@
     </row>
     <row r="1218">
       <c r="A1218" t="s">
-        <v>939</v>
+        <v>940</v>
       </c>
       <c r="B1218" s="1" t="n">
         <v>44561</v>
@@ -46014,7 +46017,7 @@
         <v>44410</v>
       </c>
       <c r="D1218" t="s">
-        <v>940</v>
+        <v>941</v>
       </c>
       <c r="E1218" t="n">
         <v>0.636363636363636</v>
@@ -46040,7 +46043,7 @@
     </row>
     <row r="1219">
       <c r="A1219" t="s">
-        <v>941</v>
+        <v>942</v>
       </c>
       <c r="B1219" s="1" t="n">
         <v>44561</v>
@@ -46049,7 +46052,7 @@
         <v>44404</v>
       </c>
       <c r="D1219" t="s">
-        <v>942</v>
+        <v>943</v>
       </c>
       <c r="E1219" t="n">
         <v>0.636363636363636</v>
@@ -46320,7 +46323,7 @@
     </row>
     <row r="1227">
       <c r="A1227" t="s">
-        <v>943</v>
+        <v>944</v>
       </c>
       <c r="B1227" s="1" t="n">
         <v>44561</v>
@@ -46329,7 +46332,7 @@
         <v>44410</v>
       </c>
       <c r="D1227" t="s">
-        <v>944</v>
+        <v>945</v>
       </c>
       <c r="E1227" t="n">
         <v>0.696969696969697</v>
@@ -46740,7 +46743,7 @@
     </row>
     <row r="1239">
       <c r="A1239" t="s">
-        <v>945</v>
+        <v>946</v>
       </c>
       <c r="B1239" s="1" t="n">
         <v>44561</v>
@@ -46749,7 +46752,7 @@
         <v>44407</v>
       </c>
       <c r="D1239" t="s">
-        <v>946</v>
+        <v>947</v>
       </c>
       <c r="E1239" t="n">
         <v>0.727272727272727</v>
@@ -48210,7 +48213,7 @@
     </row>
     <row r="1281">
       <c r="A1281" t="s">
-        <v>947</v>
+        <v>948</v>
       </c>
       <c r="B1281" s="1" t="n">
         <v>44561</v>
@@ -48219,7 +48222,7 @@
         <v>44406</v>
       </c>
       <c r="D1281" t="s">
-        <v>948</v>
+        <v>949</v>
       </c>
       <c r="E1281" t="n">
         <v>0.696969696969697</v>
@@ -48280,7 +48283,7 @@
     </row>
     <row r="1283">
       <c r="A1283" t="s">
-        <v>949</v>
+        <v>950</v>
       </c>
       <c r="B1283" s="1" t="n">
         <v>44561</v>
@@ -48289,7 +48292,7 @@
         <v>44406</v>
       </c>
       <c r="D1283" t="s">
-        <v>950</v>
+        <v>951</v>
       </c>
       <c r="E1283" t="n">
         <v>0.636363636363636</v>
@@ -48560,7 +48563,7 @@
     </row>
     <row r="1291">
       <c r="A1291" t="s">
-        <v>951</v>
+        <v>952</v>
       </c>
       <c r="B1291" s="1" t="n">
         <v>44926</v>
@@ -48569,7 +48572,7 @@
         <v>44761</v>
       </c>
       <c r="D1291" t="s">
-        <v>952</v>
+        <v>953</v>
       </c>
       <c r="E1291" t="n">
         <v>0.666666666666667</v>
@@ -48595,7 +48598,7 @@
     </row>
     <row r="1292">
       <c r="A1292" t="s">
-        <v>953</v>
+        <v>954</v>
       </c>
       <c r="B1292" s="1" t="n">
         <v>44926</v>
@@ -48604,7 +48607,7 @@
         <v>44774</v>
       </c>
       <c r="D1292" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="E1292" t="n">
         <v>0.636363636363636</v>
@@ -50065,7 +50068,7 @@
     </row>
     <row r="1334">
       <c r="A1334" t="s">
-        <v>955</v>
+        <v>956</v>
       </c>
       <c r="B1334" s="1" t="n">
         <v>44651</v>
@@ -50074,7 +50077,7 @@
         <v>44501</v>
       </c>
       <c r="D1334" t="s">
-        <v>956</v>
+        <v>957</v>
       </c>
       <c r="E1334" t="n">
         <v>0.606060606060606</v>
@@ -50765,7 +50768,7 @@
     </row>
     <row r="1354">
       <c r="A1354" t="s">
-        <v>957</v>
+        <v>958</v>
       </c>
       <c r="B1354" s="1" t="n">
         <v>44926</v>
@@ -50774,7 +50777,7 @@
         <v>44755</v>
       </c>
       <c r="D1354" t="s">
-        <v>958</v>
+        <v>959</v>
       </c>
       <c r="E1354" t="n">
         <v>0.636363636363636</v>
@@ -50835,7 +50838,7 @@
     </row>
     <row r="1356">
       <c r="A1356" t="s">
-        <v>959</v>
+        <v>960</v>
       </c>
       <c r="B1356" s="1" t="n">
         <v>44926</v>
@@ -50844,7 +50847,7 @@
         <v>44771</v>
       </c>
       <c r="D1356" t="s">
-        <v>960</v>
+        <v>961</v>
       </c>
       <c r="E1356" t="n">
         <v>0.666666666666667</v>
@@ -52165,7 +52168,7 @@
     </row>
     <row r="1394">
       <c r="A1394" t="s">
-        <v>961</v>
+        <v>962</v>
       </c>
       <c r="B1394" s="1" t="n">
         <v>44926</v>
@@ -52174,7 +52177,7 @@
         <v>44760</v>
       </c>
       <c r="D1394" t="s">
-        <v>962</v>
+        <v>963</v>
       </c>
       <c r="E1394" t="n">
         <v>0.484848484848485</v>
@@ -53075,7 +53078,7 @@
     </row>
     <row r="1420">
       <c r="A1420" t="s">
-        <v>963</v>
+        <v>964</v>
       </c>
       <c r="B1420" s="1" t="n">
         <v>44926</v>
@@ -53084,7 +53087,7 @@
         <v>44770</v>
       </c>
       <c r="D1420" t="s">
-        <v>964</v>
+        <v>965</v>
       </c>
       <c r="E1420" t="n">
         <v>0.696969696969697</v>
@@ -54020,7 +54023,7 @@
     </row>
     <row r="1447">
       <c r="A1447" t="s">
-        <v>965</v>
+        <v>966</v>
       </c>
       <c r="B1447" s="1" t="n">
         <v>44926</v>
@@ -54029,7 +54032,7 @@
         <v>44771</v>
       </c>
       <c r="D1447" t="s">
-        <v>966</v>
+        <v>967</v>
       </c>
       <c r="E1447" t="n">
         <v>0.636363636363636</v>
@@ -54545,7 +54548,7 @@
     </row>
     <row r="1462">
       <c r="A1462" t="s">
-        <v>967</v>
+        <v>968</v>
       </c>
       <c r="B1462" s="1" t="n">
         <v>44926</v>
@@ -54554,7 +54557,7 @@
         <v>44773</v>
       </c>
       <c r="D1462" t="s">
-        <v>968</v>
+        <v>969</v>
       </c>
       <c r="E1462" t="n">
         <v>0.636363636363636</v>
@@ -54930,7 +54933,7 @@
     </row>
     <row r="1473">
       <c r="A1473" t="s">
-        <v>969</v>
+        <v>970</v>
       </c>
       <c r="B1473" s="1" t="n">
         <v>44926</v>
@@ -54939,7 +54942,7 @@
         <v>44762</v>
       </c>
       <c r="D1473" t="s">
-        <v>970</v>
+        <v>971</v>
       </c>
       <c r="E1473" t="n">
         <v>0.454545454545455</v>
@@ -56575,7 +56578,7 @@
     </row>
     <row r="1520">
       <c r="A1520" t="s">
-        <v>971</v>
+        <v>972</v>
       </c>
       <c r="B1520" s="1" t="n">
         <v>44926</v>
@@ -56584,7 +56587,7 @@
         <v>44771</v>
       </c>
       <c r="D1520" t="s">
-        <v>972</v>
+        <v>973</v>
       </c>
       <c r="E1520" t="n">
         <v>0.727272727272727</v>
@@ -56680,7 +56683,7 @@
     </row>
     <row r="1523">
       <c r="A1523" t="s">
-        <v>973</v>
+        <v>974</v>
       </c>
       <c r="B1523" s="1" t="n">
         <v>44926</v>
@@ -56689,7 +56692,7 @@
         <v>44742</v>
       </c>
       <c r="D1523" t="s">
-        <v>974</v>
+        <v>975</v>
       </c>
       <c r="E1523" t="n">
         <v>0.606060606060606</v>
@@ -56715,7 +56718,7 @@
     </row>
     <row r="1524">
       <c r="A1524" t="s">
-        <v>975</v>
+        <v>976</v>
       </c>
       <c r="B1524" s="1" t="n">
         <v>44926</v>
@@ -56724,7 +56727,7 @@
         <v>44804</v>
       </c>
       <c r="D1524" t="s">
-        <v>976</v>
+        <v>977</v>
       </c>
       <c r="E1524" t="n">
         <v>0.515151515151515</v>
@@ -56785,7 +56788,7 @@
     </row>
     <row r="1526">
       <c r="A1526" t="s">
-        <v>977</v>
+        <v>978</v>
       </c>
       <c r="B1526" s="1" t="n">
         <v>44926</v>
@@ -56794,7 +56797,7 @@
         <v>44771</v>
       </c>
       <c r="D1526" t="s">
-        <v>978</v>
+        <v>979</v>
       </c>
       <c r="E1526" t="n">
         <v>0.575757575757576</v>
@@ -57030,7 +57033,7 @@
     </row>
     <row r="1533">
       <c r="A1533" t="s">
-        <v>979</v>
+        <v>980</v>
       </c>
       <c r="B1533" s="1" t="n">
         <v>44926</v>
@@ -57039,7 +57042,7 @@
         <v>44771</v>
       </c>
       <c r="D1533" t="s">
-        <v>980</v>
+        <v>981</v>
       </c>
       <c r="E1533" t="n">
         <v>0.515151515151515</v>
@@ -57380,7 +57383,7 @@
     </row>
     <row r="1543">
       <c r="A1543" t="s">
-        <v>981</v>
+        <v>982</v>
       </c>
       <c r="B1543" s="1" t="n">
         <v>44926</v>
@@ -57389,7 +57392,7 @@
         <v>44774</v>
       </c>
       <c r="D1543" t="s">
-        <v>982</v>
+        <v>983</v>
       </c>
       <c r="E1543" t="n">
         <v>0.515151515151515</v>
@@ -57800,7 +57803,7 @@
     </row>
     <row r="1555">
       <c r="A1555" t="s">
-        <v>983</v>
+        <v>984</v>
       </c>
       <c r="B1555" s="1" t="n">
         <v>44926</v>
@@ -57809,7 +57812,7 @@
         <v>44742</v>
       </c>
       <c r="D1555" t="s">
-        <v>984</v>
+        <v>985</v>
       </c>
       <c r="E1555" t="n">
         <v>0.606060606060606</v>
@@ -58045,7 +58048,7 @@
     </row>
     <row r="1562">
       <c r="A1562" t="s">
-        <v>985</v>
+        <v>986</v>
       </c>
       <c r="B1562" s="1" t="n">
         <v>44651</v>
@@ -58054,7 +58057,7 @@
         <v>44497</v>
       </c>
       <c r="D1562" t="s">
-        <v>986</v>
+        <v>987</v>
       </c>
       <c r="E1562" t="n">
         <v>0.757575757575758</v>
@@ -58535,7 +58538,7 @@
     </row>
     <row r="1576">
       <c r="A1576" t="s">
-        <v>987</v>
+        <v>988</v>
       </c>
       <c r="B1576" s="1" t="n">
         <v>44926</v>
@@ -58544,7 +58547,7 @@
         <v>44767</v>
       </c>
       <c r="D1576" t="s">
-        <v>988</v>
+        <v>989</v>
       </c>
       <c r="E1576" t="n">
         <v>0.424242424242424</v>
@@ -58640,7 +58643,7 @@
     </row>
     <row r="1579">
       <c r="A1579" t="s">
-        <v>989</v>
+        <v>990</v>
       </c>
       <c r="B1579" s="1" t="n">
         <v>44926</v>
@@ -58649,7 +58652,7 @@
         <v>44764</v>
       </c>
       <c r="D1579" t="s">
-        <v>990</v>
+        <v>991</v>
       </c>
       <c r="E1579" t="n">
         <v>0.515151515151515</v>
@@ -58780,7 +58783,7 @@
     </row>
     <row r="1583">
       <c r="A1583" t="s">
-        <v>991</v>
+        <v>992</v>
       </c>
       <c r="B1583" s="1" t="n">
         <v>44926</v>
@@ -58789,7 +58792,7 @@
         <v>44769</v>
       </c>
       <c r="D1583" t="s">
-        <v>992</v>
+        <v>993</v>
       </c>
       <c r="E1583" t="n">
         <v>0.636363636363636</v>
@@ -58955,7 +58958,7 @@
     </row>
     <row r="1588">
       <c r="A1588" t="s">
-        <v>993</v>
+        <v>994</v>
       </c>
       <c r="B1588" s="1" t="n">
         <v>44926</v>
@@ -58964,7 +58967,7 @@
         <v>44771</v>
       </c>
       <c r="D1588" t="s">
-        <v>994</v>
+        <v>995</v>
       </c>
       <c r="E1588" t="n">
         <v>0.606060606060606</v>
@@ -59314,7 +59317,7 @@
         <v>44768</v>
       </c>
       <c r="D1598" t="s">
-        <v>570</v>
+        <v>931</v>
       </c>
       <c r="E1598" t="n">
         <v>0.575757575757576</v>
@@ -59830,7 +59833,7 @@
     </row>
     <row r="1613">
       <c r="A1613" t="s">
-        <v>931</v>
+        <v>932</v>
       </c>
       <c r="B1613" s="1" t="n">
         <v>44926</v>
@@ -59839,7 +59842,7 @@
         <v>44774</v>
       </c>
       <c r="D1613" t="s">
-        <v>932</v>
+        <v>933</v>
       </c>
       <c r="E1613" t="n">
         <v>0.575757575757576</v>
@@ -59865,7 +59868,7 @@
     </row>
     <row r="1614">
       <c r="A1614" t="s">
-        <v>933</v>
+        <v>934</v>
       </c>
       <c r="B1614" s="1" t="n">
         <v>44926</v>
@@ -59874,7 +59877,7 @@
         <v>44771</v>
       </c>
       <c r="D1614" t="s">
-        <v>934</v>
+        <v>935</v>
       </c>
       <c r="E1614" t="n">
         <v>0.575757575757576</v>
@@ -59935,7 +59938,7 @@
     </row>
     <row r="1616">
       <c r="A1616" t="s">
-        <v>935</v>
+        <v>936</v>
       </c>
       <c r="B1616" s="1" t="n">
         <v>44926</v>
@@ -59944,7 +59947,7 @@
         <v>44774</v>
       </c>
       <c r="D1616" t="s">
-        <v>936</v>
+        <v>937</v>
       </c>
       <c r="E1616" t="n">
         <v>0.666666666666667</v>
@@ -60880,7 +60883,7 @@
     </row>
     <row r="1643">
       <c r="A1643" t="s">
-        <v>995</v>
+        <v>996</v>
       </c>
       <c r="B1643" s="1" t="n">
         <v>44926</v>
@@ -60889,7 +60892,7 @@
         <v>44770</v>
       </c>
       <c r="D1643" t="s">
-        <v>996</v>
+        <v>997</v>
       </c>
       <c r="E1643" t="n">
         <v>0.727272727272727</v>
@@ -60985,7 +60988,7 @@
     </row>
     <row r="1646">
       <c r="A1646" t="s">
-        <v>937</v>
+        <v>938</v>
       </c>
       <c r="B1646" s="1" t="n">
         <v>44926</v>
@@ -60994,7 +60997,7 @@
         <v>44767</v>
       </c>
       <c r="D1646" t="s">
-        <v>938</v>
+        <v>939</v>
       </c>
       <c r="E1646" t="n">
         <v>0.606060606060606</v>
@@ -61265,7 +61268,7 @@
     </row>
     <row r="1654">
       <c r="A1654" t="s">
-        <v>939</v>
+        <v>940</v>
       </c>
       <c r="B1654" s="1" t="n">
         <v>44926</v>
@@ -61274,7 +61277,7 @@
         <v>44774</v>
       </c>
       <c r="D1654" t="s">
-        <v>940</v>
+        <v>941</v>
       </c>
       <c r="E1654" t="n">
         <v>0.636363636363636</v>
@@ -61300,7 +61303,7 @@
     </row>
     <row r="1655">
       <c r="A1655" t="s">
-        <v>941</v>
+        <v>942</v>
       </c>
       <c r="B1655" s="1" t="n">
         <v>44926</v>
@@ -61309,7 +61312,7 @@
         <v>44771</v>
       </c>
       <c r="D1655" t="s">
-        <v>942</v>
+        <v>943</v>
       </c>
       <c r="E1655" t="n">
         <v>0.545454545454545</v>
@@ -61475,7 +61478,7 @@
     </row>
     <row r="1660">
       <c r="A1660" t="s">
-        <v>997</v>
+        <v>998</v>
       </c>
       <c r="B1660" s="1" t="n">
         <v>44742</v>
@@ -61484,7 +61487,7 @@
         <v>44592</v>
       </c>
       <c r="D1660" t="s">
-        <v>998</v>
+        <v>999</v>
       </c>
       <c r="E1660" t="n">
         <v>0.606060606060606</v>
@@ -61615,7 +61618,7 @@
     </row>
     <row r="1664">
       <c r="A1664" t="s">
-        <v>943</v>
+        <v>944</v>
       </c>
       <c r="B1664" s="1" t="n">
         <v>44926</v>
@@ -61624,7 +61627,7 @@
         <v>44774</v>
       </c>
       <c r="D1664" t="s">
-        <v>944</v>
+        <v>945</v>
       </c>
       <c r="E1664" t="n">
         <v>0.696969696969697</v>
@@ -62000,7 +62003,7 @@
     </row>
     <row r="1675">
       <c r="A1675" t="s">
-        <v>945</v>
+        <v>946</v>
       </c>
       <c r="B1675" s="1" t="n">
         <v>44562</v>
@@ -62009,7 +62012,7 @@
         <v>44771</v>
       </c>
       <c r="D1675" t="s">
-        <v>946</v>
+        <v>947</v>
       </c>
       <c r="E1675" t="n">
         <v>0.727272727272727</v>
@@ -62035,7 +62038,7 @@
     </row>
     <row r="1676">
       <c r="A1676" t="s">
-        <v>945</v>
+        <v>946</v>
       </c>
       <c r="B1676" s="1" t="n">
         <v>44926</v>
@@ -62044,7 +62047,7 @@
         <v>44771</v>
       </c>
       <c r="D1676" t="s">
-        <v>946</v>
+        <v>947</v>
       </c>
       <c r="E1676" t="n">
         <v>0.727272727272727</v>
@@ -63470,7 +63473,7 @@
     </row>
     <row r="1717">
       <c r="A1717" t="s">
-        <v>947</v>
+        <v>948</v>
       </c>
       <c r="B1717" s="1" t="n">
         <v>44926</v>
@@ -63479,7 +63482,7 @@
         <v>44771</v>
       </c>
       <c r="D1717" t="s">
-        <v>948</v>
+        <v>949</v>
       </c>
       <c r="E1717" t="n">
         <v>0.696969696969697</v>
@@ -63540,7 +63543,7 @@
     </row>
     <row r="1719">
       <c r="A1719" t="s">
-        <v>949</v>
+        <v>950</v>
       </c>
       <c r="B1719" s="1" t="n">
         <v>44926</v>
@@ -63549,7 +63552,7 @@
         <v>44771</v>
       </c>
       <c r="D1719" t="s">
-        <v>950</v>
+        <v>951</v>
       </c>
       <c r="E1719" t="n">
         <v>0.636363636363636</v>
@@ -63820,7 +63823,7 @@
     </row>
     <row r="1727">
       <c r="A1727" t="s">
-        <v>951</v>
+        <v>952</v>
       </c>
       <c r="B1727" s="1" t="n">
         <v>45291</v>
@@ -63829,7 +63832,7 @@
         <v>45112</v>
       </c>
       <c r="D1727" t="s">
-        <v>952</v>
+        <v>953</v>
       </c>
       <c r="E1727" t="n">
         <v>0.666666666666667</v>
@@ -63855,7 +63858,7 @@
     </row>
     <row r="1728">
       <c r="A1728" t="s">
-        <v>953</v>
+        <v>954</v>
       </c>
       <c r="B1728" s="1" t="n">
         <v>45291</v>
@@ -63864,7 +63867,7 @@
         <v>45138</v>
       </c>
       <c r="D1728" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="E1728" t="n">
         <v>0.636363636363636</v>
@@ -65185,7 +65188,7 @@
     </row>
     <row r="1766">
       <c r="A1766" t="s">
-        <v>955</v>
+        <v>956</v>
       </c>
       <c r="B1766" s="1" t="n">
         <v>45016</v>
@@ -65194,7 +65197,7 @@
         <v>44861</v>
       </c>
       <c r="D1766" t="s">
-        <v>956</v>
+        <v>957</v>
       </c>
       <c r="E1766" t="n">
         <v>0.606060606060606</v>
@@ -65815,7 +65818,7 @@
     </row>
     <row r="1784">
       <c r="A1784" t="s">
-        <v>957</v>
+        <v>958</v>
       </c>
       <c r="B1784" s="1" t="n">
         <v>45291</v>
@@ -65824,7 +65827,7 @@
         <v>45137</v>
       </c>
       <c r="D1784" t="s">
-        <v>958</v>
+        <v>959</v>
       </c>
       <c r="E1784" t="n">
         <v>0.636363636363636</v>
@@ -65885,7 +65888,7 @@
     </row>
     <row r="1786">
       <c r="A1786" t="s">
-        <v>959</v>
+        <v>960</v>
       </c>
       <c r="B1786" s="1" t="n">
         <v>45291</v>
@@ -65894,7 +65897,7 @@
         <v>45138</v>
       </c>
       <c r="D1786" t="s">
-        <v>960</v>
+        <v>961</v>
       </c>
       <c r="E1786" t="n">
         <v>0.666666666666667</v>
@@ -67145,7 +67148,7 @@
     </row>
     <row r="1822">
       <c r="A1822" t="s">
-        <v>961</v>
+        <v>962</v>
       </c>
       <c r="B1822" s="1" t="n">
         <v>45291</v>
@@ -67154,7 +67157,7 @@
         <v>45138</v>
       </c>
       <c r="D1822" t="s">
-        <v>962</v>
+        <v>963</v>
       </c>
       <c r="E1822" t="n">
         <v>0.484848484848485</v>
@@ -68055,7 +68058,7 @@
     </row>
     <row r="1848">
       <c r="A1848" t="s">
-        <v>963</v>
+        <v>964</v>
       </c>
       <c r="B1848" s="1" t="n">
         <v>45291</v>
@@ -68064,7 +68067,7 @@
         <v>45174</v>
       </c>
       <c r="D1848" t="s">
-        <v>964</v>
+        <v>965</v>
       </c>
       <c r="E1848" t="n">
         <v>0.636363636363636</v>
@@ -69385,7 +69388,7 @@
     </row>
     <row r="1886">
       <c r="A1886" t="s">
-        <v>967</v>
+        <v>968</v>
       </c>
       <c r="B1886" s="1" t="n">
         <v>45291</v>
@@ -69394,7 +69397,7 @@
         <v>45138</v>
       </c>
       <c r="D1886" t="s">
-        <v>968</v>
+        <v>969</v>
       </c>
       <c r="E1886" t="n">
         <v>0.636363636363636</v>
@@ -69770,7 +69773,7 @@
     </row>
     <row r="1897">
       <c r="A1897" t="s">
-        <v>969</v>
+        <v>970</v>
       </c>
       <c r="B1897" s="1" t="n">
         <v>45291</v>
@@ -69779,7 +69782,7 @@
         <v>45133</v>
       </c>
       <c r="D1897" t="s">
-        <v>970</v>
+        <v>971</v>
       </c>
       <c r="E1897" t="n">
         <v>0.454545454545455</v>
@@ -70925,7 +70928,7 @@
     </row>
     <row r="1930">
       <c r="A1930" t="s">
-        <v>999</v>
+        <v>1000</v>
       </c>
       <c r="B1930" s="1" t="n">
         <v>45291</v>
@@ -70934,7 +70937,7 @@
         <v>45138</v>
       </c>
       <c r="D1930" t="s">
-        <v>1000</v>
+        <v>1001</v>
       </c>
       <c r="E1930" t="n">
         <v>0.636363636363636</v>
@@ -71135,7 +71138,7 @@
     </row>
     <row r="1936">
       <c r="A1936" t="s">
-        <v>1001</v>
+        <v>1002</v>
       </c>
       <c r="B1936" s="1" t="n">
         <v>45291</v>
@@ -71144,7 +71147,7 @@
         <v>45134</v>
       </c>
       <c r="D1936" t="s">
-        <v>1002</v>
+        <v>1003</v>
       </c>
       <c r="E1936" t="n">
         <v>0.575757575757576</v>
@@ -71380,7 +71383,7 @@
     </row>
     <row r="1943">
       <c r="A1943" t="s">
-        <v>971</v>
+        <v>972</v>
       </c>
       <c r="B1943" s="1" t="n">
         <v>45291</v>
@@ -71389,7 +71392,7 @@
         <v>45138</v>
       </c>
       <c r="D1943" t="s">
-        <v>972</v>
+        <v>973</v>
       </c>
       <c r="E1943" t="n">
         <v>0.727272727272727</v>
@@ -71450,7 +71453,7 @@
     </row>
     <row r="1945">
       <c r="A1945" t="s">
-        <v>1003</v>
+        <v>1004</v>
       </c>
       <c r="B1945" s="1" t="n">
         <v>45291</v>
@@ -71459,7 +71462,7 @@
         <v>45135</v>
       </c>
       <c r="D1945" t="s">
-        <v>1004</v>
+        <v>1005</v>
       </c>
       <c r="E1945" t="n">
         <v>0.696969696969697</v>
@@ -71520,7 +71523,7 @@
     </row>
     <row r="1947">
       <c r="A1947" t="s">
-        <v>973</v>
+        <v>974</v>
       </c>
       <c r="B1947" s="1" t="n">
         <v>45291</v>
@@ -71529,7 +71532,7 @@
         <v>45135</v>
       </c>
       <c r="D1947" t="s">
-        <v>974</v>
+        <v>975</v>
       </c>
       <c r="E1947" t="n">
         <v>0.636363636363636</v>
@@ -71800,7 +71803,7 @@
     </row>
     <row r="1955">
       <c r="A1955" t="s">
-        <v>979</v>
+        <v>980</v>
       </c>
       <c r="B1955" s="1" t="n">
         <v>45291</v>
@@ -71809,7 +71812,7 @@
         <v>45138</v>
       </c>
       <c r="D1955" t="s">
-        <v>980</v>
+        <v>981</v>
       </c>
       <c r="E1955" t="n">
         <v>0.606060606060606</v>
@@ -72080,7 +72083,7 @@
     </row>
     <row r="1963">
       <c r="A1963" t="s">
-        <v>981</v>
+        <v>982</v>
       </c>
       <c r="B1963" s="1" t="n">
         <v>45291</v>
@@ -72089,7 +72092,7 @@
         <v>45138</v>
       </c>
       <c r="D1963" t="s">
-        <v>982</v>
+        <v>983</v>
       </c>
       <c r="E1963" t="n">
         <v>0.515151515151515</v>
@@ -72465,7 +72468,7 @@
     </row>
     <row r="1974">
       <c r="A1974" t="s">
-        <v>983</v>
+        <v>984</v>
       </c>
       <c r="B1974" s="1" t="n">
         <v>45291</v>
@@ -72474,7 +72477,7 @@
         <v>45106</v>
       </c>
       <c r="D1974" t="s">
-        <v>984</v>
+        <v>985</v>
       </c>
       <c r="E1974" t="n">
         <v>0.606060606060606</v>
@@ -72710,7 +72713,7 @@
     </row>
     <row r="1981">
       <c r="A1981" t="s">
-        <v>985</v>
+        <v>986</v>
       </c>
       <c r="B1981" s="1" t="n">
         <v>45016</v>
@@ -72719,7 +72722,7 @@
         <v>44865</v>
       </c>
       <c r="D1981" t="s">
-        <v>986</v>
+        <v>987</v>
       </c>
       <c r="E1981" t="n">
         <v>0.757575757575758</v>
@@ -73200,7 +73203,7 @@
     </row>
     <row r="1995">
       <c r="A1995" t="s">
-        <v>1005</v>
+        <v>1006</v>
       </c>
       <c r="B1995" s="1" t="n">
         <v>45291</v>
@@ -73209,7 +73212,7 @@
         <v>45134</v>
       </c>
       <c r="D1995" t="s">
-        <v>1006</v>
+        <v>1007</v>
       </c>
       <c r="E1995" t="n">
         <v>0.636363636363636</v>
@@ -73235,7 +73238,7 @@
     </row>
     <row r="1996">
       <c r="A1996" t="s">
-        <v>987</v>
+        <v>988</v>
       </c>
       <c r="B1996" s="1" t="n">
         <v>45291</v>
@@ -73244,7 +73247,7 @@
         <v>45138</v>
       </c>
       <c r="D1996" t="s">
-        <v>988</v>
+        <v>989</v>
       </c>
       <c r="E1996" t="n">
         <v>0.696969696969697</v>
@@ -73305,7 +73308,7 @@
     </row>
     <row r="1998">
       <c r="A1998" t="s">
-        <v>1007</v>
+        <v>1008</v>
       </c>
       <c r="B1998" s="1" t="n">
         <v>45291</v>
@@ -73314,7 +73317,7 @@
         <v>45138</v>
       </c>
       <c r="D1998" t="s">
-        <v>1008</v>
+        <v>1009</v>
       </c>
       <c r="E1998" t="n">
         <v>0.606060606060606</v>
@@ -73375,7 +73378,7 @@
     </row>
     <row r="2000">
       <c r="A2000" t="s">
-        <v>989</v>
+        <v>990</v>
       </c>
       <c r="B2000" s="1" t="n">
         <v>45291</v>
@@ -73384,7 +73387,7 @@
         <v>45132</v>
       </c>
       <c r="D2000" t="s">
-        <v>990</v>
+        <v>991</v>
       </c>
       <c r="E2000" t="n">
         <v>0.515151515151515</v>
@@ -73515,7 +73518,7 @@
     </row>
     <row r="2004">
       <c r="A2004" t="s">
-        <v>991</v>
+        <v>992</v>
       </c>
       <c r="B2004" s="1" t="n">
         <v>45291</v>
@@ -73524,7 +73527,7 @@
         <v>45135</v>
       </c>
       <c r="D2004" t="s">
-        <v>992</v>
+        <v>993</v>
       </c>
       <c r="E2004" t="n">
         <v>0.606060606060606</v>
@@ -73550,7 +73553,7 @@
     </row>
     <row r="2005">
       <c r="A2005" t="s">
-        <v>1009</v>
+        <v>1010</v>
       </c>
       <c r="B2005" s="1" t="n">
         <v>45291</v>
@@ -73559,7 +73562,7 @@
         <v>45138</v>
       </c>
       <c r="D2005" t="s">
-        <v>1010</v>
+        <v>1011</v>
       </c>
       <c r="E2005" t="n">
         <v>0.606060606060606</v>
@@ -73690,7 +73693,7 @@
     </row>
     <row r="2009">
       <c r="A2009" t="s">
-        <v>993</v>
+        <v>994</v>
       </c>
       <c r="B2009" s="1" t="n">
         <v>45291</v>
@@ -73699,7 +73702,7 @@
         <v>45138</v>
       </c>
       <c r="D2009" t="s">
-        <v>994</v>
+        <v>995</v>
       </c>
       <c r="E2009" t="n">
         <v>0.606060606060606</v>
@@ -73830,7 +73833,7 @@
     </row>
     <row r="2013">
       <c r="A2013" t="s">
-        <v>1011</v>
+        <v>1012</v>
       </c>
       <c r="B2013" s="1" t="n">
         <v>45291</v>
@@ -73839,7 +73842,7 @@
         <v>45128</v>
       </c>
       <c r="D2013" t="s">
-        <v>1012</v>
+        <v>1013</v>
       </c>
       <c r="E2013" t="n">
         <v>0.696969696969697</v>
@@ -74084,7 +74087,7 @@
         <v>45135</v>
       </c>
       <c r="D2020" t="s">
-        <v>570</v>
+        <v>931</v>
       </c>
       <c r="E2020" t="n">
         <v>0.575757575757576</v>
@@ -74600,7 +74603,7 @@
     </row>
     <row r="2035">
       <c r="A2035" t="s">
-        <v>931</v>
+        <v>932</v>
       </c>
       <c r="B2035" s="1" t="n">
         <v>45291</v>
@@ -74609,7 +74612,7 @@
         <v>45138</v>
       </c>
       <c r="D2035" t="s">
-        <v>932</v>
+        <v>933</v>
       </c>
       <c r="E2035" t="n">
         <v>0.575757575757576</v>
@@ -74635,7 +74638,7 @@
     </row>
     <row r="2036">
       <c r="A2036" t="s">
-        <v>933</v>
+        <v>934</v>
       </c>
       <c r="B2036" s="1" t="n">
         <v>45291</v>
@@ -74644,7 +74647,7 @@
         <v>45138</v>
       </c>
       <c r="D2036" t="s">
-        <v>934</v>
+        <v>935</v>
       </c>
       <c r="E2036" t="n">
         <v>0.606060606060606</v>
@@ -74705,7 +74708,7 @@
     </row>
     <row r="2038">
       <c r="A2038" t="s">
-        <v>935</v>
+        <v>936</v>
       </c>
       <c r="B2038" s="1" t="n">
         <v>45291</v>
@@ -74714,7 +74717,7 @@
         <v>45138</v>
       </c>
       <c r="D2038" t="s">
-        <v>936</v>
+        <v>937</v>
       </c>
       <c r="E2038" t="n">
         <v>0.666666666666667</v>
@@ -75615,7 +75618,7 @@
     </row>
     <row r="2064">
       <c r="A2064" t="s">
-        <v>995</v>
+        <v>996</v>
       </c>
       <c r="B2064" s="1" t="n">
         <v>45291</v>
@@ -75624,7 +75627,7 @@
         <v>45132</v>
       </c>
       <c r="D2064" t="s">
-        <v>996</v>
+        <v>997</v>
       </c>
       <c r="E2064" t="n">
         <v>0.757575757575758</v>
@@ -75720,7 +75723,7 @@
     </row>
     <row r="2067">
       <c r="A2067" t="s">
-        <v>937</v>
+        <v>938</v>
       </c>
       <c r="B2067" s="1" t="n">
         <v>45291</v>
@@ -75729,7 +75732,7 @@
         <v>45135</v>
       </c>
       <c r="D2067" t="s">
-        <v>938</v>
+        <v>939</v>
       </c>
       <c r="E2067" t="n">
         <v>0.666666666666667</v>
@@ -76000,7 +76003,7 @@
     </row>
     <row r="2075">
       <c r="A2075" t="s">
-        <v>941</v>
+        <v>942</v>
       </c>
       <c r="B2075" s="1" t="n">
         <v>45291</v>
@@ -76009,7 +76012,7 @@
         <v>45138</v>
       </c>
       <c r="D2075" t="s">
-        <v>942</v>
+        <v>943</v>
       </c>
       <c r="E2075" t="n">
         <v>0.575757575757576</v>
@@ -76175,7 +76178,7 @@
     </row>
     <row r="2080">
       <c r="A2080" t="s">
-        <v>997</v>
+        <v>998</v>
       </c>
       <c r="B2080" s="1" t="n">
         <v>45107</v>
@@ -76184,7 +76187,7 @@
         <v>44944</v>
       </c>
       <c r="D2080" t="s">
-        <v>998</v>
+        <v>999</v>
       </c>
       <c r="E2080" t="n">
         <v>0.636363636363636</v>
@@ -76315,7 +76318,7 @@
     </row>
     <row r="2084">
       <c r="A2084" t="s">
-        <v>943</v>
+        <v>944</v>
       </c>
       <c r="B2084" s="1" t="n">
         <v>45291</v>
@@ -76324,7 +76327,7 @@
         <v>45128</v>
       </c>
       <c r="D2084" t="s">
-        <v>944</v>
+        <v>945</v>
       </c>
       <c r="E2084" t="n">
         <v>0.696969696969697</v>
@@ -76665,7 +76668,7 @@
     </row>
     <row r="2094">
       <c r="A2094" t="s">
-        <v>945</v>
+        <v>946</v>
       </c>
       <c r="B2094" s="1" t="n">
         <v>45291</v>
@@ -76674,7 +76677,7 @@
         <v>45138</v>
       </c>
       <c r="D2094" t="s">
-        <v>946</v>
+        <v>947</v>
       </c>
       <c r="E2094" t="n">
         <v>0.696969696969697</v>
@@ -78065,7 +78068,7 @@
     </row>
     <row r="2134">
       <c r="A2134" t="s">
-        <v>947</v>
+        <v>948</v>
       </c>
       <c r="B2134" s="1" t="n">
         <v>45291</v>
@@ -78074,7 +78077,7 @@
         <v>45138</v>
       </c>
       <c r="D2134" t="s">
-        <v>948</v>
+        <v>949</v>
       </c>
       <c r="E2134" t="n">
         <v>0.696969696969697</v>
@@ -78135,7 +78138,7 @@
     </row>
     <row r="2136">
       <c r="A2136" t="s">
-        <v>949</v>
+        <v>950</v>
       </c>
       <c r="B2136" s="1" t="n">
         <v>45291</v>
@@ -78144,7 +78147,7 @@
         <v>45135</v>
       </c>
       <c r="D2136" t="s">
-        <v>950</v>
+        <v>951</v>
       </c>
       <c r="E2136" t="n">
         <v>0.666666666666667</v>
@@ -78415,7 +78418,7 @@
     </row>
     <row r="2144">
       <c r="A2144" t="s">
-        <v>951</v>
+        <v>952</v>
       </c>
       <c r="B2144" s="1" t="n">
         <v>45657</v>
@@ -78424,7 +78427,7 @@
         <v>45503</v>
       </c>
       <c r="D2144" t="s">
-        <v>952</v>
+        <v>953</v>
       </c>
       <c r="E2144" t="n">
         <v>0.666666666666667</v>
@@ -78450,7 +78453,7 @@
     </row>
     <row r="2145">
       <c r="A2145" t="s">
-        <v>953</v>
+        <v>954</v>
       </c>
       <c r="B2145" s="1" t="n">
         <v>45657</v>
@@ -78459,7 +78462,7 @@
         <v>45504</v>
       </c>
       <c r="D2145" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="E2145" t="n">
         <v>0.636363636363636</v>
@@ -79570,7 +79573,7 @@
     </row>
     <row r="2177">
       <c r="A2177" t="s">
-        <v>955</v>
+        <v>956</v>
       </c>
       <c r="B2177" s="1" t="n">
         <v>45382</v>
@@ -79579,7 +79582,7 @@
         <v>45230</v>
       </c>
       <c r="D2177" t="s">
-        <v>956</v>
+        <v>957</v>
       </c>
       <c r="E2177" t="n">
         <v>0.606060606060606</v>
@@ -80060,7 +80063,7 @@
     </row>
     <row r="2191">
       <c r="A2191" t="s">
-        <v>957</v>
+        <v>958</v>
       </c>
       <c r="B2191" s="1" t="n">
         <v>45657</v>
@@ -80069,7 +80072,7 @@
         <v>45489</v>
       </c>
       <c r="D2191" t="s">
-        <v>958</v>
+        <v>959</v>
       </c>
       <c r="E2191" t="n">
         <v>0.636363636363636</v>
@@ -81635,7 +81638,7 @@
     </row>
     <row r="2236">
       <c r="A2236" t="s">
-        <v>963</v>
+        <v>964</v>
       </c>
       <c r="B2236" s="1" t="n">
         <v>45657</v>
@@ -81644,7 +81647,7 @@
         <v>45492</v>
       </c>
       <c r="D2236" t="s">
-        <v>964</v>
+        <v>965</v>
       </c>
       <c r="E2236" t="n">
         <v>0.636363636363636</v>
@@ -82755,7 +82758,7 @@
     </row>
     <row r="2268">
       <c r="A2268" t="s">
-        <v>967</v>
+        <v>968</v>
       </c>
       <c r="B2268" s="1" t="n">
         <v>45657</v>
@@ -82764,7 +82767,7 @@
         <v>45504</v>
       </c>
       <c r="D2268" t="s">
-        <v>968</v>
+        <v>969</v>
       </c>
       <c r="E2268" t="n">
         <v>0.636363636363636</v>
@@ -83105,7 +83108,7 @@
     </row>
     <row r="2278">
       <c r="A2278" t="s">
-        <v>969</v>
+        <v>970</v>
       </c>
       <c r="B2278" s="1" t="n">
         <v>45657</v>
@@ -83114,7 +83117,7 @@
         <v>45503</v>
       </c>
       <c r="D2278" t="s">
-        <v>970</v>
+        <v>971</v>
       </c>
       <c r="E2278" t="n">
         <v>0.454545454545455</v>
@@ -83945,7 +83948,7 @@
     </row>
     <row r="2302">
       <c r="A2302" t="s">
-        <v>999</v>
+        <v>1000</v>
       </c>
       <c r="B2302" s="1" t="n">
         <v>45657</v>
@@ -83954,7 +83957,7 @@
         <v>45504</v>
       </c>
       <c r="D2302" t="s">
-        <v>1000</v>
+        <v>1001</v>
       </c>
       <c r="E2302" t="n">
         <v>0.636363636363636</v>
@@ -84085,7 +84088,7 @@
     </row>
     <row r="2306">
       <c r="A2306" t="s">
-        <v>1013</v>
+        <v>1014</v>
       </c>
       <c r="B2306" s="1" t="n">
         <v>45657</v>
@@ -84094,7 +84097,7 @@
         <v>45496</v>
       </c>
       <c r="D2306" t="s">
-        <v>1014</v>
+        <v>1015</v>
       </c>
       <c r="E2306" t="n">
         <v>0.636363636363636</v>
@@ -84155,7 +84158,7 @@
     </row>
     <row r="2308">
       <c r="A2308" t="s">
-        <v>1001</v>
+        <v>1002</v>
       </c>
       <c r="B2308" s="1" t="n">
         <v>45657</v>
@@ -84164,7 +84167,7 @@
         <v>45491</v>
       </c>
       <c r="D2308" t="s">
-        <v>1002</v>
+        <v>1003</v>
       </c>
       <c r="E2308" t="n">
         <v>0.575757575757576</v>
@@ -84400,7 +84403,7 @@
     </row>
     <row r="2315">
       <c r="A2315" t="s">
-        <v>1015</v>
+        <v>1016</v>
       </c>
       <c r="B2315" s="1" t="n">
         <v>45657</v>
@@ -84409,7 +84412,7 @@
         <v>45371</v>
       </c>
       <c r="D2315" t="s">
-        <v>1016</v>
+        <v>1017</v>
       </c>
       <c r="E2315" t="n">
         <v>0.666666666666667</v>
@@ -84470,7 +84473,7 @@
     </row>
     <row r="2317">
       <c r="A2317" t="s">
-        <v>1017</v>
+        <v>1018</v>
       </c>
       <c r="B2317" s="1" t="n">
         <v>45657</v>
@@ -84479,7 +84482,7 @@
         <v>45587</v>
       </c>
       <c r="D2317" t="s">
-        <v>1018</v>
+        <v>1019</v>
       </c>
       <c r="E2317" t="n">
         <v>0.636363636363636</v>
@@ -84680,7 +84683,7 @@
     </row>
     <row r="2323">
       <c r="A2323" t="s">
-        <v>979</v>
+        <v>980</v>
       </c>
       <c r="B2323" s="1" t="n">
         <v>45657</v>
@@ -84689,7 +84692,7 @@
         <v>45503</v>
       </c>
       <c r="D2323" t="s">
-        <v>980</v>
+        <v>981</v>
       </c>
       <c r="E2323" t="n">
         <v>0.606060606060606</v>
@@ -84820,7 +84823,7 @@
     </row>
     <row r="2327">
       <c r="A2327" t="s">
-        <v>981</v>
+        <v>982</v>
       </c>
       <c r="B2327" s="1" t="n">
         <v>45657</v>
@@ -84829,7 +84832,7 @@
         <v>45504</v>
       </c>
       <c r="D2327" t="s">
-        <v>982</v>
+        <v>983</v>
       </c>
       <c r="E2327" t="n">
         <v>0.636363636363636</v>
@@ -85205,7 +85208,7 @@
     </row>
     <row r="2338">
       <c r="A2338" t="s">
-        <v>983</v>
+        <v>984</v>
       </c>
       <c r="B2338" s="1" t="n">
         <v>45657</v>
@@ -85214,7 +85217,7 @@
         <v>45488</v>
       </c>
       <c r="D2338" t="s">
-        <v>984</v>
+        <v>985</v>
       </c>
       <c r="E2338" t="n">
         <v>0.606060606060606</v>
@@ -85345,7 +85348,7 @@
     </row>
     <row r="2342">
       <c r="A2342" t="s">
-        <v>985</v>
+        <v>986</v>
       </c>
       <c r="B2342" s="1" t="n">
         <v>45382</v>
@@ -85354,7 +85357,7 @@
         <v>45230</v>
       </c>
       <c r="D2342" t="s">
-        <v>986</v>
+        <v>987</v>
       </c>
       <c r="E2342" t="n">
         <v>0.727272727272727</v>
@@ -85800,7 +85803,7 @@
     </row>
     <row r="2355">
       <c r="A2355" t="s">
-        <v>987</v>
+        <v>988</v>
       </c>
       <c r="B2355" s="1" t="n">
         <v>45657</v>
@@ -85809,7 +85812,7 @@
         <v>45503</v>
       </c>
       <c r="D2355" t="s">
-        <v>988</v>
+        <v>989</v>
       </c>
       <c r="E2355" t="n">
         <v>0.696969696969697</v>
@@ -85835,7 +85838,7 @@
     </row>
     <row r="2356">
       <c r="A2356" t="s">
-        <v>1007</v>
+        <v>1008</v>
       </c>
       <c r="B2356" s="1" t="n">
         <v>45657</v>
@@ -85844,7 +85847,7 @@
         <v>45504</v>
       </c>
       <c r="D2356" t="s">
-        <v>1008</v>
+        <v>1009</v>
       </c>
       <c r="E2356" t="n">
         <v>0.606060606060606</v>
@@ -85905,7 +85908,7 @@
     </row>
     <row r="2358">
       <c r="A2358" t="s">
-        <v>989</v>
+        <v>990</v>
       </c>
       <c r="B2358" s="1" t="n">
         <v>45657</v>
@@ -85914,7 +85917,7 @@
         <v>45502</v>
       </c>
       <c r="D2358" t="s">
-        <v>990</v>
+        <v>991</v>
       </c>
       <c r="E2358" t="n">
         <v>0.515151515151515</v>
@@ -86045,7 +86048,7 @@
     </row>
     <row r="2362">
       <c r="A2362" t="s">
-        <v>991</v>
+        <v>992</v>
       </c>
       <c r="B2362" s="1" t="n">
         <v>45657</v>
@@ -86054,7 +86057,7 @@
         <v>45504</v>
       </c>
       <c r="D2362" t="s">
-        <v>992</v>
+        <v>993</v>
       </c>
       <c r="E2362" t="n">
         <v>0.575757575757576</v>
@@ -86080,7 +86083,7 @@
     </row>
     <row r="2363">
       <c r="A2363" t="s">
-        <v>1009</v>
+        <v>1010</v>
       </c>
       <c r="B2363" s="1" t="n">
         <v>45657</v>
@@ -86089,7 +86092,7 @@
         <v>45503</v>
       </c>
       <c r="D2363" t="s">
-        <v>1010</v>
+        <v>1011</v>
       </c>
       <c r="E2363" t="n">
         <v>0.636363636363636</v>
@@ -86220,7 +86223,7 @@
     </row>
     <row r="2367">
       <c r="A2367" t="s">
-        <v>993</v>
+        <v>994</v>
       </c>
       <c r="B2367" s="1" t="n">
         <v>45657</v>
@@ -86229,7 +86232,7 @@
         <v>45628</v>
       </c>
       <c r="D2367" t="s">
-        <v>994</v>
+        <v>995</v>
       </c>
       <c r="E2367" t="n">
         <v>0.606060606060606</v>
@@ -86360,7 +86363,7 @@
     </row>
     <row r="2371">
       <c r="A2371" t="s">
-        <v>1011</v>
+        <v>1012</v>
       </c>
       <c r="B2371" s="1" t="n">
         <v>45657</v>
@@ -86369,7 +86372,7 @@
         <v>45503</v>
       </c>
       <c r="D2371" t="s">
-        <v>1012</v>
+        <v>1013</v>
       </c>
       <c r="E2371" t="n">
         <v>0.696969696969697</v>
@@ -86579,7 +86582,7 @@
         <v>45499</v>
       </c>
       <c r="D2377" t="s">
-        <v>570</v>
+        <v>931</v>
       </c>
       <c r="E2377" t="n">
         <v>0.575757575757576</v>
@@ -87025,7 +87028,7 @@
     </row>
     <row r="2390">
       <c r="A2390" t="s">
-        <v>931</v>
+        <v>932</v>
       </c>
       <c r="B2390" s="1" t="n">
         <v>45657</v>
@@ -87034,7 +87037,7 @@
         <v>45503</v>
       </c>
       <c r="D2390" t="s">
-        <v>932</v>
+        <v>933</v>
       </c>
       <c r="E2390" t="n">
         <v>0.606060606060606</v>
@@ -87095,7 +87098,7 @@
     </row>
     <row r="2392">
       <c r="A2392" t="s">
-        <v>935</v>
+        <v>936</v>
       </c>
       <c r="B2392" s="1" t="n">
         <v>45657</v>
@@ -87104,7 +87107,7 @@
         <v>45503</v>
       </c>
       <c r="D2392" t="s">
-        <v>936</v>
+        <v>937</v>
       </c>
       <c r="E2392" t="n">
         <v>0.666666666666667</v>
@@ -87795,7 +87798,7 @@
     </row>
     <row r="2412">
       <c r="A2412" t="s">
-        <v>937</v>
+        <v>938</v>
       </c>
       <c r="B2412" s="1" t="n">
         <v>45657</v>
@@ -87804,7 +87807,7 @@
         <v>45504</v>
       </c>
       <c r="D2412" t="s">
-        <v>938</v>
+        <v>939</v>
       </c>
       <c r="E2412" t="n">
         <v>0.606060606060606</v>
@@ -87970,7 +87973,7 @@
     </row>
     <row r="2417">
       <c r="A2417" t="s">
-        <v>941</v>
+        <v>942</v>
       </c>
       <c r="B2417" s="1" t="n">
         <v>45657</v>
@@ -87979,7 +87982,7 @@
         <v>45504</v>
       </c>
       <c r="D2417" t="s">
-        <v>942</v>
+        <v>943</v>
       </c>
       <c r="E2417" t="n">
         <v>0.575757575757576</v>
@@ -88145,7 +88148,7 @@
     </row>
     <row r="2422">
       <c r="A2422" t="s">
-        <v>997</v>
+        <v>998</v>
       </c>
       <c r="B2422" s="1" t="n">
         <v>45473</v>
@@ -88154,7 +88157,7 @@
         <v>45322</v>
       </c>
       <c r="D2422" t="s">
-        <v>998</v>
+        <v>999</v>
       </c>
       <c r="E2422" t="n">
         <v>0.575757575757576</v>
@@ -88250,7 +88253,7 @@
     </row>
     <row r="2425">
       <c r="A2425" t="s">
-        <v>943</v>
+        <v>944</v>
       </c>
       <c r="B2425" s="1" t="n">
         <v>45657</v>
@@ -88259,7 +88262,7 @@
         <v>45503</v>
       </c>
       <c r="D2425" t="s">
-        <v>944</v>
+        <v>945</v>
       </c>
       <c r="E2425" t="n">
         <v>0.696969696969697</v>
@@ -88530,7 +88533,7 @@
     </row>
     <row r="2433">
       <c r="A2433" t="s">
-        <v>945</v>
+        <v>946</v>
       </c>
       <c r="B2433" s="1" t="n">
         <v>45657</v>
@@ -88539,7 +88542,7 @@
         <v>45504</v>
       </c>
       <c r="D2433" t="s">
-        <v>946</v>
+        <v>947</v>
       </c>
       <c r="E2433" t="n">
         <v>0.696969696969697</v>
@@ -89510,7 +89513,7 @@
     </row>
     <row r="2461">
       <c r="A2461" t="s">
-        <v>947</v>
+        <v>948</v>
       </c>
       <c r="B2461" s="1" t="n">
         <v>45657</v>
@@ -89519,7 +89522,7 @@
         <v>45504</v>
       </c>
       <c r="D2461" t="s">
-        <v>948</v>
+        <v>949</v>
       </c>
       <c r="E2461" t="n">
         <v>0.696969696969697</v>
@@ -89580,7 +89583,7 @@
     </row>
     <row r="2463">
       <c r="A2463" t="s">
-        <v>949</v>
+        <v>950</v>
       </c>
       <c r="B2463" s="1" t="n">
         <v>45657</v>
@@ -89589,7 +89592,7 @@
         <v>45504</v>
       </c>
       <c r="D2463" t="s">
-        <v>950</v>
+        <v>951</v>
       </c>
       <c r="E2463" t="n">
         <v>0.575757575757576</v>

</xml_diff>

<commit_message>
Atualização de dados automática em 2025-03-25 12:30:02 (cron)
</commit_message>
<xml_diff>
--- a/public/docs/index_07_dim_CG.xlsx
+++ b/public/docs/index_07_dim_CG.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1021" uniqueCount="1021">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1023" uniqueCount="1023">
   <si>
     <t xml:space="preserve">CNPJ_Companhia</t>
   </si>
@@ -2696,6 +2696,9 @@
     <t xml:space="preserve">HUMBERG AGRIBRASIL COMÉRCIO E EXPORTAÇÃO DE GRÃOS S.A.</t>
   </si>
   <si>
+    <t xml:space="preserve">COMPANHIA INDUSTRIAL CATAGUASES</t>
+  </si>
+  <si>
     <t xml:space="preserve">19.796.586/0001-70</t>
   </si>
   <si>
@@ -2829,6 +2832,9 @@
   </si>
   <si>
     <t xml:space="preserve">RODOBENS SA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MAHLE METAL LEVE S.A.</t>
   </si>
   <si>
     <t xml:space="preserve">61.409.892/0001-73</t>
@@ -41120,7 +41126,7 @@
         <v>44400</v>
       </c>
       <c r="D1078" t="s">
-        <v>481</v>
+        <v>894</v>
       </c>
       <c r="E1078" t="n">
         <v>0.545454545454545</v>
@@ -41146,7 +41152,7 @@
     </row>
     <row r="1079">
       <c r="A1079" t="s">
-        <v>894</v>
+        <v>895</v>
       </c>
       <c r="B1079" s="1" t="n">
         <v>44561</v>
@@ -41155,7 +41161,7 @@
         <v>44410</v>
       </c>
       <c r="D1079" t="s">
-        <v>895</v>
+        <v>896</v>
       </c>
       <c r="E1079" t="n">
         <v>0.575757575757576</v>
@@ -41216,7 +41222,7 @@
     </row>
     <row r="1081">
       <c r="A1081" t="s">
-        <v>896</v>
+        <v>897</v>
       </c>
       <c r="B1081" s="1" t="n">
         <v>44561</v>
@@ -41225,7 +41231,7 @@
         <v>44407</v>
       </c>
       <c r="D1081" t="s">
-        <v>897</v>
+        <v>898</v>
       </c>
       <c r="E1081" t="n">
         <v>0.727272727272727</v>
@@ -41286,7 +41292,7 @@
     </row>
     <row r="1083">
       <c r="A1083" t="s">
-        <v>898</v>
+        <v>899</v>
       </c>
       <c r="B1083" s="1" t="n">
         <v>44561</v>
@@ -41295,7 +41301,7 @@
         <v>44407</v>
       </c>
       <c r="D1083" t="s">
-        <v>899</v>
+        <v>900</v>
       </c>
       <c r="E1083" t="n">
         <v>0.606060606060606</v>
@@ -41496,7 +41502,7 @@
     </row>
     <row r="1089">
       <c r="A1089" t="s">
-        <v>900</v>
+        <v>901</v>
       </c>
       <c r="B1089" s="1" t="n">
         <v>44561</v>
@@ -41505,7 +41511,7 @@
         <v>44407</v>
       </c>
       <c r="D1089" t="s">
-        <v>901</v>
+        <v>902</v>
       </c>
       <c r="E1089" t="n">
         <v>0.575757575757576</v>
@@ -41636,7 +41642,7 @@
     </row>
     <row r="1093">
       <c r="A1093" t="s">
-        <v>902</v>
+        <v>903</v>
       </c>
       <c r="B1093" s="1" t="n">
         <v>44561</v>
@@ -41645,7 +41651,7 @@
         <v>44407</v>
       </c>
       <c r="D1093" t="s">
-        <v>903</v>
+        <v>904</v>
       </c>
       <c r="E1093" t="n">
         <v>0.575757575757576</v>
@@ -41671,7 +41677,7 @@
     </row>
     <row r="1094">
       <c r="A1094" t="s">
-        <v>904</v>
+        <v>905</v>
       </c>
       <c r="B1094" s="1" t="n">
         <v>44561</v>
@@ -41680,7 +41686,7 @@
         <v>44410</v>
       </c>
       <c r="D1094" t="s">
-        <v>905</v>
+        <v>906</v>
       </c>
       <c r="E1094" t="n">
         <v>0.575757575757576</v>
@@ -41706,7 +41712,7 @@
     </row>
     <row r="1095">
       <c r="A1095" t="s">
-        <v>906</v>
+        <v>907</v>
       </c>
       <c r="B1095" s="1" t="n">
         <v>44561</v>
@@ -41715,7 +41721,7 @@
         <v>44407</v>
       </c>
       <c r="D1095" t="s">
-        <v>907</v>
+        <v>908</v>
       </c>
       <c r="E1095" t="n">
         <v>0.636363636363636</v>
@@ -41776,7 +41782,7 @@
     </row>
     <row r="1097">
       <c r="A1097" t="s">
-        <v>908</v>
+        <v>909</v>
       </c>
       <c r="B1097" s="1" t="n">
         <v>44561</v>
@@ -41785,7 +41791,7 @@
         <v>44407</v>
       </c>
       <c r="D1097" t="s">
-        <v>909</v>
+        <v>910</v>
       </c>
       <c r="E1097" t="n">
         <v>0.636363636363636</v>
@@ -41811,7 +41817,7 @@
     </row>
     <row r="1098">
       <c r="A1098" t="s">
-        <v>910</v>
+        <v>911</v>
       </c>
       <c r="B1098" s="1" t="n">
         <v>44561</v>
@@ -41820,7 +41826,7 @@
         <v>44407</v>
       </c>
       <c r="D1098" t="s">
-        <v>911</v>
+        <v>912</v>
       </c>
       <c r="E1098" t="n">
         <v>0.606060606060606</v>
@@ -42056,7 +42062,7 @@
     </row>
     <row r="1105">
       <c r="A1105" t="s">
-        <v>912</v>
+        <v>913</v>
       </c>
       <c r="B1105" s="1" t="n">
         <v>44561</v>
@@ -42065,7 +42071,7 @@
         <v>44407</v>
       </c>
       <c r="D1105" t="s">
-        <v>913</v>
+        <v>914</v>
       </c>
       <c r="E1105" t="n">
         <v>0.545454545454545</v>
@@ -42161,7 +42167,7 @@
     </row>
     <row r="1108">
       <c r="A1108" t="s">
-        <v>914</v>
+        <v>915</v>
       </c>
       <c r="B1108" s="1" t="n">
         <v>44561</v>
@@ -42170,7 +42176,7 @@
         <v>44410</v>
       </c>
       <c r="D1108" t="s">
-        <v>915</v>
+        <v>916</v>
       </c>
       <c r="E1108" t="n">
         <v>0.727272727272727</v>
@@ -42196,7 +42202,7 @@
     </row>
     <row r="1109">
       <c r="A1109" t="s">
-        <v>916</v>
+        <v>917</v>
       </c>
       <c r="B1109" s="1" t="n">
         <v>44561</v>
@@ -42205,7 +42211,7 @@
         <v>44407</v>
       </c>
       <c r="D1109" t="s">
-        <v>917</v>
+        <v>918</v>
       </c>
       <c r="E1109" t="n">
         <v>0.636363636363636</v>
@@ -42231,7 +42237,7 @@
     </row>
     <row r="1110">
       <c r="A1110" t="s">
-        <v>918</v>
+        <v>919</v>
       </c>
       <c r="B1110" s="1" t="n">
         <v>44561</v>
@@ -42240,7 +42246,7 @@
         <v>44410</v>
       </c>
       <c r="D1110" t="s">
-        <v>919</v>
+        <v>920</v>
       </c>
       <c r="E1110" t="n">
         <v>0.606060606060606</v>
@@ -43176,7 +43182,7 @@
     </row>
     <row r="1137">
       <c r="A1137" t="s">
-        <v>920</v>
+        <v>921</v>
       </c>
       <c r="B1137" s="1" t="n">
         <v>44561</v>
@@ -43185,7 +43191,7 @@
         <v>44223</v>
       </c>
       <c r="D1137" t="s">
-        <v>921</v>
+        <v>922</v>
       </c>
       <c r="E1137" t="n">
         <v>0.515151515151515</v>
@@ -43281,7 +43287,7 @@
     </row>
     <row r="1140">
       <c r="A1140" t="s">
-        <v>922</v>
+        <v>923</v>
       </c>
       <c r="B1140" s="1" t="n">
         <v>44561</v>
@@ -43290,7 +43296,7 @@
         <v>44407</v>
       </c>
       <c r="D1140" t="s">
-        <v>923</v>
+        <v>924</v>
       </c>
       <c r="E1140" t="n">
         <v>0.575757575757576</v>
@@ -43316,7 +43322,7 @@
     </row>
     <row r="1141">
       <c r="A1141" t="s">
-        <v>924</v>
+        <v>925</v>
       </c>
       <c r="B1141" s="1" t="n">
         <v>44561</v>
@@ -43325,7 +43331,7 @@
         <v>44407</v>
       </c>
       <c r="D1141" t="s">
-        <v>925</v>
+        <v>926</v>
       </c>
       <c r="E1141" t="n">
         <v>0.515151515151515</v>
@@ -43351,7 +43357,7 @@
     </row>
     <row r="1142">
       <c r="A1142" t="s">
-        <v>926</v>
+        <v>927</v>
       </c>
       <c r="B1142" s="1" t="n">
         <v>44561</v>
@@ -43360,7 +43366,7 @@
         <v>44407</v>
       </c>
       <c r="D1142" t="s">
-        <v>927</v>
+        <v>928</v>
       </c>
       <c r="E1142" t="n">
         <v>0.666666666666667</v>
@@ -43386,7 +43392,7 @@
     </row>
     <row r="1143">
       <c r="A1143" t="s">
-        <v>928</v>
+        <v>929</v>
       </c>
       <c r="B1143" s="1" t="n">
         <v>44561</v>
@@ -43395,7 +43401,7 @@
         <v>44410</v>
       </c>
       <c r="D1143" t="s">
-        <v>929</v>
+        <v>930</v>
       </c>
       <c r="E1143" t="n">
         <v>0.454545454545455</v>
@@ -43736,7 +43742,7 @@
     </row>
     <row r="1153">
       <c r="A1153" t="s">
-        <v>930</v>
+        <v>931</v>
       </c>
       <c r="B1153" s="1" t="n">
         <v>44561</v>
@@ -43745,7 +43751,7 @@
         <v>44411</v>
       </c>
       <c r="D1153" t="s">
-        <v>931</v>
+        <v>932</v>
       </c>
       <c r="E1153" t="n">
         <v>0.606060606060606</v>
@@ -44025,7 +44031,7 @@
         <v>44407</v>
       </c>
       <c r="D1161" t="s">
-        <v>932</v>
+        <v>933</v>
       </c>
       <c r="E1161" t="n">
         <v>0.575757575757576</v>
@@ -44576,7 +44582,7 @@
     </row>
     <row r="1177">
       <c r="A1177" t="s">
-        <v>933</v>
+        <v>934</v>
       </c>
       <c r="B1177" s="1" t="n">
         <v>44561</v>
@@ -44585,7 +44591,7 @@
         <v>44410</v>
       </c>
       <c r="D1177" t="s">
-        <v>934</v>
+        <v>935</v>
       </c>
       <c r="E1177" t="n">
         <v>0.575757575757576</v>
@@ -44611,7 +44617,7 @@
     </row>
     <row r="1178">
       <c r="A1178" t="s">
-        <v>935</v>
+        <v>936</v>
       </c>
       <c r="B1178" s="1" t="n">
         <v>44561</v>
@@ -44620,7 +44626,7 @@
         <v>44410</v>
       </c>
       <c r="D1178" t="s">
-        <v>936</v>
+        <v>937</v>
       </c>
       <c r="E1178" t="n">
         <v>0.575757575757576</v>
@@ -44681,7 +44687,7 @@
     </row>
     <row r="1180">
       <c r="A1180" t="s">
-        <v>937</v>
+        <v>938</v>
       </c>
       <c r="B1180" s="1" t="n">
         <v>44561</v>
@@ -44690,7 +44696,7 @@
         <v>44410</v>
       </c>
       <c r="D1180" t="s">
-        <v>938</v>
+        <v>939</v>
       </c>
       <c r="E1180" t="n">
         <v>0.666666666666667</v>
@@ -44760,7 +44766,7 @@
         <v>44406</v>
       </c>
       <c r="D1182" t="s">
-        <v>600</v>
+        <v>940</v>
       </c>
       <c r="E1182" t="n">
         <v>0.575757575757576</v>
@@ -45731,7 +45737,7 @@
     </row>
     <row r="1210">
       <c r="A1210" t="s">
-        <v>939</v>
+        <v>941</v>
       </c>
       <c r="B1210" s="1" t="n">
         <v>44561</v>
@@ -45740,7 +45746,7 @@
         <v>44407</v>
       </c>
       <c r="D1210" t="s">
-        <v>940</v>
+        <v>942</v>
       </c>
       <c r="E1210" t="n">
         <v>0.606060606060606</v>
@@ -46011,7 +46017,7 @@
     </row>
     <row r="1218">
       <c r="A1218" t="s">
-        <v>941</v>
+        <v>943</v>
       </c>
       <c r="B1218" s="1" t="n">
         <v>44561</v>
@@ -46020,7 +46026,7 @@
         <v>44410</v>
       </c>
       <c r="D1218" t="s">
-        <v>942</v>
+        <v>944</v>
       </c>
       <c r="E1218" t="n">
         <v>0.636363636363636</v>
@@ -46046,7 +46052,7 @@
     </row>
     <row r="1219">
       <c r="A1219" t="s">
-        <v>943</v>
+        <v>945</v>
       </c>
       <c r="B1219" s="1" t="n">
         <v>44561</v>
@@ -46055,7 +46061,7 @@
         <v>44404</v>
       </c>
       <c r="D1219" t="s">
-        <v>944</v>
+        <v>946</v>
       </c>
       <c r="E1219" t="n">
         <v>0.636363636363636</v>
@@ -46326,7 +46332,7 @@
     </row>
     <row r="1227">
       <c r="A1227" t="s">
-        <v>945</v>
+        <v>947</v>
       </c>
       <c r="B1227" s="1" t="n">
         <v>44561</v>
@@ -46335,7 +46341,7 @@
         <v>44410</v>
       </c>
       <c r="D1227" t="s">
-        <v>946</v>
+        <v>948</v>
       </c>
       <c r="E1227" t="n">
         <v>0.696969696969697</v>
@@ -46746,7 +46752,7 @@
     </row>
     <row r="1239">
       <c r="A1239" t="s">
-        <v>947</v>
+        <v>949</v>
       </c>
       <c r="B1239" s="1" t="n">
         <v>44561</v>
@@ -46755,7 +46761,7 @@
         <v>44407</v>
       </c>
       <c r="D1239" t="s">
-        <v>948</v>
+        <v>950</v>
       </c>
       <c r="E1239" t="n">
         <v>0.727272727272727</v>
@@ -48216,7 +48222,7 @@
     </row>
     <row r="1281">
       <c r="A1281" t="s">
-        <v>949</v>
+        <v>951</v>
       </c>
       <c r="B1281" s="1" t="n">
         <v>44561</v>
@@ -48225,7 +48231,7 @@
         <v>44406</v>
       </c>
       <c r="D1281" t="s">
-        <v>950</v>
+        <v>952</v>
       </c>
       <c r="E1281" t="n">
         <v>0.696969696969697</v>
@@ -48286,7 +48292,7 @@
     </row>
     <row r="1283">
       <c r="A1283" t="s">
-        <v>951</v>
+        <v>953</v>
       </c>
       <c r="B1283" s="1" t="n">
         <v>44561</v>
@@ -48295,7 +48301,7 @@
         <v>44406</v>
       </c>
       <c r="D1283" t="s">
-        <v>952</v>
+        <v>954</v>
       </c>
       <c r="E1283" t="n">
         <v>0.636363636363636</v>
@@ -48566,7 +48572,7 @@
     </row>
     <row r="1291">
       <c r="A1291" t="s">
-        <v>953</v>
+        <v>955</v>
       </c>
       <c r="B1291" s="1" t="n">
         <v>44926</v>
@@ -48575,7 +48581,7 @@
         <v>44761</v>
       </c>
       <c r="D1291" t="s">
-        <v>954</v>
+        <v>956</v>
       </c>
       <c r="E1291" t="n">
         <v>0.666666666666667</v>
@@ -48601,7 +48607,7 @@
     </row>
     <row r="1292">
       <c r="A1292" t="s">
-        <v>955</v>
+        <v>957</v>
       </c>
       <c r="B1292" s="1" t="n">
         <v>44926</v>
@@ -48610,7 +48616,7 @@
         <v>44774</v>
       </c>
       <c r="D1292" t="s">
-        <v>956</v>
+        <v>958</v>
       </c>
       <c r="E1292" t="n">
         <v>0.636363636363636</v>
@@ -50071,7 +50077,7 @@
     </row>
     <row r="1334">
       <c r="A1334" t="s">
-        <v>957</v>
+        <v>959</v>
       </c>
       <c r="B1334" s="1" t="n">
         <v>44651</v>
@@ -50080,7 +50086,7 @@
         <v>44501</v>
       </c>
       <c r="D1334" t="s">
-        <v>958</v>
+        <v>960</v>
       </c>
       <c r="E1334" t="n">
         <v>0.606060606060606</v>
@@ -50771,7 +50777,7 @@
     </row>
     <row r="1354">
       <c r="A1354" t="s">
-        <v>959</v>
+        <v>961</v>
       </c>
       <c r="B1354" s="1" t="n">
         <v>44926</v>
@@ -50780,7 +50786,7 @@
         <v>44755</v>
       </c>
       <c r="D1354" t="s">
-        <v>960</v>
+        <v>962</v>
       </c>
       <c r="E1354" t="n">
         <v>0.636363636363636</v>
@@ -50841,7 +50847,7 @@
     </row>
     <row r="1356">
       <c r="A1356" t="s">
-        <v>961</v>
+        <v>963</v>
       </c>
       <c r="B1356" s="1" t="n">
         <v>44926</v>
@@ -50850,7 +50856,7 @@
         <v>44771</v>
       </c>
       <c r="D1356" t="s">
-        <v>962</v>
+        <v>964</v>
       </c>
       <c r="E1356" t="n">
         <v>0.666666666666667</v>
@@ -52171,7 +52177,7 @@
     </row>
     <row r="1394">
       <c r="A1394" t="s">
-        <v>963</v>
+        <v>965</v>
       </c>
       <c r="B1394" s="1" t="n">
         <v>44926</v>
@@ -52180,7 +52186,7 @@
         <v>44760</v>
       </c>
       <c r="D1394" t="s">
-        <v>964</v>
+        <v>966</v>
       </c>
       <c r="E1394" t="n">
         <v>0.484848484848485</v>
@@ -53081,7 +53087,7 @@
     </row>
     <row r="1420">
       <c r="A1420" t="s">
-        <v>965</v>
+        <v>967</v>
       </c>
       <c r="B1420" s="1" t="n">
         <v>44926</v>
@@ -53090,7 +53096,7 @@
         <v>44770</v>
       </c>
       <c r="D1420" t="s">
-        <v>966</v>
+        <v>968</v>
       </c>
       <c r="E1420" t="n">
         <v>0.696969696969697</v>
@@ -54026,7 +54032,7 @@
     </row>
     <row r="1447">
       <c r="A1447" t="s">
-        <v>967</v>
+        <v>969</v>
       </c>
       <c r="B1447" s="1" t="n">
         <v>44926</v>
@@ -54035,7 +54041,7 @@
         <v>44771</v>
       </c>
       <c r="D1447" t="s">
-        <v>968</v>
+        <v>970</v>
       </c>
       <c r="E1447" t="n">
         <v>0.636363636363636</v>
@@ -54551,7 +54557,7 @@
     </row>
     <row r="1462">
       <c r="A1462" t="s">
-        <v>969</v>
+        <v>971</v>
       </c>
       <c r="B1462" s="1" t="n">
         <v>44926</v>
@@ -54560,7 +54566,7 @@
         <v>44773</v>
       </c>
       <c r="D1462" t="s">
-        <v>970</v>
+        <v>972</v>
       </c>
       <c r="E1462" t="n">
         <v>0.636363636363636</v>
@@ -54936,7 +54942,7 @@
     </row>
     <row r="1473">
       <c r="A1473" t="s">
-        <v>971</v>
+        <v>973</v>
       </c>
       <c r="B1473" s="1" t="n">
         <v>44926</v>
@@ -54945,7 +54951,7 @@
         <v>44762</v>
       </c>
       <c r="D1473" t="s">
-        <v>972</v>
+        <v>974</v>
       </c>
       <c r="E1473" t="n">
         <v>0.454545454545455</v>
@@ -56205,7 +56211,7 @@
         <v>44774</v>
       </c>
       <c r="D1509" t="s">
-        <v>481</v>
+        <v>894</v>
       </c>
       <c r="E1509" t="n">
         <v>0.545454545454545</v>
@@ -56231,7 +56237,7 @@
     </row>
     <row r="1510">
       <c r="A1510" t="s">
-        <v>894</v>
+        <v>895</v>
       </c>
       <c r="B1510" s="1" t="n">
         <v>44926</v>
@@ -56240,7 +56246,7 @@
         <v>44771</v>
       </c>
       <c r="D1510" t="s">
-        <v>895</v>
+        <v>896</v>
       </c>
       <c r="E1510" t="n">
         <v>0.636363636363636</v>
@@ -56266,7 +56272,7 @@
     </row>
     <row r="1511">
       <c r="A1511" t="s">
-        <v>896</v>
+        <v>897</v>
       </c>
       <c r="B1511" s="1" t="n">
         <v>44926</v>
@@ -56275,7 +56281,7 @@
         <v>44771</v>
       </c>
       <c r="D1511" t="s">
-        <v>897</v>
+        <v>898</v>
       </c>
       <c r="E1511" t="n">
         <v>0.757575757575758</v>
@@ -56336,7 +56342,7 @@
     </row>
     <row r="1513">
       <c r="A1513" t="s">
-        <v>898</v>
+        <v>899</v>
       </c>
       <c r="B1513" s="1" t="n">
         <v>44926</v>
@@ -56345,7 +56351,7 @@
         <v>44771</v>
       </c>
       <c r="D1513" t="s">
-        <v>899</v>
+        <v>900</v>
       </c>
       <c r="E1513" t="n">
         <v>0.636363636363636</v>
@@ -56511,7 +56517,7 @@
     </row>
     <row r="1518">
       <c r="A1518" t="s">
-        <v>900</v>
+        <v>901</v>
       </c>
       <c r="B1518" s="1" t="n">
         <v>44926</v>
@@ -56520,7 +56526,7 @@
         <v>44771</v>
       </c>
       <c r="D1518" t="s">
-        <v>901</v>
+        <v>902</v>
       </c>
       <c r="E1518" t="n">
         <v>0.575757575757576</v>
@@ -56581,7 +56587,7 @@
     </row>
     <row r="1520">
       <c r="A1520" t="s">
-        <v>973</v>
+        <v>975</v>
       </c>
       <c r="B1520" s="1" t="n">
         <v>44926</v>
@@ -56590,7 +56596,7 @@
         <v>44771</v>
       </c>
       <c r="D1520" t="s">
-        <v>974</v>
+        <v>976</v>
       </c>
       <c r="E1520" t="n">
         <v>0.727272727272727</v>
@@ -56686,7 +56692,7 @@
     </row>
     <row r="1523">
       <c r="A1523" t="s">
-        <v>975</v>
+        <v>977</v>
       </c>
       <c r="B1523" s="1" t="n">
         <v>44926</v>
@@ -56695,7 +56701,7 @@
         <v>44742</v>
       </c>
       <c r="D1523" t="s">
-        <v>976</v>
+        <v>978</v>
       </c>
       <c r="E1523" t="n">
         <v>0.606060606060606</v>
@@ -56721,7 +56727,7 @@
     </row>
     <row r="1524">
       <c r="A1524" t="s">
-        <v>977</v>
+        <v>979</v>
       </c>
       <c r="B1524" s="1" t="n">
         <v>44926</v>
@@ -56730,7 +56736,7 @@
         <v>44804</v>
       </c>
       <c r="D1524" t="s">
-        <v>978</v>
+        <v>980</v>
       </c>
       <c r="E1524" t="n">
         <v>0.515151515151515</v>
@@ -56756,7 +56762,7 @@
     </row>
     <row r="1525">
       <c r="A1525" t="s">
-        <v>902</v>
+        <v>903</v>
       </c>
       <c r="B1525" s="1" t="n">
         <v>44926</v>
@@ -56765,7 +56771,7 @@
         <v>44771</v>
       </c>
       <c r="D1525" t="s">
-        <v>903</v>
+        <v>904</v>
       </c>
       <c r="E1525" t="n">
         <v>0.636363636363636</v>
@@ -56791,7 +56797,7 @@
     </row>
     <row r="1526">
       <c r="A1526" t="s">
-        <v>979</v>
+        <v>981</v>
       </c>
       <c r="B1526" s="1" t="n">
         <v>44926</v>
@@ -56800,7 +56806,7 @@
         <v>44771</v>
       </c>
       <c r="D1526" t="s">
-        <v>980</v>
+        <v>982</v>
       </c>
       <c r="E1526" t="n">
         <v>0.575757575757576</v>
@@ -56826,7 +56832,7 @@
     </row>
     <row r="1527">
       <c r="A1527" t="s">
-        <v>906</v>
+        <v>907</v>
       </c>
       <c r="B1527" s="1" t="n">
         <v>44926</v>
@@ -56835,7 +56841,7 @@
         <v>44771</v>
       </c>
       <c r="D1527" t="s">
-        <v>907</v>
+        <v>908</v>
       </c>
       <c r="E1527" t="n">
         <v>0.606060606060606</v>
@@ -56896,7 +56902,7 @@
     </row>
     <row r="1529">
       <c r="A1529" t="s">
-        <v>908</v>
+        <v>909</v>
       </c>
       <c r="B1529" s="1" t="n">
         <v>44926</v>
@@ -56905,7 +56911,7 @@
         <v>44742</v>
       </c>
       <c r="D1529" t="s">
-        <v>909</v>
+        <v>910</v>
       </c>
       <c r="E1529" t="n">
         <v>0.636363636363636</v>
@@ -57036,7 +57042,7 @@
     </row>
     <row r="1533">
       <c r="A1533" t="s">
-        <v>981</v>
+        <v>983</v>
       </c>
       <c r="B1533" s="1" t="n">
         <v>44926</v>
@@ -57045,7 +57051,7 @@
         <v>44771</v>
       </c>
       <c r="D1533" t="s">
-        <v>982</v>
+        <v>984</v>
       </c>
       <c r="E1533" t="n">
         <v>0.515151515151515</v>
@@ -57176,7 +57182,7 @@
     </row>
     <row r="1537">
       <c r="A1537" t="s">
-        <v>912</v>
+        <v>913</v>
       </c>
       <c r="B1537" s="1" t="n">
         <v>44926</v>
@@ -57185,7 +57191,7 @@
         <v>44774</v>
       </c>
       <c r="D1537" t="s">
-        <v>913</v>
+        <v>914</v>
       </c>
       <c r="E1537" t="n">
         <v>0.575757575757576</v>
@@ -57281,7 +57287,7 @@
     </row>
     <row r="1540">
       <c r="A1540" t="s">
-        <v>914</v>
+        <v>915</v>
       </c>
       <c r="B1540" s="1" t="n">
         <v>44926</v>
@@ -57290,7 +57296,7 @@
         <v>44771</v>
       </c>
       <c r="D1540" t="s">
-        <v>915</v>
+        <v>916</v>
       </c>
       <c r="E1540" t="n">
         <v>0.666666666666667</v>
@@ -57316,7 +57322,7 @@
     </row>
     <row r="1541">
       <c r="A1541" t="s">
-        <v>916</v>
+        <v>917</v>
       </c>
       <c r="B1541" s="1" t="n">
         <v>44926</v>
@@ -57325,7 +57331,7 @@
         <v>44771</v>
       </c>
       <c r="D1541" t="s">
-        <v>917</v>
+        <v>918</v>
       </c>
       <c r="E1541" t="n">
         <v>0.696969696969697</v>
@@ -57351,7 +57357,7 @@
     </row>
     <row r="1542">
       <c r="A1542" t="s">
-        <v>918</v>
+        <v>919</v>
       </c>
       <c r="B1542" s="1" t="n">
         <v>44926</v>
@@ -57360,7 +57366,7 @@
         <v>44776</v>
       </c>
       <c r="D1542" t="s">
-        <v>919</v>
+        <v>920</v>
       </c>
       <c r="E1542" t="n">
         <v>0.606060606060606</v>
@@ -57386,7 +57392,7 @@
     </row>
     <row r="1543">
       <c r="A1543" t="s">
-        <v>983</v>
+        <v>985</v>
       </c>
       <c r="B1543" s="1" t="n">
         <v>44926</v>
@@ -57395,7 +57401,7 @@
         <v>44774</v>
       </c>
       <c r="D1543" t="s">
-        <v>984</v>
+        <v>986</v>
       </c>
       <c r="E1543" t="n">
         <v>0.515151515151515</v>
@@ -57806,7 +57812,7 @@
     </row>
     <row r="1555">
       <c r="A1555" t="s">
-        <v>985</v>
+        <v>987</v>
       </c>
       <c r="B1555" s="1" t="n">
         <v>44926</v>
@@ -57815,7 +57821,7 @@
         <v>44742</v>
       </c>
       <c r="D1555" t="s">
-        <v>986</v>
+        <v>988</v>
       </c>
       <c r="E1555" t="n">
         <v>0.606060606060606</v>
@@ -58051,7 +58057,7 @@
     </row>
     <row r="1562">
       <c r="A1562" t="s">
-        <v>987</v>
+        <v>989</v>
       </c>
       <c r="B1562" s="1" t="n">
         <v>44651</v>
@@ -58060,7 +58066,7 @@
         <v>44497</v>
       </c>
       <c r="D1562" t="s">
-        <v>988</v>
+        <v>990</v>
       </c>
       <c r="E1562" t="n">
         <v>0.757575757575758</v>
@@ -58436,7 +58442,7 @@
     </row>
     <row r="1573">
       <c r="A1573" t="s">
-        <v>922</v>
+        <v>923</v>
       </c>
       <c r="B1573" s="1" t="n">
         <v>44926</v>
@@ -58445,7 +58451,7 @@
         <v>44771</v>
       </c>
       <c r="D1573" t="s">
-        <v>923</v>
+        <v>924</v>
       </c>
       <c r="E1573" t="n">
         <v>0.606060606060606</v>
@@ -58471,7 +58477,7 @@
     </row>
     <row r="1574">
       <c r="A1574" t="s">
-        <v>924</v>
+        <v>925</v>
       </c>
       <c r="B1574" s="1" t="n">
         <v>44926</v>
@@ -58480,7 +58486,7 @@
         <v>44771</v>
       </c>
       <c r="D1574" t="s">
-        <v>925</v>
+        <v>926</v>
       </c>
       <c r="E1574" t="n">
         <v>0.515151515151515</v>
@@ -58506,7 +58512,7 @@
     </row>
     <row r="1575">
       <c r="A1575" t="s">
-        <v>926</v>
+        <v>927</v>
       </c>
       <c r="B1575" s="1" t="n">
         <v>44926</v>
@@ -58515,7 +58521,7 @@
         <v>44773</v>
       </c>
       <c r="D1575" t="s">
-        <v>927</v>
+        <v>928</v>
       </c>
       <c r="E1575" t="n">
         <v>0.636363636363636</v>
@@ -58541,7 +58547,7 @@
     </row>
     <row r="1576">
       <c r="A1576" t="s">
-        <v>989</v>
+        <v>991</v>
       </c>
       <c r="B1576" s="1" t="n">
         <v>44926</v>
@@ -58550,7 +58556,7 @@
         <v>44767</v>
       </c>
       <c r="D1576" t="s">
-        <v>990</v>
+        <v>992</v>
       </c>
       <c r="E1576" t="n">
         <v>0.424242424242424</v>
@@ -58576,7 +58582,7 @@
     </row>
     <row r="1577">
       <c r="A1577" t="s">
-        <v>928</v>
+        <v>929</v>
       </c>
       <c r="B1577" s="1" t="n">
         <v>44926</v>
@@ -58585,7 +58591,7 @@
         <v>44774</v>
       </c>
       <c r="D1577" t="s">
-        <v>929</v>
+        <v>930</v>
       </c>
       <c r="E1577" t="n">
         <v>0.424242424242424</v>
@@ -58646,7 +58652,7 @@
     </row>
     <row r="1579">
       <c r="A1579" t="s">
-        <v>991</v>
+        <v>993</v>
       </c>
       <c r="B1579" s="1" t="n">
         <v>44926</v>
@@ -58655,7 +58661,7 @@
         <v>44764</v>
       </c>
       <c r="D1579" t="s">
-        <v>992</v>
+        <v>994</v>
       </c>
       <c r="E1579" t="n">
         <v>0.515151515151515</v>
@@ -58786,7 +58792,7 @@
     </row>
     <row r="1583">
       <c r="A1583" t="s">
-        <v>993</v>
+        <v>995</v>
       </c>
       <c r="B1583" s="1" t="n">
         <v>44926</v>
@@ -58795,7 +58801,7 @@
         <v>44769</v>
       </c>
       <c r="D1583" t="s">
-        <v>994</v>
+        <v>996</v>
       </c>
       <c r="E1583" t="n">
         <v>0.636363636363636</v>
@@ -58961,7 +58967,7 @@
     </row>
     <row r="1588">
       <c r="A1588" t="s">
-        <v>995</v>
+        <v>997</v>
       </c>
       <c r="B1588" s="1" t="n">
         <v>44926</v>
@@ -58970,7 +58976,7 @@
         <v>44771</v>
       </c>
       <c r="D1588" t="s">
-        <v>996</v>
+        <v>998</v>
       </c>
       <c r="E1588" t="n">
         <v>0.606060606060606</v>
@@ -59031,7 +59037,7 @@
     </row>
     <row r="1590">
       <c r="A1590" t="s">
-        <v>930</v>
+        <v>931</v>
       </c>
       <c r="B1590" s="1" t="n">
         <v>44926</v>
@@ -59040,7 +59046,7 @@
         <v>44771</v>
       </c>
       <c r="D1590" t="s">
-        <v>931</v>
+        <v>932</v>
       </c>
       <c r="E1590" t="n">
         <v>0.636363636363636</v>
@@ -59320,7 +59326,7 @@
         <v>44768</v>
       </c>
       <c r="D1598" t="s">
-        <v>932</v>
+        <v>933</v>
       </c>
       <c r="E1598" t="n">
         <v>0.575757575757576</v>
@@ -59836,7 +59842,7 @@
     </row>
     <row r="1613">
       <c r="A1613" t="s">
-        <v>933</v>
+        <v>934</v>
       </c>
       <c r="B1613" s="1" t="n">
         <v>44926</v>
@@ -59845,7 +59851,7 @@
         <v>44774</v>
       </c>
       <c r="D1613" t="s">
-        <v>934</v>
+        <v>935</v>
       </c>
       <c r="E1613" t="n">
         <v>0.575757575757576</v>
@@ -59871,7 +59877,7 @@
     </row>
     <row r="1614">
       <c r="A1614" t="s">
-        <v>935</v>
+        <v>936</v>
       </c>
       <c r="B1614" s="1" t="n">
         <v>44926</v>
@@ -59880,7 +59886,7 @@
         <v>44771</v>
       </c>
       <c r="D1614" t="s">
-        <v>936</v>
+        <v>937</v>
       </c>
       <c r="E1614" t="n">
         <v>0.575757575757576</v>
@@ -59941,7 +59947,7 @@
     </row>
     <row r="1616">
       <c r="A1616" t="s">
-        <v>937</v>
+        <v>938</v>
       </c>
       <c r="B1616" s="1" t="n">
         <v>44926</v>
@@ -59950,7 +59956,7 @@
         <v>44774</v>
       </c>
       <c r="D1616" t="s">
-        <v>938</v>
+        <v>939</v>
       </c>
       <c r="E1616" t="n">
         <v>0.666666666666667</v>
@@ -60020,7 +60026,7 @@
         <v>44770</v>
       </c>
       <c r="D1618" t="s">
-        <v>600</v>
+        <v>940</v>
       </c>
       <c r="E1618" t="n">
         <v>0.636363636363636</v>
@@ -60886,7 +60892,7 @@
     </row>
     <row r="1643">
       <c r="A1643" t="s">
-        <v>997</v>
+        <v>999</v>
       </c>
       <c r="B1643" s="1" t="n">
         <v>44926</v>
@@ -60895,7 +60901,7 @@
         <v>44770</v>
       </c>
       <c r="D1643" t="s">
-        <v>998</v>
+        <v>1000</v>
       </c>
       <c r="E1643" t="n">
         <v>0.727272727272727</v>
@@ -60991,7 +60997,7 @@
     </row>
     <row r="1646">
       <c r="A1646" t="s">
-        <v>939</v>
+        <v>941</v>
       </c>
       <c r="B1646" s="1" t="n">
         <v>44926</v>
@@ -61000,7 +61006,7 @@
         <v>44767</v>
       </c>
       <c r="D1646" t="s">
-        <v>940</v>
+        <v>942</v>
       </c>
       <c r="E1646" t="n">
         <v>0.606060606060606</v>
@@ -61271,7 +61277,7 @@
     </row>
     <row r="1654">
       <c r="A1654" t="s">
-        <v>941</v>
+        <v>943</v>
       </c>
       <c r="B1654" s="1" t="n">
         <v>44926</v>
@@ -61280,7 +61286,7 @@
         <v>44774</v>
       </c>
       <c r="D1654" t="s">
-        <v>942</v>
+        <v>944</v>
       </c>
       <c r="E1654" t="n">
         <v>0.636363636363636</v>
@@ -61306,7 +61312,7 @@
     </row>
     <row r="1655">
       <c r="A1655" t="s">
-        <v>943</v>
+        <v>945</v>
       </c>
       <c r="B1655" s="1" t="n">
         <v>44926</v>
@@ -61315,7 +61321,7 @@
         <v>44771</v>
       </c>
       <c r="D1655" t="s">
-        <v>944</v>
+        <v>946</v>
       </c>
       <c r="E1655" t="n">
         <v>0.545454545454545</v>
@@ -61481,7 +61487,7 @@
     </row>
     <row r="1660">
       <c r="A1660" t="s">
-        <v>999</v>
+        <v>1001</v>
       </c>
       <c r="B1660" s="1" t="n">
         <v>44742</v>
@@ -61490,7 +61496,7 @@
         <v>44592</v>
       </c>
       <c r="D1660" t="s">
-        <v>1000</v>
+        <v>1002</v>
       </c>
       <c r="E1660" t="n">
         <v>0.606060606060606</v>
@@ -61621,7 +61627,7 @@
     </row>
     <row r="1664">
       <c r="A1664" t="s">
-        <v>945</v>
+        <v>947</v>
       </c>
       <c r="B1664" s="1" t="n">
         <v>44926</v>
@@ -61630,7 +61636,7 @@
         <v>44774</v>
       </c>
       <c r="D1664" t="s">
-        <v>946</v>
+        <v>948</v>
       </c>
       <c r="E1664" t="n">
         <v>0.696969696969697</v>
@@ -62006,7 +62012,7 @@
     </row>
     <row r="1675">
       <c r="A1675" t="s">
-        <v>947</v>
+        <v>949</v>
       </c>
       <c r="B1675" s="1" t="n">
         <v>44562</v>
@@ -62015,7 +62021,7 @@
         <v>44771</v>
       </c>
       <c r="D1675" t="s">
-        <v>948</v>
+        <v>950</v>
       </c>
       <c r="E1675" t="n">
         <v>0.727272727272727</v>
@@ -62041,7 +62047,7 @@
     </row>
     <row r="1676">
       <c r="A1676" t="s">
-        <v>947</v>
+        <v>949</v>
       </c>
       <c r="B1676" s="1" t="n">
         <v>44926</v>
@@ -62050,7 +62056,7 @@
         <v>44771</v>
       </c>
       <c r="D1676" t="s">
-        <v>948</v>
+        <v>950</v>
       </c>
       <c r="E1676" t="n">
         <v>0.727272727272727</v>
@@ -63476,7 +63482,7 @@
     </row>
     <row r="1717">
       <c r="A1717" t="s">
-        <v>949</v>
+        <v>951</v>
       </c>
       <c r="B1717" s="1" t="n">
         <v>44926</v>
@@ -63485,7 +63491,7 @@
         <v>44771</v>
       </c>
       <c r="D1717" t="s">
-        <v>950</v>
+        <v>952</v>
       </c>
       <c r="E1717" t="n">
         <v>0.696969696969697</v>
@@ -63546,7 +63552,7 @@
     </row>
     <row r="1719">
       <c r="A1719" t="s">
-        <v>951</v>
+        <v>953</v>
       </c>
       <c r="B1719" s="1" t="n">
         <v>44926</v>
@@ -63555,7 +63561,7 @@
         <v>44771</v>
       </c>
       <c r="D1719" t="s">
-        <v>952</v>
+        <v>954</v>
       </c>
       <c r="E1719" t="n">
         <v>0.636363636363636</v>
@@ -63826,7 +63832,7 @@
     </row>
     <row r="1727">
       <c r="A1727" t="s">
-        <v>953</v>
+        <v>955</v>
       </c>
       <c r="B1727" s="1" t="n">
         <v>45291</v>
@@ -63835,7 +63841,7 @@
         <v>45112</v>
       </c>
       <c r="D1727" t="s">
-        <v>954</v>
+        <v>956</v>
       </c>
       <c r="E1727" t="n">
         <v>0.666666666666667</v>
@@ -63861,7 +63867,7 @@
     </row>
     <row r="1728">
       <c r="A1728" t="s">
-        <v>955</v>
+        <v>957</v>
       </c>
       <c r="B1728" s="1" t="n">
         <v>45291</v>
@@ -63870,7 +63876,7 @@
         <v>45138</v>
       </c>
       <c r="D1728" t="s">
-        <v>956</v>
+        <v>958</v>
       </c>
       <c r="E1728" t="n">
         <v>0.636363636363636</v>
@@ -65191,7 +65197,7 @@
     </row>
     <row r="1766">
       <c r="A1766" t="s">
-        <v>957</v>
+        <v>959</v>
       </c>
       <c r="B1766" s="1" t="n">
         <v>45016</v>
@@ -65200,7 +65206,7 @@
         <v>44861</v>
       </c>
       <c r="D1766" t="s">
-        <v>958</v>
+        <v>960</v>
       </c>
       <c r="E1766" t="n">
         <v>0.606060606060606</v>
@@ -65821,7 +65827,7 @@
     </row>
     <row r="1784">
       <c r="A1784" t="s">
-        <v>959</v>
+        <v>961</v>
       </c>
       <c r="B1784" s="1" t="n">
         <v>45291</v>
@@ -65830,7 +65836,7 @@
         <v>45137</v>
       </c>
       <c r="D1784" t="s">
-        <v>960</v>
+        <v>962</v>
       </c>
       <c r="E1784" t="n">
         <v>0.636363636363636</v>
@@ -65891,7 +65897,7 @@
     </row>
     <row r="1786">
       <c r="A1786" t="s">
-        <v>961</v>
+        <v>963</v>
       </c>
       <c r="B1786" s="1" t="n">
         <v>45291</v>
@@ -65900,7 +65906,7 @@
         <v>45138</v>
       </c>
       <c r="D1786" t="s">
-        <v>962</v>
+        <v>964</v>
       </c>
       <c r="E1786" t="n">
         <v>0.666666666666667</v>
@@ -67151,7 +67157,7 @@
     </row>
     <row r="1822">
       <c r="A1822" t="s">
-        <v>963</v>
+        <v>965</v>
       </c>
       <c r="B1822" s="1" t="n">
         <v>45291</v>
@@ -67160,7 +67166,7 @@
         <v>45138</v>
       </c>
       <c r="D1822" t="s">
-        <v>964</v>
+        <v>966</v>
       </c>
       <c r="E1822" t="n">
         <v>0.484848484848485</v>
@@ -68061,7 +68067,7 @@
     </row>
     <row r="1848">
       <c r="A1848" t="s">
-        <v>965</v>
+        <v>967</v>
       </c>
       <c r="B1848" s="1" t="n">
         <v>45291</v>
@@ -68070,7 +68076,7 @@
         <v>45174</v>
       </c>
       <c r="D1848" t="s">
-        <v>966</v>
+        <v>968</v>
       </c>
       <c r="E1848" t="n">
         <v>0.636363636363636</v>
@@ -69391,7 +69397,7 @@
     </row>
     <row r="1886">
       <c r="A1886" t="s">
-        <v>969</v>
+        <v>971</v>
       </c>
       <c r="B1886" s="1" t="n">
         <v>45291</v>
@@ -69400,7 +69406,7 @@
         <v>45138</v>
       </c>
       <c r="D1886" t="s">
-        <v>970</v>
+        <v>972</v>
       </c>
       <c r="E1886" t="n">
         <v>0.636363636363636</v>
@@ -69776,7 +69782,7 @@
     </row>
     <row r="1897">
       <c r="A1897" t="s">
-        <v>971</v>
+        <v>973</v>
       </c>
       <c r="B1897" s="1" t="n">
         <v>45291</v>
@@ -69785,7 +69791,7 @@
         <v>45133</v>
       </c>
       <c r="D1897" t="s">
-        <v>972</v>
+        <v>974</v>
       </c>
       <c r="E1897" t="n">
         <v>0.454545454545455</v>
@@ -70931,7 +70937,7 @@
     </row>
     <row r="1930">
       <c r="A1930" t="s">
-        <v>1001</v>
+        <v>1003</v>
       </c>
       <c r="B1930" s="1" t="n">
         <v>45291</v>
@@ -70940,7 +70946,7 @@
         <v>45138</v>
       </c>
       <c r="D1930" t="s">
-        <v>1002</v>
+        <v>1004</v>
       </c>
       <c r="E1930" t="n">
         <v>0.636363636363636</v>
@@ -70975,7 +70981,7 @@
         <v>45141</v>
       </c>
       <c r="D1931" t="s">
-        <v>481</v>
+        <v>894</v>
       </c>
       <c r="E1931" t="n">
         <v>0.545454545454545</v>
@@ -71001,7 +71007,7 @@
     </row>
     <row r="1932">
       <c r="A1932" t="s">
-        <v>894</v>
+        <v>895</v>
       </c>
       <c r="B1932" s="1" t="n">
         <v>45291</v>
@@ -71010,7 +71016,7 @@
         <v>45135</v>
       </c>
       <c r="D1932" t="s">
-        <v>895</v>
+        <v>896</v>
       </c>
       <c r="E1932" t="n">
         <v>0.606060606060606</v>
@@ -71036,7 +71042,7 @@
     </row>
     <row r="1933">
       <c r="A1933" t="s">
-        <v>896</v>
+        <v>897</v>
       </c>
       <c r="B1933" s="1" t="n">
         <v>45291</v>
@@ -71045,7 +71051,7 @@
         <v>45138</v>
       </c>
       <c r="D1933" t="s">
-        <v>897</v>
+        <v>898</v>
       </c>
       <c r="E1933" t="n">
         <v>0.757575757575758</v>
@@ -71106,7 +71112,7 @@
     </row>
     <row r="1935">
       <c r="A1935" t="s">
-        <v>898</v>
+        <v>899</v>
       </c>
       <c r="B1935" s="1" t="n">
         <v>45291</v>
@@ -71115,7 +71121,7 @@
         <v>45138</v>
       </c>
       <c r="D1935" t="s">
-        <v>899</v>
+        <v>900</v>
       </c>
       <c r="E1935" t="n">
         <v>0.696969696969697</v>
@@ -71141,7 +71147,7 @@
     </row>
     <row r="1936">
       <c r="A1936" t="s">
-        <v>1003</v>
+        <v>1005</v>
       </c>
       <c r="B1936" s="1" t="n">
         <v>45291</v>
@@ -71150,7 +71156,7 @@
         <v>45134</v>
       </c>
       <c r="D1936" t="s">
-        <v>1004</v>
+        <v>1006</v>
       </c>
       <c r="E1936" t="n">
         <v>0.575757575757576</v>
@@ -71316,7 +71322,7 @@
     </row>
     <row r="1941">
       <c r="A1941" t="s">
-        <v>900</v>
+        <v>901</v>
       </c>
       <c r="B1941" s="1" t="n">
         <v>45291</v>
@@ -71325,7 +71331,7 @@
         <v>45135</v>
       </c>
       <c r="D1941" t="s">
-        <v>901</v>
+        <v>902</v>
       </c>
       <c r="E1941" t="n">
         <v>0.575757575757576</v>
@@ -71386,7 +71392,7 @@
     </row>
     <row r="1943">
       <c r="A1943" t="s">
-        <v>973</v>
+        <v>975</v>
       </c>
       <c r="B1943" s="1" t="n">
         <v>45291</v>
@@ -71395,7 +71401,7 @@
         <v>45138</v>
       </c>
       <c r="D1943" t="s">
-        <v>974</v>
+        <v>976</v>
       </c>
       <c r="E1943" t="n">
         <v>0.727272727272727</v>
@@ -71456,7 +71462,7 @@
     </row>
     <row r="1945">
       <c r="A1945" t="s">
-        <v>1005</v>
+        <v>1007</v>
       </c>
       <c r="B1945" s="1" t="n">
         <v>45291</v>
@@ -71465,7 +71471,7 @@
         <v>45135</v>
       </c>
       <c r="D1945" t="s">
-        <v>1006</v>
+        <v>1008</v>
       </c>
       <c r="E1945" t="n">
         <v>0.696969696969697</v>
@@ -71526,7 +71532,7 @@
     </row>
     <row r="1947">
       <c r="A1947" t="s">
-        <v>975</v>
+        <v>977</v>
       </c>
       <c r="B1947" s="1" t="n">
         <v>45291</v>
@@ -71535,7 +71541,7 @@
         <v>45135</v>
       </c>
       <c r="D1947" t="s">
-        <v>976</v>
+        <v>978</v>
       </c>
       <c r="E1947" t="n">
         <v>0.636363636363636</v>
@@ -71561,7 +71567,7 @@
     </row>
     <row r="1948">
       <c r="A1948" t="s">
-        <v>902</v>
+        <v>903</v>
       </c>
       <c r="B1948" s="1" t="n">
         <v>45291</v>
@@ -71570,7 +71576,7 @@
         <v>45135</v>
       </c>
       <c r="D1948" t="s">
-        <v>903</v>
+        <v>904</v>
       </c>
       <c r="E1948" t="n">
         <v>0.575757575757576</v>
@@ -71596,7 +71602,7 @@
     </row>
     <row r="1949">
       <c r="A1949" t="s">
-        <v>906</v>
+        <v>907</v>
       </c>
       <c r="B1949" s="1" t="n">
         <v>45291</v>
@@ -71605,7 +71611,7 @@
         <v>45135</v>
       </c>
       <c r="D1949" t="s">
-        <v>907</v>
+        <v>908</v>
       </c>
       <c r="E1949" t="n">
         <v>0.606060606060606</v>
@@ -71666,7 +71672,7 @@
     </row>
     <row r="1951">
       <c r="A1951" t="s">
-        <v>908</v>
+        <v>909</v>
       </c>
       <c r="B1951" s="1" t="n">
         <v>45291</v>
@@ -71675,7 +71681,7 @@
         <v>45138</v>
       </c>
       <c r="D1951" t="s">
-        <v>909</v>
+        <v>910</v>
       </c>
       <c r="E1951" t="n">
         <v>0.666666666666667</v>
@@ -71806,7 +71812,7 @@
     </row>
     <row r="1955">
       <c r="A1955" t="s">
-        <v>981</v>
+        <v>983</v>
       </c>
       <c r="B1955" s="1" t="n">
         <v>45291</v>
@@ -71815,7 +71821,7 @@
         <v>45138</v>
       </c>
       <c r="D1955" t="s">
-        <v>982</v>
+        <v>984</v>
       </c>
       <c r="E1955" t="n">
         <v>0.606060606060606</v>
@@ -71911,7 +71917,7 @@
     </row>
     <row r="1958">
       <c r="A1958" t="s">
-        <v>912</v>
+        <v>913</v>
       </c>
       <c r="B1958" s="1" t="n">
         <v>45291</v>
@@ -71920,7 +71926,7 @@
         <v>45138</v>
       </c>
       <c r="D1958" t="s">
-        <v>913</v>
+        <v>914</v>
       </c>
       <c r="E1958" t="n">
         <v>0.545454545454545</v>
@@ -72016,7 +72022,7 @@
     </row>
     <row r="1961">
       <c r="A1961" t="s">
-        <v>914</v>
+        <v>915</v>
       </c>
       <c r="B1961" s="1" t="n">
         <v>45291</v>
@@ -72025,7 +72031,7 @@
         <v>45138</v>
       </c>
       <c r="D1961" t="s">
-        <v>915</v>
+        <v>916</v>
       </c>
       <c r="E1961" t="n">
         <v>0.666666666666667</v>
@@ -72051,7 +72057,7 @@
     </row>
     <row r="1962">
       <c r="A1962" t="s">
-        <v>916</v>
+        <v>917</v>
       </c>
       <c r="B1962" s="1" t="n">
         <v>45291</v>
@@ -72060,7 +72066,7 @@
         <v>45133</v>
       </c>
       <c r="D1962" t="s">
-        <v>917</v>
+        <v>918</v>
       </c>
       <c r="E1962" t="n">
         <v>0.696969696969697</v>
@@ -72086,7 +72092,7 @@
     </row>
     <row r="1963">
       <c r="A1963" t="s">
-        <v>983</v>
+        <v>985</v>
       </c>
       <c r="B1963" s="1" t="n">
         <v>45291</v>
@@ -72095,7 +72101,7 @@
         <v>45138</v>
       </c>
       <c r="D1963" t="s">
-        <v>984</v>
+        <v>986</v>
       </c>
       <c r="E1963" t="n">
         <v>0.515151515151515</v>
@@ -72471,7 +72477,7 @@
     </row>
     <row r="1974">
       <c r="A1974" t="s">
-        <v>985</v>
+        <v>987</v>
       </c>
       <c r="B1974" s="1" t="n">
         <v>45291</v>
@@ -72480,7 +72486,7 @@
         <v>45106</v>
       </c>
       <c r="D1974" t="s">
-        <v>986</v>
+        <v>988</v>
       </c>
       <c r="E1974" t="n">
         <v>0.606060606060606</v>
@@ -72716,7 +72722,7 @@
     </row>
     <row r="1981">
       <c r="A1981" t="s">
-        <v>987</v>
+        <v>989</v>
       </c>
       <c r="B1981" s="1" t="n">
         <v>45016</v>
@@ -72725,7 +72731,7 @@
         <v>44865</v>
       </c>
       <c r="D1981" t="s">
-        <v>988</v>
+        <v>990</v>
       </c>
       <c r="E1981" t="n">
         <v>0.757575757575758</v>
@@ -73101,7 +73107,7 @@
     </row>
     <row r="1992">
       <c r="A1992" t="s">
-        <v>922</v>
+        <v>923</v>
       </c>
       <c r="B1992" s="1" t="n">
         <v>45291</v>
@@ -73110,7 +73116,7 @@
         <v>45138</v>
       </c>
       <c r="D1992" t="s">
-        <v>923</v>
+        <v>924</v>
       </c>
       <c r="E1992" t="n">
         <v>0.606060606060606</v>
@@ -73136,7 +73142,7 @@
     </row>
     <row r="1993">
       <c r="A1993" t="s">
-        <v>924</v>
+        <v>925</v>
       </c>
       <c r="B1993" s="1" t="n">
         <v>45291</v>
@@ -73145,7 +73151,7 @@
         <v>45135</v>
       </c>
       <c r="D1993" t="s">
-        <v>925</v>
+        <v>926</v>
       </c>
       <c r="E1993" t="n">
         <v>0.515151515151515</v>
@@ -73171,7 +73177,7 @@
     </row>
     <row r="1994">
       <c r="A1994" t="s">
-        <v>926</v>
+        <v>927</v>
       </c>
       <c r="B1994" s="1" t="n">
         <v>45291</v>
@@ -73180,7 +73186,7 @@
         <v>45139</v>
       </c>
       <c r="D1994" t="s">
-        <v>927</v>
+        <v>928</v>
       </c>
       <c r="E1994" t="n">
         <v>0.636363636363636</v>
@@ -73206,7 +73212,7 @@
     </row>
     <row r="1995">
       <c r="A1995" t="s">
-        <v>1007</v>
+        <v>1009</v>
       </c>
       <c r="B1995" s="1" t="n">
         <v>45291</v>
@@ -73215,7 +73221,7 @@
         <v>45134</v>
       </c>
       <c r="D1995" t="s">
-        <v>1008</v>
+        <v>1010</v>
       </c>
       <c r="E1995" t="n">
         <v>0.636363636363636</v>
@@ -73241,7 +73247,7 @@
     </row>
     <row r="1996">
       <c r="A1996" t="s">
-        <v>989</v>
+        <v>991</v>
       </c>
       <c r="B1996" s="1" t="n">
         <v>45291</v>
@@ -73250,7 +73256,7 @@
         <v>45138</v>
       </c>
       <c r="D1996" t="s">
-        <v>990</v>
+        <v>992</v>
       </c>
       <c r="E1996" t="n">
         <v>0.696969696969697</v>
@@ -73276,7 +73282,7 @@
     </row>
     <row r="1997">
       <c r="A1997" t="s">
-        <v>928</v>
+        <v>929</v>
       </c>
       <c r="B1997" s="1" t="n">
         <v>45291</v>
@@ -73285,7 +73291,7 @@
         <v>45138</v>
       </c>
       <c r="D1997" t="s">
-        <v>929</v>
+        <v>930</v>
       </c>
       <c r="E1997" t="n">
         <v>0.424242424242424</v>
@@ -73311,7 +73317,7 @@
     </row>
     <row r="1998">
       <c r="A1998" t="s">
-        <v>1009</v>
+        <v>1011</v>
       </c>
       <c r="B1998" s="1" t="n">
         <v>45291</v>
@@ -73320,7 +73326,7 @@
         <v>45138</v>
       </c>
       <c r="D1998" t="s">
-        <v>1010</v>
+        <v>1012</v>
       </c>
       <c r="E1998" t="n">
         <v>0.606060606060606</v>
@@ -73381,7 +73387,7 @@
     </row>
     <row r="2000">
       <c r="A2000" t="s">
-        <v>991</v>
+        <v>993</v>
       </c>
       <c r="B2000" s="1" t="n">
         <v>45291</v>
@@ -73390,7 +73396,7 @@
         <v>45132</v>
       </c>
       <c r="D2000" t="s">
-        <v>992</v>
+        <v>994</v>
       </c>
       <c r="E2000" t="n">
         <v>0.515151515151515</v>
@@ -73521,7 +73527,7 @@
     </row>
     <row r="2004">
       <c r="A2004" t="s">
-        <v>993</v>
+        <v>995</v>
       </c>
       <c r="B2004" s="1" t="n">
         <v>45291</v>
@@ -73530,7 +73536,7 @@
         <v>45135</v>
       </c>
       <c r="D2004" t="s">
-        <v>994</v>
+        <v>996</v>
       </c>
       <c r="E2004" t="n">
         <v>0.606060606060606</v>
@@ -73556,7 +73562,7 @@
     </row>
     <row r="2005">
       <c r="A2005" t="s">
-        <v>1011</v>
+        <v>1013</v>
       </c>
       <c r="B2005" s="1" t="n">
         <v>45291</v>
@@ -73565,7 +73571,7 @@
         <v>45138</v>
       </c>
       <c r="D2005" t="s">
-        <v>1012</v>
+        <v>1014</v>
       </c>
       <c r="E2005" t="n">
         <v>0.606060606060606</v>
@@ -73696,7 +73702,7 @@
     </row>
     <row r="2009">
       <c r="A2009" t="s">
-        <v>995</v>
+        <v>997</v>
       </c>
       <c r="B2009" s="1" t="n">
         <v>45291</v>
@@ -73705,7 +73711,7 @@
         <v>45138</v>
       </c>
       <c r="D2009" t="s">
-        <v>996</v>
+        <v>998</v>
       </c>
       <c r="E2009" t="n">
         <v>0.606060606060606</v>
@@ -73766,7 +73772,7 @@
     </row>
     <row r="2011">
       <c r="A2011" t="s">
-        <v>930</v>
+        <v>931</v>
       </c>
       <c r="B2011" s="1" t="n">
         <v>45291</v>
@@ -73775,7 +73781,7 @@
         <v>45132</v>
       </c>
       <c r="D2011" t="s">
-        <v>931</v>
+        <v>932</v>
       </c>
       <c r="E2011" t="n">
         <v>0.606060606060606</v>
@@ -73836,7 +73842,7 @@
     </row>
     <row r="2013">
       <c r="A2013" t="s">
-        <v>1013</v>
+        <v>1015</v>
       </c>
       <c r="B2013" s="1" t="n">
         <v>45291</v>
@@ -73845,7 +73851,7 @@
         <v>45128</v>
       </c>
       <c r="D2013" t="s">
-        <v>1014</v>
+        <v>1016</v>
       </c>
       <c r="E2013" t="n">
         <v>0.696969696969697</v>
@@ -74090,7 +74096,7 @@
         <v>45135</v>
       </c>
       <c r="D2020" t="s">
-        <v>932</v>
+        <v>933</v>
       </c>
       <c r="E2020" t="n">
         <v>0.575757575757576</v>
@@ -74606,7 +74612,7 @@
     </row>
     <row r="2035">
       <c r="A2035" t="s">
-        <v>933</v>
+        <v>934</v>
       </c>
       <c r="B2035" s="1" t="n">
         <v>45291</v>
@@ -74615,7 +74621,7 @@
         <v>45138</v>
       </c>
       <c r="D2035" t="s">
-        <v>934</v>
+        <v>935</v>
       </c>
       <c r="E2035" t="n">
         <v>0.575757575757576</v>
@@ -74641,7 +74647,7 @@
     </row>
     <row r="2036">
       <c r="A2036" t="s">
-        <v>935</v>
+        <v>936</v>
       </c>
       <c r="B2036" s="1" t="n">
         <v>45291</v>
@@ -74650,7 +74656,7 @@
         <v>45138</v>
       </c>
       <c r="D2036" t="s">
-        <v>936</v>
+        <v>937</v>
       </c>
       <c r="E2036" t="n">
         <v>0.606060606060606</v>
@@ -74711,7 +74717,7 @@
     </row>
     <row r="2038">
       <c r="A2038" t="s">
-        <v>937</v>
+        <v>938</v>
       </c>
       <c r="B2038" s="1" t="n">
         <v>45291</v>
@@ -74720,7 +74726,7 @@
         <v>45138</v>
       </c>
       <c r="D2038" t="s">
-        <v>938</v>
+        <v>939</v>
       </c>
       <c r="E2038" t="n">
         <v>0.666666666666667</v>
@@ -74790,7 +74796,7 @@
         <v>45138</v>
       </c>
       <c r="D2040" t="s">
-        <v>600</v>
+        <v>940</v>
       </c>
       <c r="E2040" t="n">
         <v>0.666666666666667</v>
@@ -75621,7 +75627,7 @@
     </row>
     <row r="2064">
       <c r="A2064" t="s">
-        <v>997</v>
+        <v>999</v>
       </c>
       <c r="B2064" s="1" t="n">
         <v>45291</v>
@@ -75630,7 +75636,7 @@
         <v>45132</v>
       </c>
       <c r="D2064" t="s">
-        <v>998</v>
+        <v>1000</v>
       </c>
       <c r="E2064" t="n">
         <v>0.757575757575758</v>
@@ -75726,7 +75732,7 @@
     </row>
     <row r="2067">
       <c r="A2067" t="s">
-        <v>939</v>
+        <v>941</v>
       </c>
       <c r="B2067" s="1" t="n">
         <v>45291</v>
@@ -75735,7 +75741,7 @@
         <v>45135</v>
       </c>
       <c r="D2067" t="s">
-        <v>940</v>
+        <v>942</v>
       </c>
       <c r="E2067" t="n">
         <v>0.666666666666667</v>
@@ -76006,7 +76012,7 @@
     </row>
     <row r="2075">
       <c r="A2075" t="s">
-        <v>943</v>
+        <v>945</v>
       </c>
       <c r="B2075" s="1" t="n">
         <v>45291</v>
@@ -76015,7 +76021,7 @@
         <v>45138</v>
       </c>
       <c r="D2075" t="s">
-        <v>944</v>
+        <v>946</v>
       </c>
       <c r="E2075" t="n">
         <v>0.575757575757576</v>
@@ -76181,7 +76187,7 @@
     </row>
     <row r="2080">
       <c r="A2080" t="s">
-        <v>999</v>
+        <v>1001</v>
       </c>
       <c r="B2080" s="1" t="n">
         <v>45107</v>
@@ -76190,7 +76196,7 @@
         <v>44944</v>
       </c>
       <c r="D2080" t="s">
-        <v>1000</v>
+        <v>1002</v>
       </c>
       <c r="E2080" t="n">
         <v>0.636363636363636</v>
@@ -76321,7 +76327,7 @@
     </row>
     <row r="2084">
       <c r="A2084" t="s">
-        <v>945</v>
+        <v>947</v>
       </c>
       <c r="B2084" s="1" t="n">
         <v>45291</v>
@@ -76330,7 +76336,7 @@
         <v>45128</v>
       </c>
       <c r="D2084" t="s">
-        <v>946</v>
+        <v>948</v>
       </c>
       <c r="E2084" t="n">
         <v>0.696969696969697</v>
@@ -76671,7 +76677,7 @@
     </row>
     <row r="2094">
       <c r="A2094" t="s">
-        <v>947</v>
+        <v>949</v>
       </c>
       <c r="B2094" s="1" t="n">
         <v>45291</v>
@@ -76680,7 +76686,7 @@
         <v>45138</v>
       </c>
       <c r="D2094" t="s">
-        <v>948</v>
+        <v>950</v>
       </c>
       <c r="E2094" t="n">
         <v>0.696969696969697</v>
@@ -78071,7 +78077,7 @@
     </row>
     <row r="2134">
       <c r="A2134" t="s">
-        <v>949</v>
+        <v>951</v>
       </c>
       <c r="B2134" s="1" t="n">
         <v>45291</v>
@@ -78080,7 +78086,7 @@
         <v>45138</v>
       </c>
       <c r="D2134" t="s">
-        <v>950</v>
+        <v>952</v>
       </c>
       <c r="E2134" t="n">
         <v>0.696969696969697</v>
@@ -78141,7 +78147,7 @@
     </row>
     <row r="2136">
       <c r="A2136" t="s">
-        <v>951</v>
+        <v>953</v>
       </c>
       <c r="B2136" s="1" t="n">
         <v>45291</v>
@@ -78150,7 +78156,7 @@
         <v>45135</v>
       </c>
       <c r="D2136" t="s">
-        <v>952</v>
+        <v>954</v>
       </c>
       <c r="E2136" t="n">
         <v>0.666666666666667</v>
@@ -78421,7 +78427,7 @@
     </row>
     <row r="2144">
       <c r="A2144" t="s">
-        <v>953</v>
+        <v>955</v>
       </c>
       <c r="B2144" s="1" t="n">
         <v>45657</v>
@@ -78430,7 +78436,7 @@
         <v>45503</v>
       </c>
       <c r="D2144" t="s">
-        <v>954</v>
+        <v>956</v>
       </c>
       <c r="E2144" t="n">
         <v>0.666666666666667</v>
@@ -78456,7 +78462,7 @@
     </row>
     <row r="2145">
       <c r="A2145" t="s">
-        <v>955</v>
+        <v>957</v>
       </c>
       <c r="B2145" s="1" t="n">
         <v>45657</v>
@@ -78465,7 +78471,7 @@
         <v>45504</v>
       </c>
       <c r="D2145" t="s">
-        <v>956</v>
+        <v>958</v>
       </c>
       <c r="E2145" t="n">
         <v>0.636363636363636</v>
@@ -79576,7 +79582,7 @@
     </row>
     <row r="2177">
       <c r="A2177" t="s">
-        <v>957</v>
+        <v>959</v>
       </c>
       <c r="B2177" s="1" t="n">
         <v>45382</v>
@@ -79585,7 +79591,7 @@
         <v>45230</v>
       </c>
       <c r="D2177" t="s">
-        <v>958</v>
+        <v>960</v>
       </c>
       <c r="E2177" t="n">
         <v>0.606060606060606</v>
@@ -80066,7 +80072,7 @@
     </row>
     <row r="2191">
       <c r="A2191" t="s">
-        <v>959</v>
+        <v>961</v>
       </c>
       <c r="B2191" s="1" t="n">
         <v>45657</v>
@@ -80075,7 +80081,7 @@
         <v>45489</v>
       </c>
       <c r="D2191" t="s">
-        <v>960</v>
+        <v>962</v>
       </c>
       <c r="E2191" t="n">
         <v>0.636363636363636</v>
@@ -81641,7 +81647,7 @@
     </row>
     <row r="2236">
       <c r="A2236" t="s">
-        <v>965</v>
+        <v>967</v>
       </c>
       <c r="B2236" s="1" t="n">
         <v>45657</v>
@@ -81650,7 +81656,7 @@
         <v>45492</v>
       </c>
       <c r="D2236" t="s">
-        <v>966</v>
+        <v>968</v>
       </c>
       <c r="E2236" t="n">
         <v>0.636363636363636</v>
@@ -82761,7 +82767,7 @@
     </row>
     <row r="2268">
       <c r="A2268" t="s">
-        <v>969</v>
+        <v>971</v>
       </c>
       <c r="B2268" s="1" t="n">
         <v>45657</v>
@@ -82770,7 +82776,7 @@
         <v>45504</v>
       </c>
       <c r="D2268" t="s">
-        <v>970</v>
+        <v>972</v>
       </c>
       <c r="E2268" t="n">
         <v>0.636363636363636</v>
@@ -83111,7 +83117,7 @@
     </row>
     <row r="2278">
       <c r="A2278" t="s">
-        <v>971</v>
+        <v>973</v>
       </c>
       <c r="B2278" s="1" t="n">
         <v>45657</v>
@@ -83120,7 +83126,7 @@
         <v>45503</v>
       </c>
       <c r="D2278" t="s">
-        <v>972</v>
+        <v>974</v>
       </c>
       <c r="E2278" t="n">
         <v>0.454545454545455</v>
@@ -83951,7 +83957,7 @@
     </row>
     <row r="2302">
       <c r="A2302" t="s">
-        <v>1001</v>
+        <v>1003</v>
       </c>
       <c r="B2302" s="1" t="n">
         <v>45657</v>
@@ -83960,7 +83966,7 @@
         <v>45504</v>
       </c>
       <c r="D2302" t="s">
-        <v>1002</v>
+        <v>1004</v>
       </c>
       <c r="E2302" t="n">
         <v>0.636363636363636</v>
@@ -83995,7 +84001,7 @@
         <v>45504</v>
       </c>
       <c r="D2303" t="s">
-        <v>481</v>
+        <v>894</v>
       </c>
       <c r="E2303" t="n">
         <v>0.545454545454545</v>
@@ -84021,7 +84027,7 @@
     </row>
     <row r="2304">
       <c r="A2304" t="s">
-        <v>894</v>
+        <v>895</v>
       </c>
       <c r="B2304" s="1" t="n">
         <v>45657</v>
@@ -84030,7 +84036,7 @@
         <v>45504</v>
       </c>
       <c r="D2304" t="s">
-        <v>895</v>
+        <v>896</v>
       </c>
       <c r="E2304" t="n">
         <v>0.606060606060606</v>
@@ -84056,7 +84062,7 @@
     </row>
     <row r="2305">
       <c r="A2305" t="s">
-        <v>896</v>
+        <v>897</v>
       </c>
       <c r="B2305" s="1" t="n">
         <v>45657</v>
@@ -84065,7 +84071,7 @@
         <v>45504</v>
       </c>
       <c r="D2305" t="s">
-        <v>897</v>
+        <v>898</v>
       </c>
       <c r="E2305" t="n">
         <v>0.757575757575758</v>
@@ -84091,7 +84097,7 @@
     </row>
     <row r="2306">
       <c r="A2306" t="s">
-        <v>1015</v>
+        <v>1017</v>
       </c>
       <c r="B2306" s="1" t="n">
         <v>45657</v>
@@ -84100,7 +84106,7 @@
         <v>45496</v>
       </c>
       <c r="D2306" t="s">
-        <v>1016</v>
+        <v>1018</v>
       </c>
       <c r="E2306" t="n">
         <v>0.636363636363636</v>
@@ -84126,7 +84132,7 @@
     </row>
     <row r="2307">
       <c r="A2307" t="s">
-        <v>898</v>
+        <v>899</v>
       </c>
       <c r="B2307" s="1" t="n">
         <v>45657</v>
@@ -84135,7 +84141,7 @@
         <v>45504</v>
       </c>
       <c r="D2307" t="s">
-        <v>899</v>
+        <v>900</v>
       </c>
       <c r="E2307" t="n">
         <v>0.696969696969697</v>
@@ -84161,7 +84167,7 @@
     </row>
     <row r="2308">
       <c r="A2308" t="s">
-        <v>1003</v>
+        <v>1005</v>
       </c>
       <c r="B2308" s="1" t="n">
         <v>45657</v>
@@ -84170,7 +84176,7 @@
         <v>45491</v>
       </c>
       <c r="D2308" t="s">
-        <v>1004</v>
+        <v>1006</v>
       </c>
       <c r="E2308" t="n">
         <v>0.575757575757576</v>
@@ -84336,7 +84342,7 @@
     </row>
     <row r="2313">
       <c r="A2313" t="s">
-        <v>900</v>
+        <v>901</v>
       </c>
       <c r="B2313" s="1" t="n">
         <v>45657</v>
@@ -84345,7 +84351,7 @@
         <v>45499</v>
       </c>
       <c r="D2313" t="s">
-        <v>901</v>
+        <v>902</v>
       </c>
       <c r="E2313" t="n">
         <v>0.575757575757576</v>
@@ -84406,7 +84412,7 @@
     </row>
     <row r="2315">
       <c r="A2315" t="s">
-        <v>1017</v>
+        <v>1019</v>
       </c>
       <c r="B2315" s="1" t="n">
         <v>45657</v>
@@ -84415,7 +84421,7 @@
         <v>45371</v>
       </c>
       <c r="D2315" t="s">
-        <v>1018</v>
+        <v>1020</v>
       </c>
       <c r="E2315" t="n">
         <v>0.666666666666667</v>
@@ -84476,7 +84482,7 @@
     </row>
     <row r="2317">
       <c r="A2317" t="s">
-        <v>1019</v>
+        <v>1021</v>
       </c>
       <c r="B2317" s="1" t="n">
         <v>45657</v>
@@ -84485,7 +84491,7 @@
         <v>45587</v>
       </c>
       <c r="D2317" t="s">
-        <v>1020</v>
+        <v>1022</v>
       </c>
       <c r="E2317" t="n">
         <v>0.636363636363636</v>
@@ -84546,7 +84552,7 @@
     </row>
     <row r="2319">
       <c r="A2319" t="s">
-        <v>906</v>
+        <v>907</v>
       </c>
       <c r="B2319" s="1" t="n">
         <v>45657</v>
@@ -84555,7 +84561,7 @@
         <v>45504</v>
       </c>
       <c r="D2319" t="s">
-        <v>907</v>
+        <v>908</v>
       </c>
       <c r="E2319" t="n">
         <v>0.606060606060606</v>
@@ -84581,7 +84587,7 @@
     </row>
     <row r="2320">
       <c r="A2320" t="s">
-        <v>908</v>
+        <v>909</v>
       </c>
       <c r="B2320" s="1" t="n">
         <v>45657</v>
@@ -84590,7 +84596,7 @@
         <v>45504</v>
       </c>
       <c r="D2320" t="s">
-        <v>909</v>
+        <v>910</v>
       </c>
       <c r="E2320" t="n">
         <v>0.606060606060606</v>
@@ -84686,7 +84692,7 @@
     </row>
     <row r="2323">
       <c r="A2323" t="s">
-        <v>981</v>
+        <v>983</v>
       </c>
       <c r="B2323" s="1" t="n">
         <v>45657</v>
@@ -84695,7 +84701,7 @@
         <v>45503</v>
       </c>
       <c r="D2323" t="s">
-        <v>982</v>
+        <v>984</v>
       </c>
       <c r="E2323" t="n">
         <v>0.606060606060606</v>
@@ -84826,7 +84832,7 @@
     </row>
     <row r="2327">
       <c r="A2327" t="s">
-        <v>983</v>
+        <v>985</v>
       </c>
       <c r="B2327" s="1" t="n">
         <v>45657</v>
@@ -84835,7 +84841,7 @@
         <v>45504</v>
       </c>
       <c r="D2327" t="s">
-        <v>984</v>
+        <v>986</v>
       </c>
       <c r="E2327" t="n">
         <v>0.636363636363636</v>
@@ -85211,7 +85217,7 @@
     </row>
     <row r="2338">
       <c r="A2338" t="s">
-        <v>985</v>
+        <v>987</v>
       </c>
       <c r="B2338" s="1" t="n">
         <v>45657</v>
@@ -85220,7 +85226,7 @@
         <v>45488</v>
       </c>
       <c r="D2338" t="s">
-        <v>986</v>
+        <v>988</v>
       </c>
       <c r="E2338" t="n">
         <v>0.606060606060606</v>
@@ -85351,7 +85357,7 @@
     </row>
     <row r="2342">
       <c r="A2342" t="s">
-        <v>987</v>
+        <v>989</v>
       </c>
       <c r="B2342" s="1" t="n">
         <v>45382</v>
@@ -85360,7 +85366,7 @@
         <v>45230</v>
       </c>
       <c r="D2342" t="s">
-        <v>988</v>
+        <v>990</v>
       </c>
       <c r="E2342" t="n">
         <v>0.727272727272727</v>
@@ -85701,7 +85707,7 @@
     </row>
     <row r="2352">
       <c r="A2352" t="s">
-        <v>922</v>
+        <v>923</v>
       </c>
       <c r="B2352" s="1" t="n">
         <v>45657</v>
@@ -85710,7 +85716,7 @@
         <v>45504</v>
       </c>
       <c r="D2352" t="s">
-        <v>923</v>
+        <v>924</v>
       </c>
       <c r="E2352" t="n">
         <v>0.636363636363636</v>
@@ -85736,7 +85742,7 @@
     </row>
     <row r="2353">
       <c r="A2353" t="s">
-        <v>924</v>
+        <v>925</v>
       </c>
       <c r="B2353" s="1" t="n">
         <v>45657</v>
@@ -85745,7 +85751,7 @@
         <v>45504</v>
       </c>
       <c r="D2353" t="s">
-        <v>925</v>
+        <v>926</v>
       </c>
       <c r="E2353" t="n">
         <v>0.515151515151515</v>
@@ -85771,7 +85777,7 @@
     </row>
     <row r="2354">
       <c r="A2354" t="s">
-        <v>926</v>
+        <v>927</v>
       </c>
       <c r="B2354" s="1" t="n">
         <v>45657</v>
@@ -85780,7 +85786,7 @@
         <v>45504</v>
       </c>
       <c r="D2354" t="s">
-        <v>927</v>
+        <v>928</v>
       </c>
       <c r="E2354" t="n">
         <v>0.636363636363636</v>
@@ -85806,7 +85812,7 @@
     </row>
     <row r="2355">
       <c r="A2355" t="s">
-        <v>989</v>
+        <v>991</v>
       </c>
       <c r="B2355" s="1" t="n">
         <v>45657</v>
@@ -85815,7 +85821,7 @@
         <v>45503</v>
       </c>
       <c r="D2355" t="s">
-        <v>990</v>
+        <v>992</v>
       </c>
       <c r="E2355" t="n">
         <v>0.696969696969697</v>
@@ -85841,7 +85847,7 @@
     </row>
     <row r="2356">
       <c r="A2356" t="s">
-        <v>1009</v>
+        <v>1011</v>
       </c>
       <c r="B2356" s="1" t="n">
         <v>45657</v>
@@ -85850,7 +85856,7 @@
         <v>45504</v>
       </c>
       <c r="D2356" t="s">
-        <v>1010</v>
+        <v>1012</v>
       </c>
       <c r="E2356" t="n">
         <v>0.606060606060606</v>
@@ -85911,7 +85917,7 @@
     </row>
     <row r="2358">
       <c r="A2358" t="s">
-        <v>991</v>
+        <v>993</v>
       </c>
       <c r="B2358" s="1" t="n">
         <v>45657</v>
@@ -85920,7 +85926,7 @@
         <v>45502</v>
       </c>
       <c r="D2358" t="s">
-        <v>992</v>
+        <v>994</v>
       </c>
       <c r="E2358" t="n">
         <v>0.515151515151515</v>
@@ -86051,7 +86057,7 @@
     </row>
     <row r="2362">
       <c r="A2362" t="s">
-        <v>993</v>
+        <v>995</v>
       </c>
       <c r="B2362" s="1" t="n">
         <v>45657</v>
@@ -86060,7 +86066,7 @@
         <v>45504</v>
       </c>
       <c r="D2362" t="s">
-        <v>994</v>
+        <v>996</v>
       </c>
       <c r="E2362" t="n">
         <v>0.575757575757576</v>
@@ -86086,7 +86092,7 @@
     </row>
     <row r="2363">
       <c r="A2363" t="s">
-        <v>1011</v>
+        <v>1013</v>
       </c>
       <c r="B2363" s="1" t="n">
         <v>45657</v>
@@ -86095,7 +86101,7 @@
         <v>45503</v>
       </c>
       <c r="D2363" t="s">
-        <v>1012</v>
+        <v>1014</v>
       </c>
       <c r="E2363" t="n">
         <v>0.636363636363636</v>
@@ -86226,7 +86232,7 @@
     </row>
     <row r="2367">
       <c r="A2367" t="s">
-        <v>995</v>
+        <v>997</v>
       </c>
       <c r="B2367" s="1" t="n">
         <v>45657</v>
@@ -86235,7 +86241,7 @@
         <v>45628</v>
       </c>
       <c r="D2367" t="s">
-        <v>996</v>
+        <v>998</v>
       </c>
       <c r="E2367" t="n">
         <v>0.606060606060606</v>
@@ -86296,7 +86302,7 @@
     </row>
     <row r="2369">
       <c r="A2369" t="s">
-        <v>930</v>
+        <v>931</v>
       </c>
       <c r="B2369" s="1" t="n">
         <v>45657</v>
@@ -86305,7 +86311,7 @@
         <v>45503</v>
       </c>
       <c r="D2369" t="s">
-        <v>931</v>
+        <v>932</v>
       </c>
       <c r="E2369" t="n">
         <v>0.606060606060606</v>
@@ -86366,7 +86372,7 @@
     </row>
     <row r="2371">
       <c r="A2371" t="s">
-        <v>1013</v>
+        <v>1015</v>
       </c>
       <c r="B2371" s="1" t="n">
         <v>45657</v>
@@ -86375,7 +86381,7 @@
         <v>45503</v>
       </c>
       <c r="D2371" t="s">
-        <v>1014</v>
+        <v>1016</v>
       </c>
       <c r="E2371" t="n">
         <v>0.696969696969697</v>
@@ -86585,7 +86591,7 @@
         <v>45499</v>
       </c>
       <c r="D2377" t="s">
-        <v>932</v>
+        <v>933</v>
       </c>
       <c r="E2377" t="n">
         <v>0.575757575757576</v>
@@ -87031,7 +87037,7 @@
     </row>
     <row r="2390">
       <c r="A2390" t="s">
-        <v>933</v>
+        <v>934</v>
       </c>
       <c r="B2390" s="1" t="n">
         <v>45657</v>
@@ -87040,7 +87046,7 @@
         <v>45503</v>
       </c>
       <c r="D2390" t="s">
-        <v>934</v>
+        <v>935</v>
       </c>
       <c r="E2390" t="n">
         <v>0.606060606060606</v>
@@ -87101,7 +87107,7 @@
     </row>
     <row r="2392">
       <c r="A2392" t="s">
-        <v>937</v>
+        <v>938</v>
       </c>
       <c r="B2392" s="1" t="n">
         <v>45657</v>
@@ -87110,7 +87116,7 @@
         <v>45503</v>
       </c>
       <c r="D2392" t="s">
-        <v>938</v>
+        <v>939</v>
       </c>
       <c r="E2392" t="n">
         <v>0.666666666666667</v>
@@ -87180,7 +87186,7 @@
         <v>45499</v>
       </c>
       <c r="D2394" t="s">
-        <v>600</v>
+        <v>940</v>
       </c>
       <c r="E2394" t="n">
         <v>0.666666666666667</v>
@@ -87801,7 +87807,7 @@
     </row>
     <row r="2412">
       <c r="A2412" t="s">
-        <v>939</v>
+        <v>941</v>
       </c>
       <c r="B2412" s="1" t="n">
         <v>45657</v>
@@ -87810,7 +87816,7 @@
         <v>45504</v>
       </c>
       <c r="D2412" t="s">
-        <v>940</v>
+        <v>942</v>
       </c>
       <c r="E2412" t="n">
         <v>0.606060606060606</v>
@@ -87976,7 +87982,7 @@
     </row>
     <row r="2417">
       <c r="A2417" t="s">
-        <v>943</v>
+        <v>945</v>
       </c>
       <c r="B2417" s="1" t="n">
         <v>45657</v>
@@ -87985,7 +87991,7 @@
         <v>45504</v>
       </c>
       <c r="D2417" t="s">
-        <v>944</v>
+        <v>946</v>
       </c>
       <c r="E2417" t="n">
         <v>0.575757575757576</v>
@@ -88151,7 +88157,7 @@
     </row>
     <row r="2422">
       <c r="A2422" t="s">
-        <v>999</v>
+        <v>1001</v>
       </c>
       <c r="B2422" s="1" t="n">
         <v>45473</v>
@@ -88160,7 +88166,7 @@
         <v>45322</v>
       </c>
       <c r="D2422" t="s">
-        <v>1000</v>
+        <v>1002</v>
       </c>
       <c r="E2422" t="n">
         <v>0.575757575757576</v>
@@ -88256,7 +88262,7 @@
     </row>
     <row r="2425">
       <c r="A2425" t="s">
-        <v>945</v>
+        <v>947</v>
       </c>
       <c r="B2425" s="1" t="n">
         <v>45657</v>
@@ -88265,7 +88271,7 @@
         <v>45503</v>
       </c>
       <c r="D2425" t="s">
-        <v>946</v>
+        <v>948</v>
       </c>
       <c r="E2425" t="n">
         <v>0.696969696969697</v>
@@ -88536,7 +88542,7 @@
     </row>
     <row r="2433">
       <c r="A2433" t="s">
-        <v>947</v>
+        <v>949</v>
       </c>
       <c r="B2433" s="1" t="n">
         <v>45657</v>
@@ -88545,7 +88551,7 @@
         <v>45504</v>
       </c>
       <c r="D2433" t="s">
-        <v>948</v>
+        <v>950</v>
       </c>
       <c r="E2433" t="n">
         <v>0.696969696969697</v>
@@ -89516,7 +89522,7 @@
     </row>
     <row r="2461">
       <c r="A2461" t="s">
-        <v>949</v>
+        <v>951</v>
       </c>
       <c r="B2461" s="1" t="n">
         <v>45657</v>
@@ -89525,7 +89531,7 @@
         <v>45504</v>
       </c>
       <c r="D2461" t="s">
-        <v>950</v>
+        <v>952</v>
       </c>
       <c r="E2461" t="n">
         <v>0.696969696969697</v>
@@ -89586,7 +89592,7 @@
     </row>
     <row r="2463">
       <c r="A2463" t="s">
-        <v>951</v>
+        <v>953</v>
       </c>
       <c r="B2463" s="1" t="n">
         <v>45657</v>
@@ -89595,7 +89601,7 @@
         <v>45504</v>
       </c>
       <c r="D2463" t="s">
-        <v>952</v>
+        <v>954</v>
       </c>
       <c r="E2463" t="n">
         <v>0.575757575757576</v>

</xml_diff>

<commit_message>
Atualização de dados automática em 2025-05-13 12:30:02 (cron)
</commit_message>
<xml_diff>
--- a/public/docs/index_07_dim_CG.xlsx
+++ b/public/docs/index_07_dim_CG.xlsx
@@ -2594,7 +2594,7 @@
     <t xml:space="preserve">10.739.356/0001-03</t>
   </si>
   <si>
-    <t xml:space="preserve">BR ADVISORY PARTNERS PARTICIPAÇÕES S.A.</t>
+    <t xml:space="preserve">BRBI BR PARTNERS S.A</t>
   </si>
   <si>
     <t xml:space="preserve">10.807.374/0001-77</t>
@@ -3044,7 +3044,7 @@
     <t xml:space="preserve">23.438.929/0001-00</t>
   </si>
   <si>
-    <t xml:space="preserve">TRIPLE PLAY BRASIL PARTICIPAÇÕES S.A.</t>
+    <t xml:space="preserve">ALARES INTERNET PARTICIPAÇÕES S/A</t>
   </si>
   <si>
     <t xml:space="preserve">39.881.421/0001-04</t>

</xml_diff>

<commit_message>
Atualização de dados automática em 2025-06-10 12:30:02 (cron)
</commit_message>
<xml_diff>
--- a/public/docs/index_07_dim_CG.xlsx
+++ b/public/docs/index_07_dim_CG.xlsx
@@ -89712,141 +89712,246 @@
     </row>
     <row r="2466">
       <c r="A2466" t="s">
-        <v>486</v>
+        <v>289</v>
       </c>
       <c r="B2466" s="1" t="n">
         <v>46022</v>
       </c>
       <c r="C2466" s="1" t="n">
-        <v>45796</v>
+        <v>45813</v>
       </c>
       <c r="D2466" t="s">
-        <v>792</v>
+        <v>290</v>
       </c>
       <c r="E2466" t="n">
-        <v>0.636363636363636</v>
+        <v>0.515151515151515</v>
       </c>
       <c r="F2466" t="n">
-        <v>0.666666666666667</v>
+        <v>0.606060606060606</v>
       </c>
       <c r="G2466" t="n">
-        <v>0.75</v>
+        <v>0.458333333333333</v>
       </c>
       <c r="H2466" t="n">
-        <v>0.571428571428571</v>
+        <v>0.428571428571429</v>
       </c>
       <c r="I2466" t="n">
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
       <c r="J2466" t="n">
-        <v>0.2</v>
+        <v>0.333333333333333</v>
       </c>
       <c r="K2466" t="n">
-        <v>0.666666666666667</v>
+        <v>0.285714285714286</v>
       </c>
     </row>
     <row r="2467">
       <c r="A2467" t="s">
-        <v>631</v>
+        <v>486</v>
       </c>
       <c r="B2467" s="1" t="n">
         <v>46022</v>
       </c>
       <c r="C2467" s="1" t="n">
-        <v>45754</v>
+        <v>45796</v>
       </c>
       <c r="D2467" t="s">
-        <v>944</v>
+        <v>792</v>
       </c>
       <c r="E2467" t="n">
-        <v>0.454545454545455</v>
+        <v>0.636363636363636</v>
       </c>
       <c r="F2467" t="n">
-        <v>0.606060606060606</v>
+        <v>0.666666666666667</v>
       </c>
       <c r="G2467" t="n">
-        <v>0.625</v>
+        <v>0.75</v>
       </c>
       <c r="H2467" t="n">
         <v>0.571428571428571</v>
       </c>
       <c r="I2467" t="n">
-        <v>0.133333333333333</v>
+        <v>0.2</v>
       </c>
       <c r="J2467" t="n">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="K2467" t="n">
-        <v>0.285714285714286</v>
+        <v>0.666666666666667</v>
       </c>
     </row>
     <row r="2468">
       <c r="A2468" t="s">
-        <v>810</v>
+        <v>547</v>
       </c>
       <c r="B2468" s="1" t="n">
-        <v>45716</v>
+        <v>46022</v>
       </c>
       <c r="C2468" s="1" t="n">
-        <v>45565</v>
+        <v>45814</v>
       </c>
       <c r="D2468" t="s">
-        <v>811</v>
+        <v>548</v>
       </c>
       <c r="E2468" t="n">
-        <v>0.666666666666667</v>
+        <v>0.575757575757576</v>
       </c>
       <c r="F2468" t="n">
-        <v>0.696969696969697</v>
+        <v>0.818181818181818</v>
       </c>
       <c r="G2468" t="n">
-        <v>0.583333333333333</v>
+        <v>0.416666666666667</v>
       </c>
       <c r="H2468" t="n">
-        <v>0.571428571428571</v>
+        <v>0.619047619047619</v>
       </c>
       <c r="I2468" t="n">
-        <v>0.266666666666667</v>
+        <v>0.533333333333333</v>
       </c>
       <c r="J2468" t="n">
-        <v>0</v>
+        <v>0.0666666666666667</v>
       </c>
       <c r="K2468" t="n">
-        <v>0.571428571428571</v>
+        <v>0.428571428571429</v>
       </c>
     </row>
     <row r="2469">
       <c r="A2469" t="s">
-        <v>812</v>
+        <v>627</v>
       </c>
       <c r="B2469" s="1" t="n">
-        <v>45838</v>
+        <v>46022</v>
       </c>
       <c r="C2469" s="1" t="n">
-        <v>45681</v>
+        <v>45810</v>
       </c>
       <c r="D2469" t="s">
-        <v>813</v>
+        <v>628</v>
       </c>
       <c r="E2469" t="n">
-        <v>0.454545454545455</v>
+        <v>0.636363636363636</v>
       </c>
       <c r="F2469" t="n">
-        <v>0.575757575757576</v>
+        <v>0.757575757575758</v>
       </c>
       <c r="G2469" t="n">
         <v>0.541666666666667</v>
       </c>
       <c r="H2469" t="n">
-        <v>0.571428571428571</v>
+        <v>0.333333333333333</v>
       </c>
       <c r="I2469" t="n">
+        <v>0.133333333333333</v>
+      </c>
+      <c r="J2469" t="n">
+        <v>0</v>
+      </c>
+      <c r="K2469" t="n">
+        <v>0.571428571428571</v>
+      </c>
+    </row>
+    <row r="2470">
+      <c r="A2470" t="s">
+        <v>631</v>
+      </c>
+      <c r="B2470" s="1" t="n">
+        <v>46022</v>
+      </c>
+      <c r="C2470" s="1" t="n">
+        <v>45811</v>
+      </c>
+      <c r="D2470" t="s">
+        <v>944</v>
+      </c>
+      <c r="E2470" t="n">
+        <v>0.454545454545455</v>
+      </c>
+      <c r="F2470" t="n">
+        <v>0.606060606060606</v>
+      </c>
+      <c r="G2470" t="n">
+        <v>0.625</v>
+      </c>
+      <c r="H2470" t="n">
+        <v>0.571428571428571</v>
+      </c>
+      <c r="I2470" t="n">
+        <v>0.133333333333333</v>
+      </c>
+      <c r="J2470" t="n">
+        <v>0</v>
+      </c>
+      <c r="K2470" t="n">
+        <v>0.285714285714286</v>
+      </c>
+    </row>
+    <row r="2471">
+      <c r="A2471" t="s">
+        <v>810</v>
+      </c>
+      <c r="B2471" s="1" t="n">
+        <v>45716</v>
+      </c>
+      <c r="C2471" s="1" t="n">
+        <v>45565</v>
+      </c>
+      <c r="D2471" t="s">
+        <v>811</v>
+      </c>
+      <c r="E2471" t="n">
+        <v>0.666666666666667</v>
+      </c>
+      <c r="F2471" t="n">
+        <v>0.696969696969697</v>
+      </c>
+      <c r="G2471" t="n">
+        <v>0.583333333333333</v>
+      </c>
+      <c r="H2471" t="n">
+        <v>0.571428571428571</v>
+      </c>
+      <c r="I2471" t="n">
+        <v>0.266666666666667</v>
+      </c>
+      <c r="J2471" t="n">
+        <v>0</v>
+      </c>
+      <c r="K2471" t="n">
+        <v>0.571428571428571</v>
+      </c>
+    </row>
+    <row r="2472">
+      <c r="A2472" t="s">
+        <v>812</v>
+      </c>
+      <c r="B2472" s="1" t="n">
+        <v>45838</v>
+      </c>
+      <c r="C2472" s="1" t="n">
+        <v>45681</v>
+      </c>
+      <c r="D2472" t="s">
+        <v>813</v>
+      </c>
+      <c r="E2472" t="n">
+        <v>0.454545454545455</v>
+      </c>
+      <c r="F2472" t="n">
+        <v>0.575757575757576</v>
+      </c>
+      <c r="G2472" t="n">
+        <v>0.541666666666667</v>
+      </c>
+      <c r="H2472" t="n">
+        <v>0.571428571428571</v>
+      </c>
+      <c r="I2472" t="n">
         <v>0.333333333333333</v>
       </c>
-      <c r="J2469" t="n">
-        <v>0.133333333333333</v>
-      </c>
-      <c r="K2469" t="n">
+      <c r="J2472" t="n">
+        <v>0.133333333333333</v>
+      </c>
+      <c r="K2472" t="n">
         <v>0.619047619047619</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualização de dados automática em 2025-07-07 14:09:36 (cron)
</commit_message>
<xml_diff>
--- a/public/docs/index_07_dim_CG.xlsx
+++ b/public/docs/index_07_dim_CG.xlsx
@@ -89747,101 +89747,101 @@
     </row>
     <row r="2467">
       <c r="A2467" t="s">
-        <v>486</v>
+        <v>39</v>
       </c>
       <c r="B2467" s="1" t="n">
         <v>46022</v>
       </c>
       <c r="C2467" s="1" t="n">
-        <v>45796</v>
+        <v>45842</v>
       </c>
       <c r="D2467" t="s">
-        <v>792</v>
+        <v>40</v>
       </c>
       <c r="E2467" t="n">
-        <v>0.636363636363636</v>
+        <v>0.666666666666667</v>
       </c>
       <c r="F2467" t="n">
         <v>0.666666666666667</v>
       </c>
       <c r="G2467" t="n">
-        <v>0.75</v>
+        <v>0.5</v>
       </c>
       <c r="H2467" t="n">
-        <v>0.571428571428571</v>
+        <v>0.523809523809524</v>
       </c>
       <c r="I2467" t="n">
-        <v>0.2</v>
+        <v>0.266666666666667</v>
       </c>
       <c r="J2467" t="n">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="K2467" t="n">
-        <v>0.666666666666667</v>
+        <v>0.571428571428571</v>
       </c>
     </row>
     <row r="2468">
       <c r="A2468" t="s">
-        <v>547</v>
+        <v>831</v>
       </c>
       <c r="B2468" s="1" t="n">
         <v>46022</v>
       </c>
       <c r="C2468" s="1" t="n">
-        <v>45814</v>
+        <v>45841</v>
       </c>
       <c r="D2468" t="s">
-        <v>548</v>
+        <v>832</v>
       </c>
       <c r="E2468" t="n">
-        <v>0.575757575757576</v>
+        <v>0.606060606060606</v>
       </c>
       <c r="F2468" t="n">
-        <v>0.818181818181818</v>
+        <v>0.636363636363636</v>
       </c>
       <c r="G2468" t="n">
-        <v>0.416666666666667</v>
+        <v>0.458333333333333</v>
       </c>
       <c r="H2468" t="n">
-        <v>0.619047619047619</v>
+        <v>0.571428571428571</v>
       </c>
       <c r="I2468" t="n">
-        <v>0.533333333333333</v>
+        <v>0.2</v>
       </c>
       <c r="J2468" t="n">
-        <v>0.0666666666666667</v>
+        <v>0.6</v>
       </c>
       <c r="K2468" t="n">
-        <v>0.428571428571429</v>
+        <v>0.333333333333333</v>
       </c>
     </row>
     <row r="2469">
       <c r="A2469" t="s">
-        <v>627</v>
+        <v>401</v>
       </c>
       <c r="B2469" s="1" t="n">
         <v>46022</v>
       </c>
       <c r="C2469" s="1" t="n">
-        <v>45810</v>
+        <v>45839</v>
       </c>
       <c r="D2469" t="s">
-        <v>628</v>
+        <v>402</v>
       </c>
       <c r="E2469" t="n">
-        <v>0.636363636363636</v>
+        <v>0.575757575757576</v>
       </c>
       <c r="F2469" t="n">
-        <v>0.757575757575758</v>
+        <v>0.727272727272727</v>
       </c>
       <c r="G2469" t="n">
         <v>0.541666666666667</v>
       </c>
       <c r="H2469" t="n">
-        <v>0.333333333333333</v>
+        <v>0.571428571428571</v>
       </c>
       <c r="I2469" t="n">
-        <v>0.133333333333333</v>
+        <v>0.8</v>
       </c>
       <c r="J2469" t="n">
         <v>0</v>
@@ -89852,107 +89852,737 @@
     </row>
     <row r="2470">
       <c r="A2470" t="s">
-        <v>631</v>
+        <v>860</v>
       </c>
       <c r="B2470" s="1" t="n">
         <v>46022</v>
       </c>
       <c r="C2470" s="1" t="n">
-        <v>45811</v>
+        <v>45831</v>
       </c>
       <c r="D2470" t="s">
-        <v>944</v>
+        <v>861</v>
       </c>
       <c r="E2470" t="n">
-        <v>0.454545454545455</v>
+        <v>0.666666666666667</v>
       </c>
       <c r="F2470" t="n">
         <v>0.606060606060606</v>
       </c>
       <c r="G2470" t="n">
-        <v>0.625</v>
+        <v>0.5</v>
       </c>
       <c r="H2470" t="n">
-        <v>0.571428571428571</v>
+        <v>0.523809523809524</v>
       </c>
       <c r="I2470" t="n">
         <v>0.133333333333333</v>
       </c>
       <c r="J2470" t="n">
-        <v>0</v>
+        <v>0.466666666666667</v>
       </c>
       <c r="K2470" t="n">
-        <v>0.285714285714286</v>
+        <v>0.428571428571429</v>
       </c>
     </row>
     <row r="2471">
       <c r="A2471" t="s">
-        <v>810</v>
+        <v>978</v>
       </c>
       <c r="B2471" s="1" t="n">
-        <v>45716</v>
+        <v>46022</v>
       </c>
       <c r="C2471" s="1" t="n">
-        <v>45565</v>
+        <v>45838</v>
       </c>
       <c r="D2471" t="s">
-        <v>811</v>
+        <v>979</v>
       </c>
       <c r="E2471" t="n">
-        <v>0.666666666666667</v>
+        <v>0.454545454545455</v>
       </c>
       <c r="F2471" t="n">
-        <v>0.696969696969697</v>
+        <v>0.606060606060606</v>
       </c>
       <c r="G2471" t="n">
-        <v>0.583333333333333</v>
+        <v>0.458333333333333</v>
       </c>
       <c r="H2471" t="n">
         <v>0.571428571428571</v>
       </c>
       <c r="I2471" t="n">
-        <v>0.266666666666667</v>
+        <v>0.2</v>
       </c>
       <c r="J2471" t="n">
-        <v>0</v>
+        <v>0.533333333333333</v>
       </c>
       <c r="K2471" t="n">
-        <v>0.571428571428571</v>
+        <v>0.333333333333333</v>
       </c>
     </row>
     <row r="2472">
       <c r="A2472" t="s">
+        <v>119</v>
+      </c>
+      <c r="B2472" s="1" t="n">
+        <v>46022</v>
+      </c>
+      <c r="C2472" s="1" t="n">
+        <v>45834</v>
+      </c>
+      <c r="D2472" t="s">
+        <v>120</v>
+      </c>
+      <c r="E2472" t="n">
+        <v>0.606060606060606</v>
+      </c>
+      <c r="F2472" t="n">
+        <v>0.636363636363636</v>
+      </c>
+      <c r="G2472" t="n">
+        <v>0.625</v>
+      </c>
+      <c r="H2472" t="n">
+        <v>0.571428571428571</v>
+      </c>
+      <c r="I2472" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="J2472" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="K2472" t="n">
+        <v>0.571428571428571</v>
+      </c>
+    </row>
+    <row r="2473">
+      <c r="A2473" t="s">
+        <v>121</v>
+      </c>
+      <c r="B2473" s="1" t="n">
+        <v>46022</v>
+      </c>
+      <c r="C2473" s="1" t="n">
+        <v>45841</v>
+      </c>
+      <c r="D2473" t="s">
+        <v>122</v>
+      </c>
+      <c r="E2473" t="n">
+        <v>0.545454545454545</v>
+      </c>
+      <c r="F2473" t="n">
+        <v>0.515151515151515</v>
+      </c>
+      <c r="G2473" t="n">
+        <v>0.541666666666667</v>
+      </c>
+      <c r="H2473" t="n">
+        <v>0.571428571428571</v>
+      </c>
+      <c r="I2473" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="J2473" t="n">
+        <v>0</v>
+      </c>
+      <c r="K2473" t="n">
+        <v>0.571428571428571</v>
+      </c>
+    </row>
+    <row r="2474">
+      <c r="A2474" t="s">
+        <v>486</v>
+      </c>
+      <c r="B2474" s="1" t="n">
+        <v>46022</v>
+      </c>
+      <c r="C2474" s="1" t="n">
+        <v>45796</v>
+      </c>
+      <c r="D2474" t="s">
+        <v>792</v>
+      </c>
+      <c r="E2474" t="n">
+        <v>0.636363636363636</v>
+      </c>
+      <c r="F2474" t="n">
+        <v>0.666666666666667</v>
+      </c>
+      <c r="G2474" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="H2474" t="n">
+        <v>0.571428571428571</v>
+      </c>
+      <c r="I2474" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="J2474" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="K2474" t="n">
+        <v>0.666666666666667</v>
+      </c>
+    </row>
+    <row r="2475">
+      <c r="A2475" t="s">
+        <v>147</v>
+      </c>
+      <c r="B2475" s="1" t="n">
+        <v>46022</v>
+      </c>
+      <c r="C2475" s="1" t="n">
+        <v>45842</v>
+      </c>
+      <c r="D2475" t="s">
+        <v>148</v>
+      </c>
+      <c r="E2475" t="n">
+        <v>0.636363636363636</v>
+      </c>
+      <c r="F2475" t="n">
+        <v>0.666666666666667</v>
+      </c>
+      <c r="G2475" t="n">
+        <v>0.541666666666667</v>
+      </c>
+      <c r="H2475" t="n">
+        <v>0.571428571428571</v>
+      </c>
+      <c r="I2475" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="J2475" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="K2475" t="n">
+        <v>0.571428571428571</v>
+      </c>
+    </row>
+    <row r="2476">
+      <c r="A2476" t="s">
+        <v>547</v>
+      </c>
+      <c r="B2476" s="1" t="n">
+        <v>46022</v>
+      </c>
+      <c r="C2476" s="1" t="n">
+        <v>45814</v>
+      </c>
+      <c r="D2476" t="s">
+        <v>548</v>
+      </c>
+      <c r="E2476" t="n">
+        <v>0.575757575757576</v>
+      </c>
+      <c r="F2476" t="n">
+        <v>0.818181818181818</v>
+      </c>
+      <c r="G2476" t="n">
+        <v>0.416666666666667</v>
+      </c>
+      <c r="H2476" t="n">
+        <v>0.619047619047619</v>
+      </c>
+      <c r="I2476" t="n">
+        <v>0.533333333333333</v>
+      </c>
+      <c r="J2476" t="n">
+        <v>0.0666666666666667</v>
+      </c>
+      <c r="K2476" t="n">
+        <v>0.428571428571429</v>
+      </c>
+    </row>
+    <row r="2477">
+      <c r="A2477" t="s">
+        <v>563</v>
+      </c>
+      <c r="B2477" s="1" t="n">
+        <v>46022</v>
+      </c>
+      <c r="C2477" s="1" t="n">
+        <v>45835</v>
+      </c>
+      <c r="D2477" t="s">
+        <v>564</v>
+      </c>
+      <c r="E2477" t="n">
+        <v>0.484848484848485</v>
+      </c>
+      <c r="F2477" t="n">
+        <v>0.636363636363636</v>
+      </c>
+      <c r="G2477" t="n">
+        <v>0.625</v>
+      </c>
+      <c r="H2477" t="n">
+        <v>0.571428571428571</v>
+      </c>
+      <c r="I2477" t="n">
+        <v>0.533333333333333</v>
+      </c>
+      <c r="J2477" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="K2477" t="n">
+        <v>0.571428571428571</v>
+      </c>
+    </row>
+    <row r="2478">
+      <c r="A2478" t="s">
+        <v>583</v>
+      </c>
+      <c r="B2478" s="1" t="n">
+        <v>46022</v>
+      </c>
+      <c r="C2478" s="1" t="n">
+        <v>45841</v>
+      </c>
+      <c r="D2478" t="s">
+        <v>584</v>
+      </c>
+      <c r="E2478" t="n">
+        <v>0.545454545454545</v>
+      </c>
+      <c r="F2478" t="n">
+        <v>0.545454545454545</v>
+      </c>
+      <c r="G2478" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="H2478" t="n">
+        <v>0.476190476190476</v>
+      </c>
+      <c r="I2478" t="n">
+        <v>0.333333333333333</v>
+      </c>
+      <c r="J2478" t="n">
+        <v>0.266666666666667</v>
+      </c>
+      <c r="K2478" t="n">
+        <v>0.666666666666667</v>
+      </c>
+    </row>
+    <row r="2479">
+      <c r="A2479" t="s">
+        <v>193</v>
+      </c>
+      <c r="B2479" s="1" t="n">
+        <v>46022</v>
+      </c>
+      <c r="C2479" s="1" t="n">
+        <v>45841</v>
+      </c>
+      <c r="D2479" t="s">
+        <v>194</v>
+      </c>
+      <c r="E2479" t="n">
+        <v>0.636363636363636</v>
+      </c>
+      <c r="F2479" t="n">
+        <v>0.666666666666667</v>
+      </c>
+      <c r="G2479" t="n">
+        <v>0.625</v>
+      </c>
+      <c r="H2479" t="n">
+        <v>0.571428571428571</v>
+      </c>
+      <c r="I2479" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="J2479" t="n">
+        <v>0</v>
+      </c>
+      <c r="K2479" t="n">
+        <v>0.571428571428571</v>
+      </c>
+    </row>
+    <row r="2480">
+      <c r="A2480" t="s">
+        <v>617</v>
+      </c>
+      <c r="B2480" s="1" t="n">
+        <v>46022</v>
+      </c>
+      <c r="C2480" s="1" t="n">
+        <v>45835</v>
+      </c>
+      <c r="D2480" t="s">
+        <v>618</v>
+      </c>
+      <c r="E2480" t="n">
+        <v>0.636363636363636</v>
+      </c>
+      <c r="F2480" t="n">
+        <v>0.454545454545455</v>
+      </c>
+      <c r="G2480" t="n">
+        <v>0.416666666666667</v>
+      </c>
+      <c r="H2480" t="n">
+        <v>0.666666666666667</v>
+      </c>
+      <c r="I2480" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="J2480" t="n">
+        <v>0</v>
+      </c>
+      <c r="K2480" t="n">
+        <v>0.761904761904762</v>
+      </c>
+    </row>
+    <row r="2481">
+      <c r="A2481" t="s">
+        <v>627</v>
+      </c>
+      <c r="B2481" s="1" t="n">
+        <v>46022</v>
+      </c>
+      <c r="C2481" s="1" t="n">
+        <v>45810</v>
+      </c>
+      <c r="D2481" t="s">
+        <v>628</v>
+      </c>
+      <c r="E2481" t="n">
+        <v>0.636363636363636</v>
+      </c>
+      <c r="F2481" t="n">
+        <v>0.757575757575758</v>
+      </c>
+      <c r="G2481" t="n">
+        <v>0.541666666666667</v>
+      </c>
+      <c r="H2481" t="n">
+        <v>0.333333333333333</v>
+      </c>
+      <c r="I2481" t="n">
+        <v>0.133333333333333</v>
+      </c>
+      <c r="J2481" t="n">
+        <v>0</v>
+      </c>
+      <c r="K2481" t="n">
+        <v>0.571428571428571</v>
+      </c>
+    </row>
+    <row r="2482">
+      <c r="A2482" t="s">
+        <v>631</v>
+      </c>
+      <c r="B2482" s="1" t="n">
+        <v>46022</v>
+      </c>
+      <c r="C2482" s="1" t="n">
+        <v>45811</v>
+      </c>
+      <c r="D2482" t="s">
+        <v>944</v>
+      </c>
+      <c r="E2482" t="n">
+        <v>0.454545454545455</v>
+      </c>
+      <c r="F2482" t="n">
+        <v>0.606060606060606</v>
+      </c>
+      <c r="G2482" t="n">
+        <v>0.625</v>
+      </c>
+      <c r="H2482" t="n">
+        <v>0.571428571428571</v>
+      </c>
+      <c r="I2482" t="n">
+        <v>0.133333333333333</v>
+      </c>
+      <c r="J2482" t="n">
+        <v>0</v>
+      </c>
+      <c r="K2482" t="n">
+        <v>0.285714285714286</v>
+      </c>
+    </row>
+    <row r="2483">
+      <c r="A2483" t="s">
+        <v>647</v>
+      </c>
+      <c r="B2483" s="1" t="n">
+        <v>46022</v>
+      </c>
+      <c r="C2483" s="1" t="n">
+        <v>45831</v>
+      </c>
+      <c r="D2483" t="s">
+        <v>648</v>
+      </c>
+      <c r="E2483" t="n">
+        <v>0.575757575757576</v>
+      </c>
+      <c r="F2483" t="n">
+        <v>0.545454545454545</v>
+      </c>
+      <c r="G2483" t="n">
+        <v>0.416666666666667</v>
+      </c>
+      <c r="H2483" t="n">
+        <v>0.476190476190476</v>
+      </c>
+      <c r="I2483" t="n">
+        <v>0.466666666666667</v>
+      </c>
+      <c r="J2483" t="n">
+        <v>0.133333333333333</v>
+      </c>
+      <c r="K2483" t="n">
+        <v>0.523809523809524</v>
+      </c>
+    </row>
+    <row r="2484">
+      <c r="A2484" t="s">
+        <v>810</v>
+      </c>
+      <c r="B2484" s="1" t="n">
+        <v>45716</v>
+      </c>
+      <c r="C2484" s="1" t="n">
+        <v>45565</v>
+      </c>
+      <c r="D2484" t="s">
+        <v>811</v>
+      </c>
+      <c r="E2484" t="n">
+        <v>0.666666666666667</v>
+      </c>
+      <c r="F2484" t="n">
+        <v>0.696969696969697</v>
+      </c>
+      <c r="G2484" t="n">
+        <v>0.583333333333333</v>
+      </c>
+      <c r="H2484" t="n">
+        <v>0.571428571428571</v>
+      </c>
+      <c r="I2484" t="n">
+        <v>0.266666666666667</v>
+      </c>
+      <c r="J2484" t="n">
+        <v>0</v>
+      </c>
+      <c r="K2484" t="n">
+        <v>0.571428571428571</v>
+      </c>
+    </row>
+    <row r="2485">
+      <c r="A2485" t="s">
+        <v>667</v>
+      </c>
+      <c r="B2485" s="1" t="n">
+        <v>46022</v>
+      </c>
+      <c r="C2485" s="1" t="n">
+        <v>45832</v>
+      </c>
+      <c r="D2485" t="s">
+        <v>668</v>
+      </c>
+      <c r="E2485" t="n">
+        <v>0.727272727272727</v>
+      </c>
+      <c r="F2485" t="n">
+        <v>0.636363636363636</v>
+      </c>
+      <c r="G2485" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="H2485" t="n">
+        <v>0.571428571428571</v>
+      </c>
+      <c r="I2485" t="n">
+        <v>0.533333333333333</v>
+      </c>
+      <c r="J2485" t="n">
+        <v>0</v>
+      </c>
+      <c r="K2485" t="n">
+        <v>0.571428571428571</v>
+      </c>
+    </row>
+    <row r="2486">
+      <c r="A2486" t="s">
+        <v>675</v>
+      </c>
+      <c r="B2486" s="1" t="n">
+        <v>46022</v>
+      </c>
+      <c r="C2486" s="1" t="n">
+        <v>45825</v>
+      </c>
+      <c r="D2486" t="s">
+        <v>676</v>
+      </c>
+      <c r="E2486" t="n">
+        <v>0.484848484848485</v>
+      </c>
+      <c r="F2486" t="n">
+        <v>0.484848484848485</v>
+      </c>
+      <c r="G2486" t="n">
+        <v>0.458333333333333</v>
+      </c>
+      <c r="H2486" t="n">
+        <v>0.476190476190476</v>
+      </c>
+      <c r="I2486" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="J2486" t="n">
+        <v>0.133333333333333</v>
+      </c>
+      <c r="K2486" t="n">
+        <v>0.523809523809524</v>
+      </c>
+    </row>
+    <row r="2487">
+      <c r="A2487" t="s">
+        <v>679</v>
+      </c>
+      <c r="B2487" s="1" t="n">
+        <v>46022</v>
+      </c>
+      <c r="C2487" s="1" t="n">
+        <v>45840</v>
+      </c>
+      <c r="D2487" t="s">
+        <v>680</v>
+      </c>
+      <c r="E2487" t="n">
+        <v>0.636363636363636</v>
+      </c>
+      <c r="F2487" t="n">
+        <v>0.636363636363636</v>
+      </c>
+      <c r="G2487" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="H2487" t="n">
+        <v>0.571428571428571</v>
+      </c>
+      <c r="I2487" t="n">
+        <v>0.666666666666667</v>
+      </c>
+      <c r="J2487" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="K2487" t="n">
+        <v>0.619047619047619</v>
+      </c>
+    </row>
+    <row r="2488">
+      <c r="A2488" t="s">
         <v>812</v>
       </c>
-      <c r="B2472" s="1" t="n">
+      <c r="B2488" s="1" t="n">
         <v>45838</v>
       </c>
-      <c r="C2472" s="1" t="n">
+      <c r="C2488" s="1" t="n">
         <v>45681</v>
       </c>
-      <c r="D2472" t="s">
+      <c r="D2488" t="s">
         <v>813</v>
       </c>
-      <c r="E2472" t="n">
+      <c r="E2488" t="n">
         <v>0.454545454545455</v>
       </c>
-      <c r="F2472" t="n">
+      <c r="F2488" t="n">
         <v>0.575757575757576</v>
       </c>
-      <c r="G2472" t="n">
+      <c r="G2488" t="n">
         <v>0.541666666666667</v>
       </c>
-      <c r="H2472" t="n">
-        <v>0.571428571428571</v>
-      </c>
-      <c r="I2472" t="n">
+      <c r="H2488" t="n">
+        <v>0.571428571428571</v>
+      </c>
+      <c r="I2488" t="n">
         <v>0.333333333333333</v>
       </c>
-      <c r="J2472" t="n">
-        <v>0.133333333333333</v>
-      </c>
-      <c r="K2472" t="n">
+      <c r="J2488" t="n">
+        <v>0.133333333333333</v>
+      </c>
+      <c r="K2488" t="n">
         <v>0.619047619047619</v>
+      </c>
+    </row>
+    <row r="2489">
+      <c r="A2489" t="s">
+        <v>721</v>
+      </c>
+      <c r="B2489" s="1" t="n">
+        <v>46022</v>
+      </c>
+      <c r="C2489" s="1" t="n">
+        <v>45834</v>
+      </c>
+      <c r="D2489" t="s">
+        <v>722</v>
+      </c>
+      <c r="E2489" t="n">
+        <v>0.484848484848485</v>
+      </c>
+      <c r="F2489" t="n">
+        <v>0.515151515151515</v>
+      </c>
+      <c r="G2489" t="n">
+        <v>0.458333333333333</v>
+      </c>
+      <c r="H2489" t="n">
+        <v>0.476190476190476</v>
+      </c>
+      <c r="I2489" t="n">
+        <v>0.133333333333333</v>
+      </c>
+      <c r="J2489" t="n">
+        <v>0.133333333333333</v>
+      </c>
+      <c r="K2489" t="n">
+        <v>0.666666666666667</v>
+      </c>
+    </row>
+    <row r="2490">
+      <c r="A2490" t="s">
+        <v>815</v>
+      </c>
+      <c r="B2490" s="1" t="n">
+        <v>46022</v>
+      </c>
+      <c r="C2490" s="1" t="n">
+        <v>45838</v>
+      </c>
+      <c r="D2490" t="s">
+        <v>816</v>
+      </c>
+      <c r="E2490" t="n">
+        <v>0.666666666666667</v>
+      </c>
+      <c r="F2490" t="n">
+        <v>0.636363636363636</v>
+      </c>
+      <c r="G2490" t="n">
+        <v>0.541666666666667</v>
+      </c>
+      <c r="H2490" t="n">
+        <v>0.571428571428571</v>
+      </c>
+      <c r="I2490" t="n">
+        <v>0.133333333333333</v>
+      </c>
+      <c r="J2490" t="n">
+        <v>0</v>
+      </c>
+      <c r="K2490" t="n">
+        <v>0.571428571428571</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Atualização de dados automática em 2025-07-13 12:30:03 (cron)
</commit_message>
<xml_diff>
--- a/public/docs/index_07_dim_CG.xlsx
+++ b/public/docs/index_07_dim_CG.xlsx
@@ -89712,92 +89712,92 @@
     </row>
     <row r="2466">
       <c r="A2466" t="s">
-        <v>289</v>
+        <v>263</v>
       </c>
       <c r="B2466" s="1" t="n">
         <v>46022</v>
       </c>
       <c r="C2466" s="1" t="n">
-        <v>45813</v>
+        <v>45845</v>
       </c>
       <c r="D2466" t="s">
-        <v>290</v>
+        <v>264</v>
       </c>
       <c r="E2466" t="n">
-        <v>0.515151515151515</v>
+        <v>0.666666666666667</v>
       </c>
       <c r="F2466" t="n">
-        <v>0.606060606060606</v>
+        <v>0.666666666666667</v>
       </c>
       <c r="G2466" t="n">
-        <v>0.458333333333333</v>
+        <v>0.583333333333333</v>
       </c>
       <c r="H2466" t="n">
-        <v>0.428571428571429</v>
+        <v>0.523809523809524</v>
       </c>
       <c r="I2466" t="n">
-        <v>0.4</v>
+        <v>0.133333333333333</v>
       </c>
       <c r="J2466" t="n">
-        <v>0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="K2466" t="n">
-        <v>0.285714285714286</v>
+        <v>0.571428571428571</v>
       </c>
     </row>
     <row r="2467">
       <c r="A2467" t="s">
-        <v>39</v>
+        <v>289</v>
       </c>
       <c r="B2467" s="1" t="n">
         <v>46022</v>
       </c>
       <c r="C2467" s="1" t="n">
-        <v>45842</v>
+        <v>45813</v>
       </c>
       <c r="D2467" t="s">
-        <v>40</v>
+        <v>290</v>
       </c>
       <c r="E2467" t="n">
-        <v>0.666666666666667</v>
+        <v>0.515151515151515</v>
       </c>
       <c r="F2467" t="n">
-        <v>0.666666666666667</v>
+        <v>0.606060606060606</v>
       </c>
       <c r="G2467" t="n">
-        <v>0.5</v>
+        <v>0.458333333333333</v>
       </c>
       <c r="H2467" t="n">
-        <v>0.523809523809524</v>
+        <v>0.428571428571429</v>
       </c>
       <c r="I2467" t="n">
-        <v>0.266666666666667</v>
+        <v>0.4</v>
       </c>
       <c r="J2467" t="n">
-        <v>0</v>
+        <v>0.333333333333333</v>
       </c>
       <c r="K2467" t="n">
-        <v>0.571428571428571</v>
+        <v>0.285714285714286</v>
       </c>
     </row>
     <row r="2468">
       <c r="A2468" t="s">
-        <v>831</v>
+        <v>293</v>
       </c>
       <c r="B2468" s="1" t="n">
         <v>46022</v>
       </c>
       <c r="C2468" s="1" t="n">
-        <v>45841</v>
+        <v>45845</v>
       </c>
       <c r="D2468" t="s">
-        <v>832</v>
+        <v>294</v>
       </c>
       <c r="E2468" t="n">
-        <v>0.606060606060606</v>
+        <v>0.696969696969697</v>
       </c>
       <c r="F2468" t="n">
-        <v>0.636363636363636</v>
+        <v>0.515151515151515</v>
       </c>
       <c r="G2468" t="n">
         <v>0.458333333333333</v>
@@ -89806,42 +89806,42 @@
         <v>0.571428571428571</v>
       </c>
       <c r="I2468" t="n">
-        <v>0.2</v>
+        <v>0.133333333333333</v>
       </c>
       <c r="J2468" t="n">
-        <v>0.6</v>
+        <v>0</v>
       </c>
       <c r="K2468" t="n">
-        <v>0.333333333333333</v>
+        <v>0.571428571428571</v>
       </c>
     </row>
     <row r="2469">
       <c r="A2469" t="s">
-        <v>401</v>
+        <v>39</v>
       </c>
       <c r="B2469" s="1" t="n">
         <v>46022</v>
       </c>
       <c r="C2469" s="1" t="n">
-        <v>45839</v>
+        <v>45842</v>
       </c>
       <c r="D2469" t="s">
-        <v>402</v>
+        <v>40</v>
       </c>
       <c r="E2469" t="n">
-        <v>0.575757575757576</v>
+        <v>0.666666666666667</v>
       </c>
       <c r="F2469" t="n">
-        <v>0.727272727272727</v>
+        <v>0.666666666666667</v>
       </c>
       <c r="G2469" t="n">
-        <v>0.541666666666667</v>
+        <v>0.5</v>
       </c>
       <c r="H2469" t="n">
-        <v>0.571428571428571</v>
+        <v>0.523809523809524</v>
       </c>
       <c r="I2469" t="n">
-        <v>0.8</v>
+        <v>0.266666666666667</v>
       </c>
       <c r="J2469" t="n">
         <v>0</v>
@@ -89852,57 +89852,57 @@
     </row>
     <row r="2470">
       <c r="A2470" t="s">
-        <v>860</v>
+        <v>319</v>
       </c>
       <c r="B2470" s="1" t="n">
         <v>46022</v>
       </c>
       <c r="C2470" s="1" t="n">
-        <v>45831</v>
+        <v>45849</v>
       </c>
       <c r="D2470" t="s">
-        <v>861</v>
+        <v>320</v>
       </c>
       <c r="E2470" t="n">
-        <v>0.666666666666667</v>
+        <v>0.545454545454545</v>
       </c>
       <c r="F2470" t="n">
-        <v>0.606060606060606</v>
+        <v>0.545454545454545</v>
       </c>
       <c r="G2470" t="n">
         <v>0.5</v>
       </c>
       <c r="H2470" t="n">
-        <v>0.523809523809524</v>
+        <v>0.476190476190476</v>
       </c>
       <c r="I2470" t="n">
-        <v>0.133333333333333</v>
+        <v>0.4</v>
       </c>
       <c r="J2470" t="n">
-        <v>0.466666666666667</v>
+        <v>0.333333333333333</v>
       </c>
       <c r="K2470" t="n">
-        <v>0.428571428571429</v>
+        <v>0.19047619047619</v>
       </c>
     </row>
     <row r="2471">
       <c r="A2471" t="s">
-        <v>978</v>
+        <v>831</v>
       </c>
       <c r="B2471" s="1" t="n">
         <v>46022</v>
       </c>
       <c r="C2471" s="1" t="n">
-        <v>45838</v>
+        <v>45841</v>
       </c>
       <c r="D2471" t="s">
-        <v>979</v>
+        <v>832</v>
       </c>
       <c r="E2471" t="n">
-        <v>0.454545454545455</v>
+        <v>0.606060606060606</v>
       </c>
       <c r="F2471" t="n">
-        <v>0.606060606060606</v>
+        <v>0.636363636363636</v>
       </c>
       <c r="G2471" t="n">
         <v>0.458333333333333</v>
@@ -89914,7 +89914,7 @@
         <v>0.2</v>
       </c>
       <c r="J2471" t="n">
-        <v>0.533333333333333</v>
+        <v>0.6</v>
       </c>
       <c r="K2471" t="n">
         <v>0.333333333333333</v>
@@ -89922,16 +89922,16 @@
     </row>
     <row r="2472">
       <c r="A2472" t="s">
-        <v>119</v>
+        <v>365</v>
       </c>
       <c r="B2472" s="1" t="n">
         <v>46022</v>
       </c>
       <c r="C2472" s="1" t="n">
-        <v>45834</v>
+        <v>45848</v>
       </c>
       <c r="D2472" t="s">
-        <v>120</v>
+        <v>366</v>
       </c>
       <c r="E2472" t="n">
         <v>0.606060606060606</v>
@@ -89940,16 +89940,16 @@
         <v>0.636363636363636</v>
       </c>
       <c r="G2472" t="n">
-        <v>0.625</v>
+        <v>0.583333333333333</v>
       </c>
       <c r="H2472" t="n">
         <v>0.571428571428571</v>
       </c>
       <c r="I2472" t="n">
-        <v>0.2</v>
+        <v>0.533333333333333</v>
       </c>
       <c r="J2472" t="n">
-        <v>0.4</v>
+        <v>0.266666666666667</v>
       </c>
       <c r="K2472" t="n">
         <v>0.571428571428571</v>
@@ -89957,22 +89957,22 @@
     </row>
     <row r="2473">
       <c r="A2473" t="s">
-        <v>121</v>
+        <v>401</v>
       </c>
       <c r="B2473" s="1" t="n">
         <v>46022</v>
       </c>
       <c r="C2473" s="1" t="n">
-        <v>45841</v>
+        <v>45839</v>
       </c>
       <c r="D2473" t="s">
-        <v>122</v>
+        <v>402</v>
       </c>
       <c r="E2473" t="n">
-        <v>0.545454545454545</v>
+        <v>0.575757575757576</v>
       </c>
       <c r="F2473" t="n">
-        <v>0.515151515151515</v>
+        <v>0.727272727272727</v>
       </c>
       <c r="G2473" t="n">
         <v>0.541666666666667</v>
@@ -89981,7 +89981,7 @@
         <v>0.571428571428571</v>
       </c>
       <c r="I2473" t="n">
-        <v>0.6</v>
+        <v>0.8</v>
       </c>
       <c r="J2473" t="n">
         <v>0</v>
@@ -89992,182 +89992,182 @@
     </row>
     <row r="2474">
       <c r="A2474" t="s">
-        <v>486</v>
+        <v>434</v>
       </c>
       <c r="B2474" s="1" t="n">
         <v>46022</v>
       </c>
       <c r="C2474" s="1" t="n">
-        <v>45796</v>
+        <v>45845</v>
       </c>
       <c r="D2474" t="s">
-        <v>792</v>
+        <v>435</v>
       </c>
       <c r="E2474" t="n">
+        <v>0.666666666666667</v>
+      </c>
+      <c r="F2474" t="n">
         <v>0.636363636363636</v>
       </c>
-      <c r="F2474" t="n">
-        <v>0.666666666666667</v>
-      </c>
       <c r="G2474" t="n">
-        <v>0.75</v>
+        <v>0.458333333333333</v>
       </c>
       <c r="H2474" t="n">
-        <v>0.571428571428571</v>
+        <v>0.619047619047619</v>
       </c>
       <c r="I2474" t="n">
-        <v>0.2</v>
+        <v>0.133333333333333</v>
       </c>
       <c r="J2474" t="n">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="K2474" t="n">
-        <v>0.666666666666667</v>
+        <v>0.333333333333333</v>
       </c>
     </row>
     <row r="2475">
       <c r="A2475" t="s">
-        <v>147</v>
+        <v>860</v>
       </c>
       <c r="B2475" s="1" t="n">
         <v>46022</v>
       </c>
       <c r="C2475" s="1" t="n">
-        <v>45842</v>
+        <v>45831</v>
       </c>
       <c r="D2475" t="s">
-        <v>148</v>
+        <v>861</v>
       </c>
       <c r="E2475" t="n">
-        <v>0.636363636363636</v>
+        <v>0.666666666666667</v>
       </c>
       <c r="F2475" t="n">
-        <v>0.666666666666667</v>
+        <v>0.606060606060606</v>
       </c>
       <c r="G2475" t="n">
-        <v>0.541666666666667</v>
+        <v>0.5</v>
       </c>
       <c r="H2475" t="n">
-        <v>0.571428571428571</v>
+        <v>0.523809523809524</v>
       </c>
       <c r="I2475" t="n">
-        <v>0.6</v>
+        <v>0.133333333333333</v>
       </c>
       <c r="J2475" t="n">
-        <v>0.2</v>
+        <v>0.466666666666667</v>
       </c>
       <c r="K2475" t="n">
-        <v>0.571428571428571</v>
+        <v>0.428571428571429</v>
       </c>
     </row>
     <row r="2476">
       <c r="A2476" t="s">
-        <v>547</v>
+        <v>978</v>
       </c>
       <c r="B2476" s="1" t="n">
         <v>46022</v>
       </c>
       <c r="C2476" s="1" t="n">
-        <v>45814</v>
+        <v>45838</v>
       </c>
       <c r="D2476" t="s">
-        <v>548</v>
+        <v>979</v>
       </c>
       <c r="E2476" t="n">
-        <v>0.575757575757576</v>
+        <v>0.454545454545455</v>
       </c>
       <c r="F2476" t="n">
-        <v>0.818181818181818</v>
+        <v>0.606060606060606</v>
       </c>
       <c r="G2476" t="n">
-        <v>0.416666666666667</v>
+        <v>0.458333333333333</v>
       </c>
       <c r="H2476" t="n">
-        <v>0.619047619047619</v>
+        <v>0.571428571428571</v>
       </c>
       <c r="I2476" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="J2476" t="n">
         <v>0.533333333333333</v>
       </c>
-      <c r="J2476" t="n">
-        <v>0.0666666666666667</v>
-      </c>
       <c r="K2476" t="n">
-        <v>0.428571428571429</v>
+        <v>0.333333333333333</v>
       </c>
     </row>
     <row r="2477">
       <c r="A2477" t="s">
-        <v>563</v>
+        <v>462</v>
       </c>
       <c r="B2477" s="1" t="n">
         <v>46022</v>
       </c>
       <c r="C2477" s="1" t="n">
-        <v>45835</v>
+        <v>45845</v>
       </c>
       <c r="D2477" t="s">
-        <v>564</v>
+        <v>463</v>
       </c>
       <c r="E2477" t="n">
-        <v>0.484848484848485</v>
+        <v>0.666666666666667</v>
       </c>
       <c r="F2477" t="n">
-        <v>0.636363636363636</v>
+        <v>0.515151515151515</v>
       </c>
       <c r="G2477" t="n">
-        <v>0.625</v>
+        <v>0.458333333333333</v>
       </c>
       <c r="H2477" t="n">
-        <v>0.571428571428571</v>
+        <v>0.619047619047619</v>
       </c>
       <c r="I2477" t="n">
-        <v>0.533333333333333</v>
+        <v>0.133333333333333</v>
       </c>
       <c r="J2477" t="n">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="K2477" t="n">
-        <v>0.571428571428571</v>
+        <v>0.619047619047619</v>
       </c>
     </row>
     <row r="2478">
       <c r="A2478" t="s">
-        <v>583</v>
+        <v>119</v>
       </c>
       <c r="B2478" s="1" t="n">
         <v>46022</v>
       </c>
       <c r="C2478" s="1" t="n">
-        <v>45841</v>
+        <v>45834</v>
       </c>
       <c r="D2478" t="s">
-        <v>584</v>
+        <v>120</v>
       </c>
       <c r="E2478" t="n">
-        <v>0.545454545454545</v>
+        <v>0.606060606060606</v>
       </c>
       <c r="F2478" t="n">
-        <v>0.545454545454545</v>
+        <v>0.636363636363636</v>
       </c>
       <c r="G2478" t="n">
-        <v>0.5</v>
+        <v>0.625</v>
       </c>
       <c r="H2478" t="n">
-        <v>0.476190476190476</v>
+        <v>0.571428571428571</v>
       </c>
       <c r="I2478" t="n">
-        <v>0.333333333333333</v>
+        <v>0.2</v>
       </c>
       <c r="J2478" t="n">
-        <v>0.266666666666667</v>
+        <v>0.4</v>
       </c>
       <c r="K2478" t="n">
-        <v>0.666666666666667</v>
+        <v>0.571428571428571</v>
       </c>
     </row>
     <row r="2479">
       <c r="A2479" t="s">
-        <v>193</v>
+        <v>121</v>
       </c>
       <c r="B2479" s="1" t="n">
         <v>46022</v>
@@ -90176,22 +90176,22 @@
         <v>45841</v>
       </c>
       <c r="D2479" t="s">
-        <v>194</v>
+        <v>122</v>
       </c>
       <c r="E2479" t="n">
-        <v>0.636363636363636</v>
+        <v>0.545454545454545</v>
       </c>
       <c r="F2479" t="n">
-        <v>0.666666666666667</v>
+        <v>0.515151515151515</v>
       </c>
       <c r="G2479" t="n">
-        <v>0.625</v>
+        <v>0.541666666666667</v>
       </c>
       <c r="H2479" t="n">
         <v>0.571428571428571</v>
       </c>
       <c r="I2479" t="n">
-        <v>0.2</v>
+        <v>0.6</v>
       </c>
       <c r="J2479" t="n">
         <v>0</v>
@@ -90202,69 +90202,69 @@
     </row>
     <row r="2480">
       <c r="A2480" t="s">
-        <v>617</v>
+        <v>486</v>
       </c>
       <c r="B2480" s="1" t="n">
         <v>46022</v>
       </c>
       <c r="C2480" s="1" t="n">
-        <v>45835</v>
+        <v>45796</v>
       </c>
       <c r="D2480" t="s">
-        <v>618</v>
+        <v>792</v>
       </c>
       <c r="E2480" t="n">
         <v>0.636363636363636</v>
       </c>
       <c r="F2480" t="n">
-        <v>0.454545454545455</v>
+        <v>0.666666666666667</v>
       </c>
       <c r="G2480" t="n">
-        <v>0.416666666666667</v>
+        <v>0.75</v>
       </c>
       <c r="H2480" t="n">
-        <v>0.666666666666667</v>
+        <v>0.571428571428571</v>
       </c>
       <c r="I2480" t="n">
         <v>0.2</v>
       </c>
       <c r="J2480" t="n">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="K2480" t="n">
-        <v>0.761904761904762</v>
+        <v>0.666666666666667</v>
       </c>
     </row>
     <row r="2481">
       <c r="A2481" t="s">
-        <v>627</v>
+        <v>512</v>
       </c>
       <c r="B2481" s="1" t="n">
         <v>46022</v>
       </c>
       <c r="C2481" s="1" t="n">
-        <v>45810</v>
+        <v>45846</v>
       </c>
       <c r="D2481" t="s">
-        <v>628</v>
+        <v>513</v>
       </c>
       <c r="E2481" t="n">
-        <v>0.636363636363636</v>
+        <v>0.666666666666667</v>
       </c>
       <c r="F2481" t="n">
-        <v>0.757575757575758</v>
+        <v>0.424242424242424</v>
       </c>
       <c r="G2481" t="n">
-        <v>0.541666666666667</v>
+        <v>0.5</v>
       </c>
       <c r="H2481" t="n">
-        <v>0.333333333333333</v>
+        <v>0.619047619047619</v>
       </c>
       <c r="I2481" t="n">
-        <v>0.133333333333333</v>
+        <v>0</v>
       </c>
       <c r="J2481" t="n">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="K2481" t="n">
         <v>0.571428571428571</v>
@@ -90272,104 +90272,104 @@
     </row>
     <row r="2482">
       <c r="A2482" t="s">
-        <v>631</v>
+        <v>147</v>
       </c>
       <c r="B2482" s="1" t="n">
         <v>46022</v>
       </c>
       <c r="C2482" s="1" t="n">
-        <v>45811</v>
+        <v>45842</v>
       </c>
       <c r="D2482" t="s">
-        <v>944</v>
+        <v>148</v>
       </c>
       <c r="E2482" t="n">
-        <v>0.454545454545455</v>
+        <v>0.636363636363636</v>
       </c>
       <c r="F2482" t="n">
-        <v>0.606060606060606</v>
+        <v>0.666666666666667</v>
       </c>
       <c r="G2482" t="n">
-        <v>0.625</v>
+        <v>0.541666666666667</v>
       </c>
       <c r="H2482" t="n">
         <v>0.571428571428571</v>
       </c>
       <c r="I2482" t="n">
-        <v>0.133333333333333</v>
+        <v>0.6</v>
       </c>
       <c r="J2482" t="n">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="K2482" t="n">
-        <v>0.285714285714286</v>
+        <v>0.571428571428571</v>
       </c>
     </row>
     <row r="2483">
       <c r="A2483" t="s">
-        <v>647</v>
+        <v>533</v>
       </c>
       <c r="B2483" s="1" t="n">
         <v>46022</v>
       </c>
       <c r="C2483" s="1" t="n">
-        <v>45831</v>
+        <v>45849</v>
       </c>
       <c r="D2483" t="s">
-        <v>648</v>
+        <v>534</v>
       </c>
       <c r="E2483" t="n">
+        <v>0.636363636363636</v>
+      </c>
+      <c r="F2483" t="n">
         <v>0.575757575757576</v>
-      </c>
-      <c r="F2483" t="n">
-        <v>0.545454545454545</v>
       </c>
       <c r="G2483" t="n">
         <v>0.416666666666667</v>
       </c>
       <c r="H2483" t="n">
-        <v>0.476190476190476</v>
+        <v>0.571428571428571</v>
       </c>
       <c r="I2483" t="n">
-        <v>0.466666666666667</v>
+        <v>0.2</v>
       </c>
       <c r="J2483" t="n">
-        <v>0.133333333333333</v>
+        <v>0.0666666666666667</v>
       </c>
       <c r="K2483" t="n">
-        <v>0.523809523809524</v>
+        <v>0.571428571428571</v>
       </c>
     </row>
     <row r="2484">
       <c r="A2484" t="s">
-        <v>810</v>
+        <v>545</v>
       </c>
       <c r="B2484" s="1" t="n">
-        <v>45716</v>
+        <v>46022</v>
       </c>
       <c r="C2484" s="1" t="n">
-        <v>45565</v>
+        <v>45845</v>
       </c>
       <c r="D2484" t="s">
-        <v>811</v>
+        <v>546</v>
       </c>
       <c r="E2484" t="n">
-        <v>0.666666666666667</v>
+        <v>0.636363636363636</v>
       </c>
       <c r="F2484" t="n">
-        <v>0.696969696969697</v>
+        <v>0.636363636363636</v>
       </c>
       <c r="G2484" t="n">
-        <v>0.583333333333333</v>
+        <v>0.625</v>
       </c>
       <c r="H2484" t="n">
         <v>0.571428571428571</v>
       </c>
       <c r="I2484" t="n">
-        <v>0.266666666666667</v>
+        <v>0.2</v>
       </c>
       <c r="J2484" t="n">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="K2484" t="n">
         <v>0.571428571428571</v>
@@ -90377,203 +90377,203 @@
     </row>
     <row r="2485">
       <c r="A2485" t="s">
-        <v>667</v>
+        <v>547</v>
       </c>
       <c r="B2485" s="1" t="n">
         <v>46022</v>
       </c>
       <c r="C2485" s="1" t="n">
-        <v>45832</v>
+        <v>45814</v>
       </c>
       <c r="D2485" t="s">
-        <v>668</v>
+        <v>548</v>
       </c>
       <c r="E2485" t="n">
-        <v>0.727272727272727</v>
+        <v>0.575757575757576</v>
       </c>
       <c r="F2485" t="n">
-        <v>0.636363636363636</v>
+        <v>0.818181818181818</v>
       </c>
       <c r="G2485" t="n">
-        <v>0.5</v>
+        <v>0.416666666666667</v>
       </c>
       <c r="H2485" t="n">
-        <v>0.571428571428571</v>
+        <v>0.619047619047619</v>
       </c>
       <c r="I2485" t="n">
         <v>0.533333333333333</v>
       </c>
       <c r="J2485" t="n">
-        <v>0</v>
+        <v>0.0666666666666667</v>
       </c>
       <c r="K2485" t="n">
-        <v>0.571428571428571</v>
+        <v>0.428571428571429</v>
       </c>
     </row>
     <row r="2486">
       <c r="A2486" t="s">
-        <v>675</v>
+        <v>563</v>
       </c>
       <c r="B2486" s="1" t="n">
         <v>46022</v>
       </c>
       <c r="C2486" s="1" t="n">
-        <v>45825</v>
+        <v>45835</v>
       </c>
       <c r="D2486" t="s">
-        <v>676</v>
+        <v>564</v>
       </c>
       <c r="E2486" t="n">
         <v>0.484848484848485</v>
       </c>
       <c r="F2486" t="n">
-        <v>0.484848484848485</v>
+        <v>0.636363636363636</v>
       </c>
       <c r="G2486" t="n">
-        <v>0.458333333333333</v>
+        <v>0.625</v>
       </c>
       <c r="H2486" t="n">
-        <v>0.476190476190476</v>
+        <v>0.571428571428571</v>
       </c>
       <c r="I2486" t="n">
-        <v>0.2</v>
+        <v>0.533333333333333</v>
       </c>
       <c r="J2486" t="n">
-        <v>0.133333333333333</v>
+        <v>0.2</v>
       </c>
       <c r="K2486" t="n">
-        <v>0.523809523809524</v>
+        <v>0.571428571428571</v>
       </c>
     </row>
     <row r="2487">
       <c r="A2487" t="s">
-        <v>679</v>
+        <v>583</v>
       </c>
       <c r="B2487" s="1" t="n">
         <v>46022</v>
       </c>
       <c r="C2487" s="1" t="n">
-        <v>45840</v>
+        <v>45841</v>
       </c>
       <c r="D2487" t="s">
-        <v>680</v>
+        <v>584</v>
       </c>
       <c r="E2487" t="n">
-        <v>0.636363636363636</v>
+        <v>0.545454545454545</v>
       </c>
       <c r="F2487" t="n">
-        <v>0.636363636363636</v>
+        <v>0.545454545454545</v>
       </c>
       <c r="G2487" t="n">
         <v>0.5</v>
       </c>
       <c r="H2487" t="n">
-        <v>0.571428571428571</v>
+        <v>0.476190476190476</v>
       </c>
       <c r="I2487" t="n">
-        <v>0.666666666666667</v>
+        <v>0.333333333333333</v>
       </c>
       <c r="J2487" t="n">
-        <v>0.4</v>
+        <v>0.266666666666667</v>
       </c>
       <c r="K2487" t="n">
-        <v>0.619047619047619</v>
+        <v>0.666666666666667</v>
       </c>
     </row>
     <row r="2488">
       <c r="A2488" t="s">
-        <v>812</v>
+        <v>193</v>
       </c>
       <c r="B2488" s="1" t="n">
-        <v>45838</v>
+        <v>46022</v>
       </c>
       <c r="C2488" s="1" t="n">
-        <v>45681</v>
+        <v>45841</v>
       </c>
       <c r="D2488" t="s">
-        <v>813</v>
+        <v>194</v>
       </c>
       <c r="E2488" t="n">
-        <v>0.454545454545455</v>
+        <v>0.636363636363636</v>
       </c>
       <c r="F2488" t="n">
-        <v>0.575757575757576</v>
+        <v>0.666666666666667</v>
       </c>
       <c r="G2488" t="n">
-        <v>0.541666666666667</v>
+        <v>0.625</v>
       </c>
       <c r="H2488" t="n">
         <v>0.571428571428571</v>
       </c>
       <c r="I2488" t="n">
-        <v>0.333333333333333</v>
+        <v>0.2</v>
       </c>
       <c r="J2488" t="n">
-        <v>0.133333333333333</v>
+        <v>0</v>
       </c>
       <c r="K2488" t="n">
-        <v>0.619047619047619</v>
+        <v>0.571428571428571</v>
       </c>
     </row>
     <row r="2489">
       <c r="A2489" t="s">
-        <v>721</v>
+        <v>617</v>
       </c>
       <c r="B2489" s="1" t="n">
         <v>46022</v>
       </c>
       <c r="C2489" s="1" t="n">
-        <v>45834</v>
+        <v>45835</v>
       </c>
       <c r="D2489" t="s">
-        <v>722</v>
+        <v>618</v>
       </c>
       <c r="E2489" t="n">
-        <v>0.484848484848485</v>
+        <v>0.636363636363636</v>
       </c>
       <c r="F2489" t="n">
-        <v>0.515151515151515</v>
+        <v>0.454545454545455</v>
       </c>
       <c r="G2489" t="n">
-        <v>0.458333333333333</v>
+        <v>0.416666666666667</v>
       </c>
       <c r="H2489" t="n">
-        <v>0.476190476190476</v>
+        <v>0.666666666666667</v>
       </c>
       <c r="I2489" t="n">
-        <v>0.133333333333333</v>
+        <v>0.2</v>
       </c>
       <c r="J2489" t="n">
-        <v>0.133333333333333</v>
+        <v>0</v>
       </c>
       <c r="K2489" t="n">
-        <v>0.666666666666667</v>
+        <v>0.761904761904762</v>
       </c>
     </row>
     <row r="2490">
       <c r="A2490" t="s">
-        <v>815</v>
+        <v>627</v>
       </c>
       <c r="B2490" s="1" t="n">
         <v>46022</v>
       </c>
       <c r="C2490" s="1" t="n">
-        <v>45838</v>
+        <v>45810</v>
       </c>
       <c r="D2490" t="s">
-        <v>816</v>
+        <v>628</v>
       </c>
       <c r="E2490" t="n">
-        <v>0.666666666666667</v>
+        <v>0.636363636363636</v>
       </c>
       <c r="F2490" t="n">
-        <v>0.636363636363636</v>
+        <v>0.757575757575758</v>
       </c>
       <c r="G2490" t="n">
         <v>0.541666666666667</v>
       </c>
       <c r="H2490" t="n">
-        <v>0.571428571428571</v>
+        <v>0.333333333333333</v>
       </c>
       <c r="I2490" t="n">
         <v>0.133333333333333</v>
@@ -90582,6 +90582,356 @@
         <v>0</v>
       </c>
       <c r="K2490" t="n">
+        <v>0.571428571428571</v>
+      </c>
+    </row>
+    <row r="2491">
+      <c r="A2491" t="s">
+        <v>631</v>
+      </c>
+      <c r="B2491" s="1" t="n">
+        <v>46022</v>
+      </c>
+      <c r="C2491" s="1" t="n">
+        <v>45811</v>
+      </c>
+      <c r="D2491" t="s">
+        <v>944</v>
+      </c>
+      <c r="E2491" t="n">
+        <v>0.454545454545455</v>
+      </c>
+      <c r="F2491" t="n">
+        <v>0.606060606060606</v>
+      </c>
+      <c r="G2491" t="n">
+        <v>0.625</v>
+      </c>
+      <c r="H2491" t="n">
+        <v>0.571428571428571</v>
+      </c>
+      <c r="I2491" t="n">
+        <v>0.133333333333333</v>
+      </c>
+      <c r="J2491" t="n">
+        <v>0</v>
+      </c>
+      <c r="K2491" t="n">
+        <v>0.285714285714286</v>
+      </c>
+    </row>
+    <row r="2492">
+      <c r="A2492" t="s">
+        <v>647</v>
+      </c>
+      <c r="B2492" s="1" t="n">
+        <v>46022</v>
+      </c>
+      <c r="C2492" s="1" t="n">
+        <v>45831</v>
+      </c>
+      <c r="D2492" t="s">
+        <v>648</v>
+      </c>
+      <c r="E2492" t="n">
+        <v>0.575757575757576</v>
+      </c>
+      <c r="F2492" t="n">
+        <v>0.545454545454545</v>
+      </c>
+      <c r="G2492" t="n">
+        <v>0.416666666666667</v>
+      </c>
+      <c r="H2492" t="n">
+        <v>0.476190476190476</v>
+      </c>
+      <c r="I2492" t="n">
+        <v>0.466666666666667</v>
+      </c>
+      <c r="J2492" t="n">
+        <v>0.133333333333333</v>
+      </c>
+      <c r="K2492" t="n">
+        <v>0.523809523809524</v>
+      </c>
+    </row>
+    <row r="2493">
+      <c r="A2493" t="s">
+        <v>810</v>
+      </c>
+      <c r="B2493" s="1" t="n">
+        <v>45716</v>
+      </c>
+      <c r="C2493" s="1" t="n">
+        <v>45565</v>
+      </c>
+      <c r="D2493" t="s">
+        <v>811</v>
+      </c>
+      <c r="E2493" t="n">
+        <v>0.666666666666667</v>
+      </c>
+      <c r="F2493" t="n">
+        <v>0.696969696969697</v>
+      </c>
+      <c r="G2493" t="n">
+        <v>0.583333333333333</v>
+      </c>
+      <c r="H2493" t="n">
+        <v>0.571428571428571</v>
+      </c>
+      <c r="I2493" t="n">
+        <v>0.266666666666667</v>
+      </c>
+      <c r="J2493" t="n">
+        <v>0</v>
+      </c>
+      <c r="K2493" t="n">
+        <v>0.571428571428571</v>
+      </c>
+    </row>
+    <row r="2494">
+      <c r="A2494" t="s">
+        <v>667</v>
+      </c>
+      <c r="B2494" s="1" t="n">
+        <v>46022</v>
+      </c>
+      <c r="C2494" s="1" t="n">
+        <v>45832</v>
+      </c>
+      <c r="D2494" t="s">
+        <v>668</v>
+      </c>
+      <c r="E2494" t="n">
+        <v>0.727272727272727</v>
+      </c>
+      <c r="F2494" t="n">
+        <v>0.636363636363636</v>
+      </c>
+      <c r="G2494" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="H2494" t="n">
+        <v>0.571428571428571</v>
+      </c>
+      <c r="I2494" t="n">
+        <v>0.533333333333333</v>
+      </c>
+      <c r="J2494" t="n">
+        <v>0</v>
+      </c>
+      <c r="K2494" t="n">
+        <v>0.571428571428571</v>
+      </c>
+    </row>
+    <row r="2495">
+      <c r="A2495" t="s">
+        <v>675</v>
+      </c>
+      <c r="B2495" s="1" t="n">
+        <v>46022</v>
+      </c>
+      <c r="C2495" s="1" t="n">
+        <v>45825</v>
+      </c>
+      <c r="D2495" t="s">
+        <v>676</v>
+      </c>
+      <c r="E2495" t="n">
+        <v>0.484848484848485</v>
+      </c>
+      <c r="F2495" t="n">
+        <v>0.484848484848485</v>
+      </c>
+      <c r="G2495" t="n">
+        <v>0.458333333333333</v>
+      </c>
+      <c r="H2495" t="n">
+        <v>0.476190476190476</v>
+      </c>
+      <c r="I2495" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="J2495" t="n">
+        <v>0.133333333333333</v>
+      </c>
+      <c r="K2495" t="n">
+        <v>0.523809523809524</v>
+      </c>
+    </row>
+    <row r="2496">
+      <c r="A2496" t="s">
+        <v>679</v>
+      </c>
+      <c r="B2496" s="1" t="n">
+        <v>46022</v>
+      </c>
+      <c r="C2496" s="1" t="n">
+        <v>45840</v>
+      </c>
+      <c r="D2496" t="s">
+        <v>680</v>
+      </c>
+      <c r="E2496" t="n">
+        <v>0.636363636363636</v>
+      </c>
+      <c r="F2496" t="n">
+        <v>0.636363636363636</v>
+      </c>
+      <c r="G2496" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="H2496" t="n">
+        <v>0.571428571428571</v>
+      </c>
+      <c r="I2496" t="n">
+        <v>0.666666666666667</v>
+      </c>
+      <c r="J2496" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="K2496" t="n">
+        <v>0.619047619047619</v>
+      </c>
+    </row>
+    <row r="2497">
+      <c r="A2497" t="s">
+        <v>689</v>
+      </c>
+      <c r="B2497" s="1" t="n">
+        <v>46022</v>
+      </c>
+      <c r="C2497" s="1" t="n">
+        <v>45848</v>
+      </c>
+      <c r="D2497" t="s">
+        <v>690</v>
+      </c>
+      <c r="E2497" t="n">
+        <v>0.454545454545455</v>
+      </c>
+      <c r="F2497" t="n">
+        <v>0.454545454545455</v>
+      </c>
+      <c r="G2497" t="n">
+        <v>0.333333333333333</v>
+      </c>
+      <c r="H2497" t="n">
+        <v>0.571428571428571</v>
+      </c>
+      <c r="I2497" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="J2497" t="n">
+        <v>0.266666666666667</v>
+      </c>
+      <c r="K2497" t="n">
+        <v>0.666666666666667</v>
+      </c>
+    </row>
+    <row r="2498">
+      <c r="A2498" t="s">
+        <v>812</v>
+      </c>
+      <c r="B2498" s="1" t="n">
+        <v>45838</v>
+      </c>
+      <c r="C2498" s="1" t="n">
+        <v>45681</v>
+      </c>
+      <c r="D2498" t="s">
+        <v>813</v>
+      </c>
+      <c r="E2498" t="n">
+        <v>0.454545454545455</v>
+      </c>
+      <c r="F2498" t="n">
+        <v>0.575757575757576</v>
+      </c>
+      <c r="G2498" t="n">
+        <v>0.541666666666667</v>
+      </c>
+      <c r="H2498" t="n">
+        <v>0.571428571428571</v>
+      </c>
+      <c r="I2498" t="n">
+        <v>0.333333333333333</v>
+      </c>
+      <c r="J2498" t="n">
+        <v>0.133333333333333</v>
+      </c>
+      <c r="K2498" t="n">
+        <v>0.619047619047619</v>
+      </c>
+    </row>
+    <row r="2499">
+      <c r="A2499" t="s">
+        <v>721</v>
+      </c>
+      <c r="B2499" s="1" t="n">
+        <v>46022</v>
+      </c>
+      <c r="C2499" s="1" t="n">
+        <v>45834</v>
+      </c>
+      <c r="D2499" t="s">
+        <v>722</v>
+      </c>
+      <c r="E2499" t="n">
+        <v>0.484848484848485</v>
+      </c>
+      <c r="F2499" t="n">
+        <v>0.515151515151515</v>
+      </c>
+      <c r="G2499" t="n">
+        <v>0.458333333333333</v>
+      </c>
+      <c r="H2499" t="n">
+        <v>0.476190476190476</v>
+      </c>
+      <c r="I2499" t="n">
+        <v>0.133333333333333</v>
+      </c>
+      <c r="J2499" t="n">
+        <v>0.133333333333333</v>
+      </c>
+      <c r="K2499" t="n">
+        <v>0.666666666666667</v>
+      </c>
+    </row>
+    <row r="2500">
+      <c r="A2500" t="s">
+        <v>815</v>
+      </c>
+      <c r="B2500" s="1" t="n">
+        <v>46022</v>
+      </c>
+      <c r="C2500" s="1" t="n">
+        <v>45838</v>
+      </c>
+      <c r="D2500" t="s">
+        <v>816</v>
+      </c>
+      <c r="E2500" t="n">
+        <v>0.666666666666667</v>
+      </c>
+      <c r="F2500" t="n">
+        <v>0.636363636363636</v>
+      </c>
+      <c r="G2500" t="n">
+        <v>0.541666666666667</v>
+      </c>
+      <c r="H2500" t="n">
+        <v>0.571428571428571</v>
+      </c>
+      <c r="I2500" t="n">
+        <v>0.133333333333333</v>
+      </c>
+      <c r="J2500" t="n">
+        <v>0</v>
+      </c>
+      <c r="K2500" t="n">
         <v>0.571428571428571</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualização de dados automática em 2025-07-31 18:31:32 (cron)
</commit_message>
<xml_diff>
--- a/public/docs/index_07_dim_CG.xlsx
+++ b/public/docs/index_07_dim_CG.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1028" uniqueCount="1028">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1034" uniqueCount="1034">
   <si>
     <t xml:space="preserve">CNPJ_Companhia</t>
   </si>
@@ -3096,6 +3096,24 @@
   </si>
   <si>
     <t xml:space="preserve">ATOM EDUCAÇÃO E EDITORA S.A.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">52.270.350/0001-71</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CIABRASF - CIA. BRASILEIRA DE SERVIÇOS FINANCEIROS S.A.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">52.805.925/0001-03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BELORA RDVC CITY DESENVOLVIMENTO IMOBILIÁRIO S.A.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">52.841.191/0001-18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">REVEE S.A.</t>
   </si>
 </sst>
 </file>
@@ -89712,34 +89730,34 @@
     </row>
     <row r="2466">
       <c r="A2466" t="s">
-        <v>263</v>
+        <v>13</v>
       </c>
       <c r="B2466" s="1" t="n">
         <v>46022</v>
       </c>
       <c r="C2466" s="1" t="n">
-        <v>45845</v>
+        <v>45862</v>
       </c>
       <c r="D2466" t="s">
-        <v>264</v>
+        <v>14</v>
       </c>
       <c r="E2466" t="n">
-        <v>0.666666666666667</v>
+        <v>0.636363636363636</v>
       </c>
       <c r="F2466" t="n">
-        <v>0.666666666666667</v>
+        <v>0.575757575757576</v>
       </c>
       <c r="G2466" t="n">
         <v>0.583333333333333</v>
       </c>
       <c r="H2466" t="n">
-        <v>0.523809523809524</v>
+        <v>0.571428571428571</v>
       </c>
       <c r="I2466" t="n">
-        <v>0.133333333333333</v>
+        <v>0.2</v>
       </c>
       <c r="J2466" t="n">
-        <v>0</v>
+        <v>0.266666666666667</v>
       </c>
       <c r="K2466" t="n">
         <v>0.571428571428571</v>
@@ -89747,69 +89765,69 @@
     </row>
     <row r="2467">
       <c r="A2467" t="s">
-        <v>289</v>
+        <v>259</v>
       </c>
       <c r="B2467" s="1" t="n">
         <v>46022</v>
       </c>
       <c r="C2467" s="1" t="n">
-        <v>45813</v>
+        <v>45853</v>
       </c>
       <c r="D2467" t="s">
-        <v>290</v>
+        <v>260</v>
       </c>
       <c r="E2467" t="n">
-        <v>0.515151515151515</v>
+        <v>0.484848484848485</v>
       </c>
       <c r="F2467" t="n">
-        <v>0.606060606060606</v>
+        <v>0.575757575757576</v>
       </c>
       <c r="G2467" t="n">
-        <v>0.458333333333333</v>
+        <v>0.416666666666667</v>
       </c>
       <c r="H2467" t="n">
-        <v>0.428571428571429</v>
+        <v>0.571428571428571</v>
       </c>
       <c r="I2467" t="n">
-        <v>0.4</v>
+        <v>0.133333333333333</v>
       </c>
       <c r="J2467" t="n">
-        <v>0.333333333333333</v>
+        <v>0.133333333333333</v>
       </c>
       <c r="K2467" t="n">
-        <v>0.285714285714286</v>
+        <v>0.476190476190476</v>
       </c>
     </row>
     <row r="2468">
       <c r="A2468" t="s">
-        <v>293</v>
+        <v>261</v>
       </c>
       <c r="B2468" s="1" t="n">
         <v>46022</v>
       </c>
       <c r="C2468" s="1" t="n">
-        <v>45845</v>
+        <v>45859</v>
       </c>
       <c r="D2468" t="s">
-        <v>294</v>
+        <v>262</v>
       </c>
       <c r="E2468" t="n">
-        <v>0.696969696969697</v>
+        <v>0.636363636363636</v>
       </c>
       <c r="F2468" t="n">
-        <v>0.515151515151515</v>
+        <v>0.454545454545455</v>
       </c>
       <c r="G2468" t="n">
-        <v>0.458333333333333</v>
+        <v>0.291666666666667</v>
       </c>
       <c r="H2468" t="n">
-        <v>0.571428571428571</v>
+        <v>0.666666666666667</v>
       </c>
       <c r="I2468" t="n">
-        <v>0.133333333333333</v>
+        <v>0.533333333333333</v>
       </c>
       <c r="J2468" t="n">
-        <v>0</v>
+        <v>0.466666666666667</v>
       </c>
       <c r="K2468" t="n">
         <v>0.571428571428571</v>
@@ -89817,16 +89835,16 @@
     </row>
     <row r="2469">
       <c r="A2469" t="s">
-        <v>39</v>
+        <v>263</v>
       </c>
       <c r="B2469" s="1" t="n">
         <v>46022</v>
       </c>
       <c r="C2469" s="1" t="n">
-        <v>45842</v>
+        <v>45845</v>
       </c>
       <c r="D2469" t="s">
-        <v>40</v>
+        <v>264</v>
       </c>
       <c r="E2469" t="n">
         <v>0.666666666666667</v>
@@ -89835,13 +89853,13 @@
         <v>0.666666666666667</v>
       </c>
       <c r="G2469" t="n">
-        <v>0.5</v>
+        <v>0.583333333333333</v>
       </c>
       <c r="H2469" t="n">
         <v>0.523809523809524</v>
       </c>
       <c r="I2469" t="n">
-        <v>0.266666666666667</v>
+        <v>0.133333333333333</v>
       </c>
       <c r="J2469" t="n">
         <v>0</v>
@@ -89852,28 +89870,28 @@
     </row>
     <row r="2470">
       <c r="A2470" t="s">
-        <v>319</v>
+        <v>289</v>
       </c>
       <c r="B2470" s="1" t="n">
         <v>46022</v>
       </c>
       <c r="C2470" s="1" t="n">
-        <v>45849</v>
+        <v>45813</v>
       </c>
       <c r="D2470" t="s">
-        <v>320</v>
+        <v>290</v>
       </c>
       <c r="E2470" t="n">
-        <v>0.545454545454545</v>
+        <v>0.515151515151515</v>
       </c>
       <c r="F2470" t="n">
-        <v>0.545454545454545</v>
+        <v>0.606060606060606</v>
       </c>
       <c r="G2470" t="n">
-        <v>0.5</v>
+        <v>0.458333333333333</v>
       </c>
       <c r="H2470" t="n">
-        <v>0.476190476190476</v>
+        <v>0.428571428571429</v>
       </c>
       <c r="I2470" t="n">
         <v>0.4</v>
@@ -89882,27 +89900,27 @@
         <v>0.333333333333333</v>
       </c>
       <c r="K2470" t="n">
-        <v>0.19047619047619</v>
+        <v>0.285714285714286</v>
       </c>
     </row>
     <row r="2471">
       <c r="A2471" t="s">
-        <v>831</v>
+        <v>293</v>
       </c>
       <c r="B2471" s="1" t="n">
         <v>46022</v>
       </c>
       <c r="C2471" s="1" t="n">
-        <v>45841</v>
+        <v>45845</v>
       </c>
       <c r="D2471" t="s">
-        <v>832</v>
+        <v>294</v>
       </c>
       <c r="E2471" t="n">
-        <v>0.606060606060606</v>
+        <v>0.696969696969697</v>
       </c>
       <c r="F2471" t="n">
-        <v>0.636363636363636</v>
+        <v>0.515151515151515</v>
       </c>
       <c r="G2471" t="n">
         <v>0.458333333333333</v>
@@ -89911,80 +89929,80 @@
         <v>0.571428571428571</v>
       </c>
       <c r="I2471" t="n">
-        <v>0.2</v>
+        <v>0.133333333333333</v>
       </c>
       <c r="J2471" t="n">
-        <v>0.6</v>
+        <v>0</v>
       </c>
       <c r="K2471" t="n">
-        <v>0.333333333333333</v>
+        <v>0.571428571428571</v>
       </c>
     </row>
     <row r="2472">
       <c r="A2472" t="s">
-        <v>365</v>
+        <v>748</v>
       </c>
       <c r="B2472" s="1" t="n">
         <v>46022</v>
       </c>
       <c r="C2472" s="1" t="n">
-        <v>45848</v>
+        <v>45863</v>
       </c>
       <c r="D2472" t="s">
-        <v>366</v>
+        <v>749</v>
       </c>
       <c r="E2472" t="n">
         <v>0.606060606060606</v>
       </c>
       <c r="F2472" t="n">
-        <v>0.636363636363636</v>
+        <v>0.606060606060606</v>
       </c>
       <c r="G2472" t="n">
-        <v>0.583333333333333</v>
+        <v>0.541666666666667</v>
       </c>
       <c r="H2472" t="n">
         <v>0.571428571428571</v>
       </c>
       <c r="I2472" t="n">
-        <v>0.533333333333333</v>
+        <v>0.333333333333333</v>
       </c>
       <c r="J2472" t="n">
-        <v>0.266666666666667</v>
+        <v>0.6</v>
       </c>
       <c r="K2472" t="n">
-        <v>0.571428571428571</v>
+        <v>0.666666666666667</v>
       </c>
     </row>
     <row r="2473">
       <c r="A2473" t="s">
-        <v>401</v>
+        <v>297</v>
       </c>
       <c r="B2473" s="1" t="n">
         <v>46022</v>
       </c>
       <c r="C2473" s="1" t="n">
-        <v>45839</v>
+        <v>45860</v>
       </c>
       <c r="D2473" t="s">
-        <v>402</v>
+        <v>298</v>
       </c>
       <c r="E2473" t="n">
-        <v>0.575757575757576</v>
+        <v>0.636363636363636</v>
       </c>
       <c r="F2473" t="n">
-        <v>0.727272727272727</v>
+        <v>0.606060606060606</v>
       </c>
       <c r="G2473" t="n">
-        <v>0.541666666666667</v>
+        <v>0.625</v>
       </c>
       <c r="H2473" t="n">
         <v>0.571428571428571</v>
       </c>
       <c r="I2473" t="n">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="J2473" t="n">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="K2473" t="n">
         <v>0.571428571428571</v>
@@ -89992,156 +90010,156 @@
     </row>
     <row r="2474">
       <c r="A2474" t="s">
-        <v>434</v>
+        <v>39</v>
       </c>
       <c r="B2474" s="1" t="n">
         <v>46022</v>
       </c>
       <c r="C2474" s="1" t="n">
-        <v>45845</v>
+        <v>45842</v>
       </c>
       <c r="D2474" t="s">
-        <v>435</v>
+        <v>40</v>
       </c>
       <c r="E2474" t="n">
         <v>0.666666666666667</v>
       </c>
       <c r="F2474" t="n">
-        <v>0.636363636363636</v>
+        <v>0.666666666666667</v>
       </c>
       <c r="G2474" t="n">
-        <v>0.458333333333333</v>
+        <v>0.5</v>
       </c>
       <c r="H2474" t="n">
-        <v>0.619047619047619</v>
+        <v>0.523809523809524</v>
       </c>
       <c r="I2474" t="n">
-        <v>0.133333333333333</v>
+        <v>0.266666666666667</v>
       </c>
       <c r="J2474" t="n">
         <v>0</v>
       </c>
       <c r="K2474" t="n">
-        <v>0.333333333333333</v>
+        <v>0.571428571428571</v>
       </c>
     </row>
     <row r="2475">
       <c r="A2475" t="s">
-        <v>860</v>
+        <v>299</v>
       </c>
       <c r="B2475" s="1" t="n">
         <v>46022</v>
       </c>
       <c r="C2475" s="1" t="n">
-        <v>45831</v>
+        <v>45860</v>
       </c>
       <c r="D2475" t="s">
-        <v>861</v>
+        <v>300</v>
       </c>
       <c r="E2475" t="n">
-        <v>0.666666666666667</v>
+        <v>0.454545454545455</v>
       </c>
       <c r="F2475" t="n">
-        <v>0.606060606060606</v>
+        <v>0.696969696969697</v>
       </c>
       <c r="G2475" t="n">
         <v>0.5</v>
       </c>
       <c r="H2475" t="n">
-        <v>0.523809523809524</v>
+        <v>0.619047619047619</v>
       </c>
       <c r="I2475" t="n">
         <v>0.133333333333333</v>
       </c>
       <c r="J2475" t="n">
-        <v>0.466666666666667</v>
+        <v>0.2</v>
       </c>
       <c r="K2475" t="n">
-        <v>0.428571428571429</v>
+        <v>0.571428571428571</v>
       </c>
     </row>
     <row r="2476">
       <c r="A2476" t="s">
-        <v>978</v>
+        <v>319</v>
       </c>
       <c r="B2476" s="1" t="n">
         <v>46022</v>
       </c>
       <c r="C2476" s="1" t="n">
-        <v>45838</v>
+        <v>45849</v>
       </c>
       <c r="D2476" t="s">
-        <v>979</v>
+        <v>320</v>
       </c>
       <c r="E2476" t="n">
-        <v>0.454545454545455</v>
+        <v>0.545454545454545</v>
       </c>
       <c r="F2476" t="n">
-        <v>0.606060606060606</v>
+        <v>0.545454545454545</v>
       </c>
       <c r="G2476" t="n">
-        <v>0.458333333333333</v>
+        <v>0.5</v>
       </c>
       <c r="H2476" t="n">
-        <v>0.571428571428571</v>
+        <v>0.476190476190476</v>
       </c>
       <c r="I2476" t="n">
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
       <c r="J2476" t="n">
-        <v>0.533333333333333</v>
+        <v>0.333333333333333</v>
       </c>
       <c r="K2476" t="n">
-        <v>0.333333333333333</v>
+        <v>0.19047619047619</v>
       </c>
     </row>
     <row r="2477">
       <c r="A2477" t="s">
-        <v>462</v>
+        <v>344</v>
       </c>
       <c r="B2477" s="1" t="n">
         <v>46022</v>
       </c>
       <c r="C2477" s="1" t="n">
-        <v>45845</v>
+        <v>45854</v>
       </c>
       <c r="D2477" t="s">
-        <v>463</v>
+        <v>345</v>
       </c>
       <c r="E2477" t="n">
-        <v>0.666666666666667</v>
+        <v>0.606060606060606</v>
       </c>
       <c r="F2477" t="n">
-        <v>0.515151515151515</v>
+        <v>0.606060606060606</v>
       </c>
       <c r="G2477" t="n">
-        <v>0.458333333333333</v>
+        <v>0.583333333333333</v>
       </c>
       <c r="H2477" t="n">
-        <v>0.619047619047619</v>
+        <v>0.523809523809524</v>
       </c>
       <c r="I2477" t="n">
-        <v>0.133333333333333</v>
+        <v>0.466666666666667</v>
       </c>
       <c r="J2477" t="n">
-        <v>0</v>
+        <v>0.133333333333333</v>
       </c>
       <c r="K2477" t="n">
-        <v>0.619047619047619</v>
+        <v>0.571428571428571</v>
       </c>
     </row>
     <row r="2478">
       <c r="A2478" t="s">
-        <v>119</v>
+        <v>831</v>
       </c>
       <c r="B2478" s="1" t="n">
         <v>46022</v>
       </c>
       <c r="C2478" s="1" t="n">
-        <v>45834</v>
+        <v>45841</v>
       </c>
       <c r="D2478" t="s">
-        <v>120</v>
+        <v>832</v>
       </c>
       <c r="E2478" t="n">
         <v>0.606060606060606</v>
@@ -90150,7 +90168,7 @@
         <v>0.636363636363636</v>
       </c>
       <c r="G2478" t="n">
-        <v>0.625</v>
+        <v>0.458333333333333</v>
       </c>
       <c r="H2478" t="n">
         <v>0.571428571428571</v>
@@ -90159,129 +90177,129 @@
         <v>0.2</v>
       </c>
       <c r="J2478" t="n">
-        <v>0.4</v>
+        <v>0.6</v>
       </c>
       <c r="K2478" t="n">
-        <v>0.571428571428571</v>
+        <v>0.333333333333333</v>
       </c>
     </row>
     <row r="2479">
       <c r="A2479" t="s">
-        <v>121</v>
+        <v>73</v>
       </c>
       <c r="B2479" s="1" t="n">
         <v>46022</v>
       </c>
       <c r="C2479" s="1" t="n">
-        <v>45841</v>
+        <v>45859</v>
       </c>
       <c r="D2479" t="s">
-        <v>122</v>
+        <v>74</v>
       </c>
       <c r="E2479" t="n">
-        <v>0.545454545454545</v>
+        <v>0.606060606060606</v>
       </c>
       <c r="F2479" t="n">
-        <v>0.515151515151515</v>
+        <v>0.484848484848485</v>
       </c>
       <c r="G2479" t="n">
-        <v>0.541666666666667</v>
+        <v>0.5</v>
       </c>
       <c r="H2479" t="n">
-        <v>0.571428571428571</v>
+        <v>0.476190476190476</v>
       </c>
       <c r="I2479" t="n">
-        <v>0.6</v>
+        <v>0.133333333333333</v>
       </c>
       <c r="J2479" t="n">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="K2479" t="n">
-        <v>0.571428571428571</v>
+        <v>0.619047619047619</v>
       </c>
     </row>
     <row r="2480">
       <c r="A2480" t="s">
-        <v>486</v>
+        <v>365</v>
       </c>
       <c r="B2480" s="1" t="n">
         <v>46022</v>
       </c>
       <c r="C2480" s="1" t="n">
-        <v>45796</v>
+        <v>45848</v>
       </c>
       <c r="D2480" t="s">
-        <v>792</v>
+        <v>366</v>
       </c>
       <c r="E2480" t="n">
+        <v>0.606060606060606</v>
+      </c>
+      <c r="F2480" t="n">
         <v>0.636363636363636</v>
       </c>
-      <c r="F2480" t="n">
-        <v>0.666666666666667</v>
-      </c>
       <c r="G2480" t="n">
-        <v>0.75</v>
+        <v>0.583333333333333</v>
       </c>
       <c r="H2480" t="n">
         <v>0.571428571428571</v>
       </c>
       <c r="I2480" t="n">
-        <v>0.2</v>
+        <v>0.533333333333333</v>
       </c>
       <c r="J2480" t="n">
-        <v>0.2</v>
+        <v>0.266666666666667</v>
       </c>
       <c r="K2480" t="n">
-        <v>0.666666666666667</v>
+        <v>0.571428571428571</v>
       </c>
     </row>
     <row r="2481">
       <c r="A2481" t="s">
-        <v>512</v>
+        <v>387</v>
       </c>
       <c r="B2481" s="1" t="n">
         <v>46022</v>
       </c>
       <c r="C2481" s="1" t="n">
-        <v>45846</v>
+        <v>45863</v>
       </c>
       <c r="D2481" t="s">
-        <v>513</v>
+        <v>388</v>
       </c>
       <c r="E2481" t="n">
-        <v>0.666666666666667</v>
+        <v>0.606060606060606</v>
       </c>
       <c r="F2481" t="n">
-        <v>0.424242424242424</v>
+        <v>0.606060606060606</v>
       </c>
       <c r="G2481" t="n">
-        <v>0.5</v>
+        <v>0.375</v>
       </c>
       <c r="H2481" t="n">
         <v>0.619047619047619</v>
       </c>
       <c r="I2481" t="n">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="J2481" t="n">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="K2481" t="n">
-        <v>0.571428571428571</v>
+        <v>0.333333333333333</v>
       </c>
     </row>
     <row r="2482">
       <c r="A2482" t="s">
-        <v>147</v>
+        <v>93</v>
       </c>
       <c r="B2482" s="1" t="n">
         <v>46022</v>
       </c>
       <c r="C2482" s="1" t="n">
-        <v>45842</v>
+        <v>45860</v>
       </c>
       <c r="D2482" t="s">
-        <v>148</v>
+        <v>94</v>
       </c>
       <c r="E2482" t="n">
         <v>0.636363636363636</v>
@@ -90290,86 +90308,86 @@
         <v>0.666666666666667</v>
       </c>
       <c r="G2482" t="n">
-        <v>0.541666666666667</v>
+        <v>0.458333333333333</v>
       </c>
       <c r="H2482" t="n">
-        <v>0.571428571428571</v>
+        <v>0.476190476190476</v>
       </c>
       <c r="I2482" t="n">
-        <v>0.6</v>
+        <v>0.2</v>
       </c>
       <c r="J2482" t="n">
         <v>0.2</v>
       </c>
       <c r="K2482" t="n">
-        <v>0.571428571428571</v>
+        <v>0.380952380952381</v>
       </c>
     </row>
     <row r="2483">
       <c r="A2483" t="s">
-        <v>533</v>
+        <v>95</v>
       </c>
       <c r="B2483" s="1" t="n">
         <v>46022</v>
       </c>
       <c r="C2483" s="1" t="n">
-        <v>45849</v>
+        <v>45852</v>
       </c>
       <c r="D2483" t="s">
-        <v>534</v>
+        <v>96</v>
       </c>
       <c r="E2483" t="n">
-        <v>0.636363636363636</v>
+        <v>0.515151515151515</v>
       </c>
       <c r="F2483" t="n">
-        <v>0.575757575757576</v>
+        <v>0.515151515151515</v>
       </c>
       <c r="G2483" t="n">
-        <v>0.416666666666667</v>
+        <v>0.375</v>
       </c>
       <c r="H2483" t="n">
-        <v>0.571428571428571</v>
+        <v>0.476190476190476</v>
       </c>
       <c r="I2483" t="n">
-        <v>0.2</v>
+        <v>0.266666666666667</v>
       </c>
       <c r="J2483" t="n">
-        <v>0.0666666666666667</v>
+        <v>0.333333333333333</v>
       </c>
       <c r="K2483" t="n">
-        <v>0.571428571428571</v>
+        <v>0.476190476190476</v>
       </c>
     </row>
     <row r="2484">
       <c r="A2484" t="s">
-        <v>545</v>
+        <v>401</v>
       </c>
       <c r="B2484" s="1" t="n">
         <v>46022</v>
       </c>
       <c r="C2484" s="1" t="n">
-        <v>45845</v>
+        <v>45839</v>
       </c>
       <c r="D2484" t="s">
-        <v>546</v>
+        <v>402</v>
       </c>
       <c r="E2484" t="n">
-        <v>0.636363636363636</v>
+        <v>0.575757575757576</v>
       </c>
       <c r="F2484" t="n">
-        <v>0.636363636363636</v>
+        <v>0.727272727272727</v>
       </c>
       <c r="G2484" t="n">
-        <v>0.625</v>
+        <v>0.541666666666667</v>
       </c>
       <c r="H2484" t="n">
         <v>0.571428571428571</v>
       </c>
       <c r="I2484" t="n">
-        <v>0.2</v>
+        <v>0.8</v>
       </c>
       <c r="J2484" t="n">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="K2484" t="n">
         <v>0.571428571428571</v>
@@ -90377,454 +90395,454 @@
     </row>
     <row r="2485">
       <c r="A2485" t="s">
-        <v>547</v>
+        <v>769</v>
       </c>
       <c r="B2485" s="1" t="n">
         <v>46022</v>
       </c>
       <c r="C2485" s="1" t="n">
-        <v>45814</v>
+        <v>45859</v>
       </c>
       <c r="D2485" t="s">
-        <v>548</v>
+        <v>770</v>
       </c>
       <c r="E2485" t="n">
-        <v>0.575757575757576</v>
+        <v>0.666666666666667</v>
       </c>
       <c r="F2485" t="n">
-        <v>0.818181818181818</v>
+        <v>0.666666666666667</v>
       </c>
       <c r="G2485" t="n">
-        <v>0.416666666666667</v>
+        <v>0.375</v>
       </c>
       <c r="H2485" t="n">
-        <v>0.619047619047619</v>
+        <v>0.380952380952381</v>
       </c>
       <c r="I2485" t="n">
-        <v>0.533333333333333</v>
+        <v>0.266666666666667</v>
       </c>
       <c r="J2485" t="n">
-        <v>0.0666666666666667</v>
+        <v>0.133333333333333</v>
       </c>
       <c r="K2485" t="n">
-        <v>0.428571428571429</v>
+        <v>0.666666666666667</v>
       </c>
     </row>
     <row r="2486">
       <c r="A2486" t="s">
-        <v>563</v>
+        <v>842</v>
       </c>
       <c r="B2486" s="1" t="n">
         <v>46022</v>
       </c>
       <c r="C2486" s="1" t="n">
-        <v>45835</v>
+        <v>45863</v>
       </c>
       <c r="D2486" t="s">
-        <v>564</v>
+        <v>843</v>
       </c>
       <c r="E2486" t="n">
-        <v>0.484848484848485</v>
+        <v>0.606060606060606</v>
       </c>
       <c r="F2486" t="n">
-        <v>0.636363636363636</v>
+        <v>0.696969696969697</v>
       </c>
       <c r="G2486" t="n">
-        <v>0.625</v>
+        <v>0.541666666666667</v>
       </c>
       <c r="H2486" t="n">
-        <v>0.571428571428571</v>
+        <v>0.380952380952381</v>
       </c>
       <c r="I2486" t="n">
-        <v>0.533333333333333</v>
+        <v>0.266666666666667</v>
       </c>
       <c r="J2486" t="n">
-        <v>0.2</v>
+        <v>0.133333333333333</v>
       </c>
       <c r="K2486" t="n">
-        <v>0.571428571428571</v>
+        <v>0.333333333333333</v>
       </c>
     </row>
     <row r="2487">
       <c r="A2487" t="s">
-        <v>583</v>
+        <v>103</v>
       </c>
       <c r="B2487" s="1" t="n">
         <v>46022</v>
       </c>
       <c r="C2487" s="1" t="n">
-        <v>45841</v>
+        <v>45853</v>
       </c>
       <c r="D2487" t="s">
-        <v>584</v>
+        <v>104</v>
       </c>
       <c r="E2487" t="n">
-        <v>0.545454545454545</v>
+        <v>0.636363636363636</v>
       </c>
       <c r="F2487" t="n">
-        <v>0.545454545454545</v>
+        <v>0.636363636363636</v>
       </c>
       <c r="G2487" t="n">
-        <v>0.5</v>
+        <v>0.625</v>
       </c>
       <c r="H2487" t="n">
-        <v>0.476190476190476</v>
+        <v>0.571428571428571</v>
       </c>
       <c r="I2487" t="n">
-        <v>0.333333333333333</v>
+        <v>0.133333333333333</v>
       </c>
       <c r="J2487" t="n">
-        <v>0.266666666666667</v>
+        <v>0.4</v>
       </c>
       <c r="K2487" t="n">
-        <v>0.666666666666667</v>
+        <v>0.571428571428571</v>
       </c>
     </row>
     <row r="2488">
       <c r="A2488" t="s">
-        <v>193</v>
+        <v>434</v>
       </c>
       <c r="B2488" s="1" t="n">
         <v>46022</v>
       </c>
       <c r="C2488" s="1" t="n">
-        <v>45841</v>
+        <v>45845</v>
       </c>
       <c r="D2488" t="s">
-        <v>194</v>
+        <v>435</v>
       </c>
       <c r="E2488" t="n">
+        <v>0.666666666666667</v>
+      </c>
+      <c r="F2488" t="n">
         <v>0.636363636363636</v>
       </c>
-      <c r="F2488" t="n">
-        <v>0.666666666666667</v>
-      </c>
       <c r="G2488" t="n">
-        <v>0.625</v>
+        <v>0.458333333333333</v>
       </c>
       <c r="H2488" t="n">
-        <v>0.571428571428571</v>
+        <v>0.619047619047619</v>
       </c>
       <c r="I2488" t="n">
-        <v>0.2</v>
+        <v>0.133333333333333</v>
       </c>
       <c r="J2488" t="n">
         <v>0</v>
       </c>
       <c r="K2488" t="n">
-        <v>0.571428571428571</v>
+        <v>0.333333333333333</v>
       </c>
     </row>
     <row r="2489">
       <c r="A2489" t="s">
-        <v>617</v>
+        <v>438</v>
       </c>
       <c r="B2489" s="1" t="n">
         <v>46022</v>
       </c>
       <c r="C2489" s="1" t="n">
-        <v>45835</v>
+        <v>45855</v>
       </c>
       <c r="D2489" t="s">
-        <v>618</v>
+        <v>439</v>
       </c>
       <c r="E2489" t="n">
         <v>0.636363636363636</v>
       </c>
       <c r="F2489" t="n">
-        <v>0.454545454545455</v>
+        <v>0.606060606060606</v>
       </c>
       <c r="G2489" t="n">
-        <v>0.416666666666667</v>
+        <v>0.375</v>
       </c>
       <c r="H2489" t="n">
-        <v>0.666666666666667</v>
+        <v>0.523809523809524</v>
       </c>
       <c r="I2489" t="n">
         <v>0.2</v>
       </c>
       <c r="J2489" t="n">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="K2489" t="n">
-        <v>0.761904761904762</v>
+        <v>0.619047619047619</v>
       </c>
     </row>
     <row r="2490">
       <c r="A2490" t="s">
-        <v>627</v>
+        <v>860</v>
       </c>
       <c r="B2490" s="1" t="n">
         <v>46022</v>
       </c>
       <c r="C2490" s="1" t="n">
-        <v>45810</v>
+        <v>45831</v>
       </c>
       <c r="D2490" t="s">
-        <v>628</v>
+        <v>861</v>
       </c>
       <c r="E2490" t="n">
-        <v>0.636363636363636</v>
+        <v>0.666666666666667</v>
       </c>
       <c r="F2490" t="n">
-        <v>0.757575757575758</v>
+        <v>0.606060606060606</v>
       </c>
       <c r="G2490" t="n">
-        <v>0.541666666666667</v>
+        <v>0.5</v>
       </c>
       <c r="H2490" t="n">
-        <v>0.333333333333333</v>
+        <v>0.523809523809524</v>
       </c>
       <c r="I2490" t="n">
         <v>0.133333333333333</v>
       </c>
       <c r="J2490" t="n">
-        <v>0</v>
+        <v>0.466666666666667</v>
       </c>
       <c r="K2490" t="n">
-        <v>0.571428571428571</v>
+        <v>0.428571428571429</v>
       </c>
     </row>
     <row r="2491">
       <c r="A2491" t="s">
-        <v>631</v>
+        <v>872</v>
       </c>
       <c r="B2491" s="1" t="n">
         <v>46022</v>
       </c>
       <c r="C2491" s="1" t="n">
-        <v>45811</v>
+        <v>45863</v>
       </c>
       <c r="D2491" t="s">
-        <v>944</v>
+        <v>873</v>
       </c>
       <c r="E2491" t="n">
-        <v>0.454545454545455</v>
+        <v>0.666666666666667</v>
       </c>
       <c r="F2491" t="n">
-        <v>0.606060606060606</v>
+        <v>0.545454545454545</v>
       </c>
       <c r="G2491" t="n">
-        <v>0.625</v>
+        <v>0.458333333333333</v>
       </c>
       <c r="H2491" t="n">
-        <v>0.571428571428571</v>
+        <v>0.523809523809524</v>
       </c>
       <c r="I2491" t="n">
-        <v>0.133333333333333</v>
+        <v>0.2</v>
       </c>
       <c r="J2491" t="n">
-        <v>0</v>
+        <v>0.466666666666667</v>
       </c>
       <c r="K2491" t="n">
-        <v>0.285714285714286</v>
+        <v>0.714285714285714</v>
       </c>
     </row>
     <row r="2492">
       <c r="A2492" t="s">
-        <v>647</v>
+        <v>978</v>
       </c>
       <c r="B2492" s="1" t="n">
         <v>46022</v>
       </c>
       <c r="C2492" s="1" t="n">
-        <v>45831</v>
+        <v>45838</v>
       </c>
       <c r="D2492" t="s">
-        <v>648</v>
+        <v>979</v>
       </c>
       <c r="E2492" t="n">
-        <v>0.575757575757576</v>
+        <v>0.454545454545455</v>
       </c>
       <c r="F2492" t="n">
-        <v>0.545454545454545</v>
+        <v>0.606060606060606</v>
       </c>
       <c r="G2492" t="n">
-        <v>0.416666666666667</v>
+        <v>0.458333333333333</v>
       </c>
       <c r="H2492" t="n">
-        <v>0.476190476190476</v>
+        <v>0.571428571428571</v>
       </c>
       <c r="I2492" t="n">
-        <v>0.466666666666667</v>
+        <v>0.2</v>
       </c>
       <c r="J2492" t="n">
-        <v>0.133333333333333</v>
+        <v>0.533333333333333</v>
       </c>
       <c r="K2492" t="n">
-        <v>0.523809523809524</v>
+        <v>0.333333333333333</v>
       </c>
     </row>
     <row r="2493">
       <c r="A2493" t="s">
-        <v>810</v>
+        <v>878</v>
       </c>
       <c r="B2493" s="1" t="n">
-        <v>45716</v>
+        <v>46022</v>
       </c>
       <c r="C2493" s="1" t="n">
-        <v>45565</v>
+        <v>45861</v>
       </c>
       <c r="D2493" t="s">
-        <v>811</v>
+        <v>879</v>
       </c>
       <c r="E2493" t="n">
-        <v>0.666666666666667</v>
+        <v>0.575757575757576</v>
       </c>
       <c r="F2493" t="n">
-        <v>0.696969696969697</v>
+        <v>0.636363636363636</v>
       </c>
       <c r="G2493" t="n">
-        <v>0.583333333333333</v>
+        <v>0.458333333333333</v>
       </c>
       <c r="H2493" t="n">
         <v>0.571428571428571</v>
       </c>
       <c r="I2493" t="n">
-        <v>0.266666666666667</v>
+        <v>0</v>
       </c>
       <c r="J2493" t="n">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="K2493" t="n">
-        <v>0.571428571428571</v>
+        <v>0.285714285714286</v>
       </c>
     </row>
     <row r="2494">
       <c r="A2494" t="s">
-        <v>667</v>
+        <v>462</v>
       </c>
       <c r="B2494" s="1" t="n">
         <v>46022</v>
       </c>
       <c r="C2494" s="1" t="n">
-        <v>45832</v>
+        <v>45845</v>
       </c>
       <c r="D2494" t="s">
-        <v>668</v>
+        <v>463</v>
       </c>
       <c r="E2494" t="n">
-        <v>0.727272727272727</v>
+        <v>0.666666666666667</v>
       </c>
       <c r="F2494" t="n">
-        <v>0.636363636363636</v>
+        <v>0.515151515151515</v>
       </c>
       <c r="G2494" t="n">
-        <v>0.5</v>
+        <v>0.458333333333333</v>
       </c>
       <c r="H2494" t="n">
-        <v>0.571428571428571</v>
+        <v>0.619047619047619</v>
       </c>
       <c r="I2494" t="n">
-        <v>0.533333333333333</v>
+        <v>0.133333333333333</v>
       </c>
       <c r="J2494" t="n">
         <v>0</v>
       </c>
       <c r="K2494" t="n">
-        <v>0.571428571428571</v>
+        <v>0.619047619047619</v>
       </c>
     </row>
     <row r="2495">
       <c r="A2495" t="s">
-        <v>675</v>
+        <v>117</v>
       </c>
       <c r="B2495" s="1" t="n">
         <v>46022</v>
       </c>
       <c r="C2495" s="1" t="n">
-        <v>45825</v>
+        <v>45863</v>
       </c>
       <c r="D2495" t="s">
-        <v>676</v>
+        <v>118</v>
       </c>
       <c r="E2495" t="n">
-        <v>0.484848484848485</v>
+        <v>0.636363636363636</v>
       </c>
       <c r="F2495" t="n">
-        <v>0.484848484848485</v>
+        <v>0.545454545454545</v>
       </c>
       <c r="G2495" t="n">
-        <v>0.458333333333333</v>
+        <v>0.541666666666667</v>
       </c>
       <c r="H2495" t="n">
-        <v>0.476190476190476</v>
+        <v>0.571428571428571</v>
       </c>
       <c r="I2495" t="n">
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
       <c r="J2495" t="n">
-        <v>0.133333333333333</v>
+        <v>0.4</v>
       </c>
       <c r="K2495" t="n">
-        <v>0.523809523809524</v>
+        <v>0.571428571428571</v>
       </c>
     </row>
     <row r="2496">
       <c r="A2496" t="s">
-        <v>679</v>
+        <v>119</v>
       </c>
       <c r="B2496" s="1" t="n">
         <v>46022</v>
       </c>
       <c r="C2496" s="1" t="n">
-        <v>45840</v>
+        <v>45834</v>
       </c>
       <c r="D2496" t="s">
-        <v>680</v>
+        <v>120</v>
       </c>
       <c r="E2496" t="n">
-        <v>0.636363636363636</v>
+        <v>0.606060606060606</v>
       </c>
       <c r="F2496" t="n">
         <v>0.636363636363636</v>
       </c>
       <c r="G2496" t="n">
-        <v>0.5</v>
+        <v>0.625</v>
       </c>
       <c r="H2496" t="n">
         <v>0.571428571428571</v>
       </c>
       <c r="I2496" t="n">
-        <v>0.666666666666667</v>
+        <v>0.2</v>
       </c>
       <c r="J2496" t="n">
         <v>0.4</v>
       </c>
       <c r="K2496" t="n">
-        <v>0.619047619047619</v>
+        <v>0.571428571428571</v>
       </c>
     </row>
     <row r="2497">
       <c r="A2497" t="s">
-        <v>689</v>
+        <v>886</v>
       </c>
       <c r="B2497" s="1" t="n">
         <v>46022</v>
       </c>
       <c r="C2497" s="1" t="n">
-        <v>45848</v>
+        <v>45859</v>
       </c>
       <c r="D2497" t="s">
-        <v>690</v>
+        <v>887</v>
       </c>
       <c r="E2497" t="n">
-        <v>0.454545454545455</v>
+        <v>0.727272727272727</v>
       </c>
       <c r="F2497" t="n">
-        <v>0.454545454545455</v>
+        <v>0.787878787878788</v>
       </c>
       <c r="G2497" t="n">
+        <v>0.416666666666667</v>
+      </c>
+      <c r="H2497" t="n">
+        <v>0.428571428571429</v>
+      </c>
+      <c r="I2497" t="n">
         <v>0.333333333333333</v>
       </c>
-      <c r="H2497" t="n">
-        <v>0.571428571428571</v>
-      </c>
-      <c r="I2497" t="n">
-        <v>0.2</v>
-      </c>
       <c r="J2497" t="n">
-        <v>0.266666666666667</v>
+        <v>0.4</v>
       </c>
       <c r="K2497" t="n">
         <v>0.666666666666667</v>
@@ -90832,22 +90850,22 @@
     </row>
     <row r="2498">
       <c r="A2498" t="s">
-        <v>812</v>
+        <v>121</v>
       </c>
       <c r="B2498" s="1" t="n">
-        <v>45838</v>
+        <v>46022</v>
       </c>
       <c r="C2498" s="1" t="n">
-        <v>45681</v>
+        <v>45841</v>
       </c>
       <c r="D2498" t="s">
-        <v>813</v>
+        <v>122</v>
       </c>
       <c r="E2498" t="n">
-        <v>0.454545454545455</v>
+        <v>0.545454545454545</v>
       </c>
       <c r="F2498" t="n">
-        <v>0.575757575757576</v>
+        <v>0.515151515151515</v>
       </c>
       <c r="G2498" t="n">
         <v>0.541666666666667</v>
@@ -90856,36 +90874,36 @@
         <v>0.571428571428571</v>
       </c>
       <c r="I2498" t="n">
-        <v>0.333333333333333</v>
+        <v>0.6</v>
       </c>
       <c r="J2498" t="n">
-        <v>0.133333333333333</v>
+        <v>0</v>
       </c>
       <c r="K2498" t="n">
-        <v>0.619047619047619</v>
+        <v>0.571428571428571</v>
       </c>
     </row>
     <row r="2499">
       <c r="A2499" t="s">
-        <v>721</v>
+        <v>894</v>
       </c>
       <c r="B2499" s="1" t="n">
         <v>46022</v>
       </c>
       <c r="C2499" s="1" t="n">
-        <v>45834</v>
+        <v>45862</v>
       </c>
       <c r="D2499" t="s">
-        <v>722</v>
+        <v>895</v>
       </c>
       <c r="E2499" t="n">
-        <v>0.484848484848485</v>
+        <v>0.606060606060606</v>
       </c>
       <c r="F2499" t="n">
-        <v>0.515151515151515</v>
+        <v>0.727272727272727</v>
       </c>
       <c r="G2499" t="n">
-        <v>0.458333333333333</v>
+        <v>0.375</v>
       </c>
       <c r="H2499" t="n">
         <v>0.476190476190476</v>
@@ -90894,44 +90912,1654 @@
         <v>0.133333333333333</v>
       </c>
       <c r="J2499" t="n">
-        <v>0.133333333333333</v>
+        <v>0.4</v>
       </c>
       <c r="K2499" t="n">
-        <v>0.666666666666667</v>
+        <v>0.285714285714286</v>
       </c>
     </row>
     <row r="2500">
       <c r="A2500" t="s">
-        <v>815</v>
+        <v>486</v>
       </c>
       <c r="B2500" s="1" t="n">
         <v>46022</v>
       </c>
       <c r="C2500" s="1" t="n">
+        <v>45796</v>
+      </c>
+      <c r="D2500" t="s">
+        <v>792</v>
+      </c>
+      <c r="E2500" t="n">
+        <v>0.636363636363636</v>
+      </c>
+      <c r="F2500" t="n">
+        <v>0.666666666666667</v>
+      </c>
+      <c r="G2500" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="H2500" t="n">
+        <v>0.571428571428571</v>
+      </c>
+      <c r="I2500" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="J2500" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="K2500" t="n">
+        <v>0.666666666666667</v>
+      </c>
+    </row>
+    <row r="2501">
+      <c r="A2501" t="s">
+        <v>1010</v>
+      </c>
+      <c r="B2501" s="1" t="n">
+        <v>46022</v>
+      </c>
+      <c r="C2501" s="1" t="n">
+        <v>45860</v>
+      </c>
+      <c r="D2501" t="s">
+        <v>1011</v>
+      </c>
+      <c r="E2501" t="n">
+        <v>0.575757575757576</v>
+      </c>
+      <c r="F2501" t="n">
+        <v>0.757575757575758</v>
+      </c>
+      <c r="G2501" t="n">
+        <v>0.541666666666667</v>
+      </c>
+      <c r="H2501" t="n">
+        <v>0.619047619047619</v>
+      </c>
+      <c r="I2501" t="n">
+        <v>0</v>
+      </c>
+      <c r="J2501" t="n">
+        <v>0</v>
+      </c>
+      <c r="K2501" t="n">
+        <v>0.619047619047619</v>
+      </c>
+    </row>
+    <row r="2502">
+      <c r="A2502" t="s">
+        <v>512</v>
+      </c>
+      <c r="B2502" s="1" t="n">
+        <v>46022</v>
+      </c>
+      <c r="C2502" s="1" t="n">
+        <v>45846</v>
+      </c>
+      <c r="D2502" t="s">
+        <v>513</v>
+      </c>
+      <c r="E2502" t="n">
+        <v>0.666666666666667</v>
+      </c>
+      <c r="F2502" t="n">
+        <v>0.424242424242424</v>
+      </c>
+      <c r="G2502" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="H2502" t="n">
+        <v>0.619047619047619</v>
+      </c>
+      <c r="I2502" t="n">
+        <v>0</v>
+      </c>
+      <c r="J2502" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="K2502" t="n">
+        <v>0.571428571428571</v>
+      </c>
+    </row>
+    <row r="2503">
+      <c r="A2503" t="s">
+        <v>990</v>
+      </c>
+      <c r="B2503" s="1" t="n">
+        <v>46022</v>
+      </c>
+      <c r="C2503" s="1" t="n">
+        <v>45859</v>
+      </c>
+      <c r="D2503" t="s">
+        <v>991</v>
+      </c>
+      <c r="E2503" t="n">
+        <v>0.636363636363636</v>
+      </c>
+      <c r="F2503" t="n">
+        <v>0.787878787878788</v>
+      </c>
+      <c r="G2503" t="n">
+        <v>0.416666666666667</v>
+      </c>
+      <c r="H2503" t="n">
+        <v>0.476190476190476</v>
+      </c>
+      <c r="I2503" t="n">
+        <v>0.266666666666667</v>
+      </c>
+      <c r="J2503" t="n">
+        <v>0</v>
+      </c>
+      <c r="K2503" t="n">
+        <v>0.571428571428571</v>
+      </c>
+    </row>
+    <row r="2504">
+      <c r="A2504" t="s">
+        <v>147</v>
+      </c>
+      <c r="B2504" s="1" t="n">
+        <v>46022</v>
+      </c>
+      <c r="C2504" s="1" t="n">
+        <v>45842</v>
+      </c>
+      <c r="D2504" t="s">
+        <v>148</v>
+      </c>
+      <c r="E2504" t="n">
+        <v>0.636363636363636</v>
+      </c>
+      <c r="F2504" t="n">
+        <v>0.666666666666667</v>
+      </c>
+      <c r="G2504" t="n">
+        <v>0.541666666666667</v>
+      </c>
+      <c r="H2504" t="n">
+        <v>0.571428571428571</v>
+      </c>
+      <c r="I2504" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="J2504" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="K2504" t="n">
+        <v>0.571428571428571</v>
+      </c>
+    </row>
+    <row r="2505">
+      <c r="A2505" t="s">
+        <v>153</v>
+      </c>
+      <c r="B2505" s="1" t="n">
+        <v>46022</v>
+      </c>
+      <c r="C2505" s="1" t="n">
+        <v>45863</v>
+      </c>
+      <c r="D2505" t="s">
+        <v>154</v>
+      </c>
+      <c r="E2505" t="n">
+        <v>0.666666666666667</v>
+      </c>
+      <c r="F2505" t="n">
+        <v>0.515151515151515</v>
+      </c>
+      <c r="G2505" t="n">
+        <v>0.541666666666667</v>
+      </c>
+      <c r="H2505" t="n">
+        <v>0.428571428571429</v>
+      </c>
+      <c r="I2505" t="n">
+        <v>0.333333333333333</v>
+      </c>
+      <c r="J2505" t="n">
+        <v>0</v>
+      </c>
+      <c r="K2505" t="n">
+        <v>0.619047619047619</v>
+      </c>
+    </row>
+    <row r="2506">
+      <c r="A2506" t="s">
+        <v>992</v>
+      </c>
+      <c r="B2506" s="1" t="n">
+        <v>46022</v>
+      </c>
+      <c r="C2506" s="1" t="n">
+        <v>45856</v>
+      </c>
+      <c r="D2506" t="s">
+        <v>993</v>
+      </c>
+      <c r="E2506" t="n">
+        <v>0.606060606060606</v>
+      </c>
+      <c r="F2506" t="n">
+        <v>0.636363636363636</v>
+      </c>
+      <c r="G2506" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="H2506" t="n">
+        <v>0.476190476190476</v>
+      </c>
+      <c r="I2506" t="n">
+        <v>0</v>
+      </c>
+      <c r="J2506" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="K2506" t="n">
+        <v>0.666666666666667</v>
+      </c>
+    </row>
+    <row r="2507">
+      <c r="A2507" t="s">
+        <v>533</v>
+      </c>
+      <c r="B2507" s="1" t="n">
+        <v>46022</v>
+      </c>
+      <c r="C2507" s="1" t="n">
+        <v>45849</v>
+      </c>
+      <c r="D2507" t="s">
+        <v>534</v>
+      </c>
+      <c r="E2507" t="n">
+        <v>0.636363636363636</v>
+      </c>
+      <c r="F2507" t="n">
+        <v>0.575757575757576</v>
+      </c>
+      <c r="G2507" t="n">
+        <v>0.416666666666667</v>
+      </c>
+      <c r="H2507" t="n">
+        <v>0.571428571428571</v>
+      </c>
+      <c r="I2507" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="J2507" t="n">
+        <v>0.0666666666666667</v>
+      </c>
+      <c r="K2507" t="n">
+        <v>0.571428571428571</v>
+      </c>
+    </row>
+    <row r="2508">
+      <c r="A2508" t="s">
+        <v>161</v>
+      </c>
+      <c r="B2508" s="1" t="n">
+        <v>46022</v>
+      </c>
+      <c r="C2508" s="1" t="n">
+        <v>45862</v>
+      </c>
+      <c r="D2508" t="s">
+        <v>162</v>
+      </c>
+      <c r="E2508" t="n">
+        <v>0.636363636363636</v>
+      </c>
+      <c r="F2508" t="n">
+        <v>0.636363636363636</v>
+      </c>
+      <c r="G2508" t="n">
+        <v>0.625</v>
+      </c>
+      <c r="H2508" t="n">
+        <v>0.571428571428571</v>
+      </c>
+      <c r="I2508" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="J2508" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="K2508" t="n">
+        <v>0.571428571428571</v>
+      </c>
+    </row>
+    <row r="2509">
+      <c r="A2509" t="s">
+        <v>545</v>
+      </c>
+      <c r="B2509" s="1" t="n">
+        <v>46022</v>
+      </c>
+      <c r="C2509" s="1" t="n">
+        <v>45845</v>
+      </c>
+      <c r="D2509" t="s">
+        <v>546</v>
+      </c>
+      <c r="E2509" t="n">
+        <v>0.636363636363636</v>
+      </c>
+      <c r="F2509" t="n">
+        <v>0.636363636363636</v>
+      </c>
+      <c r="G2509" t="n">
+        <v>0.625</v>
+      </c>
+      <c r="H2509" t="n">
+        <v>0.571428571428571</v>
+      </c>
+      <c r="I2509" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="J2509" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="K2509" t="n">
+        <v>0.571428571428571</v>
+      </c>
+    </row>
+    <row r="2510">
+      <c r="A2510" t="s">
+        <v>547</v>
+      </c>
+      <c r="B2510" s="1" t="n">
+        <v>46022</v>
+      </c>
+      <c r="C2510" s="1" t="n">
+        <v>45814</v>
+      </c>
+      <c r="D2510" t="s">
+        <v>548</v>
+      </c>
+      <c r="E2510" t="n">
+        <v>0.575757575757576</v>
+      </c>
+      <c r="F2510" t="n">
+        <v>0.818181818181818</v>
+      </c>
+      <c r="G2510" t="n">
+        <v>0.416666666666667</v>
+      </c>
+      <c r="H2510" t="n">
+        <v>0.619047619047619</v>
+      </c>
+      <c r="I2510" t="n">
+        <v>0.533333333333333</v>
+      </c>
+      <c r="J2510" t="n">
+        <v>0.0666666666666667</v>
+      </c>
+      <c r="K2510" t="n">
+        <v>0.428571428571429</v>
+      </c>
+    </row>
+    <row r="2511">
+      <c r="A2511" t="s">
+        <v>551</v>
+      </c>
+      <c r="B2511" s="1" t="n">
+        <v>46022</v>
+      </c>
+      <c r="C2511" s="1" t="n">
+        <v>45861</v>
+      </c>
+      <c r="D2511" t="s">
+        <v>552</v>
+      </c>
+      <c r="E2511" t="n">
+        <v>0.606060606060606</v>
+      </c>
+      <c r="F2511" t="n">
+        <v>0.696969696969697</v>
+      </c>
+      <c r="G2511" t="n">
+        <v>0.625</v>
+      </c>
+      <c r="H2511" t="n">
+        <v>0.571428571428571</v>
+      </c>
+      <c r="I2511" t="n">
+        <v>0</v>
+      </c>
+      <c r="J2511" t="n">
+        <v>0</v>
+      </c>
+      <c r="K2511" t="n">
+        <v>0.428571428571429</v>
+      </c>
+    </row>
+    <row r="2512">
+      <c r="A2512" t="s">
+        <v>933</v>
+      </c>
+      <c r="B2512" s="1" t="n">
+        <v>46022</v>
+      </c>
+      <c r="C2512" s="1" t="n">
+        <v>45861</v>
+      </c>
+      <c r="D2512" t="s">
+        <v>934</v>
+      </c>
+      <c r="E2512" t="n">
+        <v>0.606060606060606</v>
+      </c>
+      <c r="F2512" t="n">
+        <v>0.757575757575758</v>
+      </c>
+      <c r="G2512" t="n">
+        <v>0.541666666666667</v>
+      </c>
+      <c r="H2512" t="n">
+        <v>0.571428571428571</v>
+      </c>
+      <c r="I2512" t="n">
+        <v>0</v>
+      </c>
+      <c r="J2512" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="K2512" t="n">
+        <v>0.333333333333333</v>
+      </c>
+    </row>
+    <row r="2513">
+      <c r="A2513" t="s">
+        <v>563</v>
+      </c>
+      <c r="B2513" s="1" t="n">
+        <v>46022</v>
+      </c>
+      <c r="C2513" s="1" t="n">
+        <v>45835</v>
+      </c>
+      <c r="D2513" t="s">
+        <v>564</v>
+      </c>
+      <c r="E2513" t="n">
+        <v>0.484848484848485</v>
+      </c>
+      <c r="F2513" t="n">
+        <v>0.636363636363636</v>
+      </c>
+      <c r="G2513" t="n">
+        <v>0.625</v>
+      </c>
+      <c r="H2513" t="n">
+        <v>0.571428571428571</v>
+      </c>
+      <c r="I2513" t="n">
+        <v>0.533333333333333</v>
+      </c>
+      <c r="J2513" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="K2513" t="n">
+        <v>0.571428571428571</v>
+      </c>
+    </row>
+    <row r="2514">
+      <c r="A2514" t="s">
+        <v>1028</v>
+      </c>
+      <c r="B2514" s="1" t="n">
+        <v>46022</v>
+      </c>
+      <c r="C2514" s="1" t="n">
+        <v>45861</v>
+      </c>
+      <c r="D2514" t="s">
+        <v>1029</v>
+      </c>
+      <c r="E2514" t="n">
+        <v>0.545454545454545</v>
+      </c>
+      <c r="F2514" t="n">
+        <v>0.666666666666667</v>
+      </c>
+      <c r="G2514" t="n">
+        <v>0.458333333333333</v>
+      </c>
+      <c r="H2514" t="n">
+        <v>0.571428571428571</v>
+      </c>
+      <c r="I2514" t="n">
+        <v>0</v>
+      </c>
+      <c r="J2514" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="K2514" t="n">
+        <v>0.285714285714286</v>
+      </c>
+    </row>
+    <row r="2515">
+      <c r="A2515" t="s">
+        <v>1030</v>
+      </c>
+      <c r="B2515" s="1" t="n">
+        <v>46022</v>
+      </c>
+      <c r="C2515" s="1" t="n">
+        <v>45861</v>
+      </c>
+      <c r="D2515" t="s">
+        <v>1031</v>
+      </c>
+      <c r="E2515" t="n">
+        <v>0.545454545454545</v>
+      </c>
+      <c r="F2515" t="n">
+        <v>0.666666666666667</v>
+      </c>
+      <c r="G2515" t="n">
+        <v>0.458333333333333</v>
+      </c>
+      <c r="H2515" t="n">
+        <v>0.571428571428571</v>
+      </c>
+      <c r="I2515" t="n">
+        <v>0</v>
+      </c>
+      <c r="J2515" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="K2515" t="n">
+        <v>0.285714285714286</v>
+      </c>
+    </row>
+    <row r="2516">
+      <c r="A2516" t="s">
+        <v>1032</v>
+      </c>
+      <c r="B2516" s="1" t="n">
+        <v>46022</v>
+      </c>
+      <c r="C2516" s="1" t="n">
+        <v>45861</v>
+      </c>
+      <c r="D2516" t="s">
+        <v>1033</v>
+      </c>
+      <c r="E2516" t="n">
+        <v>0.545454545454545</v>
+      </c>
+      <c r="F2516" t="n">
+        <v>0.666666666666667</v>
+      </c>
+      <c r="G2516" t="n">
+        <v>0.458333333333333</v>
+      </c>
+      <c r="H2516" t="n">
+        <v>0.571428571428571</v>
+      </c>
+      <c r="I2516" t="n">
+        <v>0</v>
+      </c>
+      <c r="J2516" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="K2516" t="n">
+        <v>0.285714285714286</v>
+      </c>
+    </row>
+    <row r="2517">
+      <c r="A2517" t="s">
+        <v>583</v>
+      </c>
+      <c r="B2517" s="1" t="n">
+        <v>46022</v>
+      </c>
+      <c r="C2517" s="1" t="n">
+        <v>45841</v>
+      </c>
+      <c r="D2517" t="s">
+        <v>584</v>
+      </c>
+      <c r="E2517" t="n">
+        <v>0.545454545454545</v>
+      </c>
+      <c r="F2517" t="n">
+        <v>0.545454545454545</v>
+      </c>
+      <c r="G2517" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="H2517" t="n">
+        <v>0.476190476190476</v>
+      </c>
+      <c r="I2517" t="n">
+        <v>0.333333333333333</v>
+      </c>
+      <c r="J2517" t="n">
+        <v>0.266666666666667</v>
+      </c>
+      <c r="K2517" t="n">
+        <v>0.666666666666667</v>
+      </c>
+    </row>
+    <row r="2518">
+      <c r="A2518" t="s">
+        <v>587</v>
+      </c>
+      <c r="B2518" s="1" t="n">
+        <v>46022</v>
+      </c>
+      <c r="C2518" s="1" t="n">
+        <v>45853</v>
+      </c>
+      <c r="D2518" t="s">
+        <v>588</v>
+      </c>
+      <c r="E2518" t="n">
+        <v>0.454545454545455</v>
+      </c>
+      <c r="F2518" t="n">
+        <v>0.606060606060606</v>
+      </c>
+      <c r="G2518" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="H2518" t="n">
+        <v>0.523809523809524</v>
+      </c>
+      <c r="I2518" t="n">
+        <v>0.133333333333333</v>
+      </c>
+      <c r="J2518" t="n">
+        <v>0.133333333333333</v>
+      </c>
+      <c r="K2518" t="n">
+        <v>0.714285714285714</v>
+      </c>
+    </row>
+    <row r="2519">
+      <c r="A2519" t="s">
+        <v>595</v>
+      </c>
+      <c r="B2519" s="1" t="n">
+        <v>46022</v>
+      </c>
+      <c r="C2519" s="1" t="n">
+        <v>45853</v>
+      </c>
+      <c r="D2519" t="s">
+        <v>596</v>
+      </c>
+      <c r="E2519" t="n">
+        <v>0.545454545454545</v>
+      </c>
+      <c r="F2519" t="n">
+        <v>0.515151515151515</v>
+      </c>
+      <c r="G2519" t="n">
+        <v>0.333333333333333</v>
+      </c>
+      <c r="H2519" t="n">
+        <v>0.476190476190476</v>
+      </c>
+      <c r="I2519" t="n">
+        <v>0.133333333333333</v>
+      </c>
+      <c r="J2519" t="n">
+        <v>0.133333333333333</v>
+      </c>
+      <c r="K2519" t="n">
+        <v>0.476190476190476</v>
+      </c>
+    </row>
+    <row r="2520">
+      <c r="A2520" t="s">
+        <v>597</v>
+      </c>
+      <c r="B2520" s="1" t="n">
+        <v>46022</v>
+      </c>
+      <c r="C2520" s="1" t="n">
+        <v>45862</v>
+      </c>
+      <c r="D2520" t="s">
+        <v>598</v>
+      </c>
+      <c r="E2520" t="n">
+        <v>0.636363636363636</v>
+      </c>
+      <c r="F2520" t="n">
+        <v>0.666666666666667</v>
+      </c>
+      <c r="G2520" t="n">
+        <v>0.583333333333333</v>
+      </c>
+      <c r="H2520" t="n">
+        <v>0.571428571428571</v>
+      </c>
+      <c r="I2520" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="J2520" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="K2520" t="n">
+        <v>0.571428571428571</v>
+      </c>
+    </row>
+    <row r="2521">
+      <c r="A2521" t="s">
+        <v>605</v>
+      </c>
+      <c r="B2521" s="1" t="n">
+        <v>46022</v>
+      </c>
+      <c r="C2521" s="1" t="n">
+        <v>45853</v>
+      </c>
+      <c r="D2521" t="s">
+        <v>606</v>
+      </c>
+      <c r="E2521" t="n">
+        <v>0.606060606060606</v>
+      </c>
+      <c r="F2521" t="n">
+        <v>0.484848484848485</v>
+      </c>
+      <c r="G2521" t="n">
+        <v>0.333333333333333</v>
+      </c>
+      <c r="H2521" t="n">
+        <v>0.523809523809524</v>
+      </c>
+      <c r="I2521" t="n">
+        <v>0.333333333333333</v>
+      </c>
+      <c r="J2521" t="n">
+        <v>0.133333333333333</v>
+      </c>
+      <c r="K2521" t="n">
+        <v>0.380952380952381</v>
+      </c>
+    </row>
+    <row r="2522">
+      <c r="A2522" t="s">
+        <v>607</v>
+      </c>
+      <c r="B2522" s="1" t="n">
+        <v>46022</v>
+      </c>
+      <c r="C2522" s="1" t="n">
+        <v>45863</v>
+      </c>
+      <c r="D2522" t="s">
+        <v>608</v>
+      </c>
+      <c r="E2522" t="n">
+        <v>0.757575757575758</v>
+      </c>
+      <c r="F2522" t="n">
+        <v>0.575757575757576</v>
+      </c>
+      <c r="G2522" t="n">
+        <v>0.416666666666667</v>
+      </c>
+      <c r="H2522" t="n">
+        <v>0.571428571428571</v>
+      </c>
+      <c r="I2522" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="J2522" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="K2522" t="n">
+        <v>0.428571428571429</v>
+      </c>
+    </row>
+    <row r="2523">
+      <c r="A2523" t="s">
+        <v>193</v>
+      </c>
+      <c r="B2523" s="1" t="n">
+        <v>46022</v>
+      </c>
+      <c r="C2523" s="1" t="n">
+        <v>45841</v>
+      </c>
+      <c r="D2523" t="s">
+        <v>194</v>
+      </c>
+      <c r="E2523" t="n">
+        <v>0.636363636363636</v>
+      </c>
+      <c r="F2523" t="n">
+        <v>0.666666666666667</v>
+      </c>
+      <c r="G2523" t="n">
+        <v>0.625</v>
+      </c>
+      <c r="H2523" t="n">
+        <v>0.571428571428571</v>
+      </c>
+      <c r="I2523" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="J2523" t="n">
+        <v>0</v>
+      </c>
+      <c r="K2523" t="n">
+        <v>0.571428571428571</v>
+      </c>
+    </row>
+    <row r="2524">
+      <c r="A2524" t="s">
+        <v>617</v>
+      </c>
+      <c r="B2524" s="1" t="n">
+        <v>46022</v>
+      </c>
+      <c r="C2524" s="1" t="n">
+        <v>45835</v>
+      </c>
+      <c r="D2524" t="s">
+        <v>618</v>
+      </c>
+      <c r="E2524" t="n">
+        <v>0.636363636363636</v>
+      </c>
+      <c r="F2524" t="n">
+        <v>0.454545454545455</v>
+      </c>
+      <c r="G2524" t="n">
+        <v>0.416666666666667</v>
+      </c>
+      <c r="H2524" t="n">
+        <v>0.666666666666667</v>
+      </c>
+      <c r="I2524" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="J2524" t="n">
+        <v>0</v>
+      </c>
+      <c r="K2524" t="n">
+        <v>0.761904761904762</v>
+      </c>
+    </row>
+    <row r="2525">
+      <c r="A2525" t="s">
+        <v>625</v>
+      </c>
+      <c r="B2525" s="1" t="n">
+        <v>46022</v>
+      </c>
+      <c r="C2525" s="1" t="n">
+        <v>45853</v>
+      </c>
+      <c r="D2525" t="s">
+        <v>626</v>
+      </c>
+      <c r="E2525" t="n">
+        <v>0.515151515151515</v>
+      </c>
+      <c r="F2525" t="n">
+        <v>0.545454545454545</v>
+      </c>
+      <c r="G2525" t="n">
+        <v>0.666666666666667</v>
+      </c>
+      <c r="H2525" t="n">
+        <v>0.571428571428571</v>
+      </c>
+      <c r="I2525" t="n">
+        <v>0.0666666666666667</v>
+      </c>
+      <c r="J2525" t="n">
+        <v>0.133333333333333</v>
+      </c>
+      <c r="K2525" t="n">
+        <v>0.238095238095238</v>
+      </c>
+    </row>
+    <row r="2526">
+      <c r="A2526" t="s">
+        <v>627</v>
+      </c>
+      <c r="B2526" s="1" t="n">
+        <v>46022</v>
+      </c>
+      <c r="C2526" s="1" t="n">
+        <v>45810</v>
+      </c>
+      <c r="D2526" t="s">
+        <v>628</v>
+      </c>
+      <c r="E2526" t="n">
+        <v>0.636363636363636</v>
+      </c>
+      <c r="F2526" t="n">
+        <v>0.757575757575758</v>
+      </c>
+      <c r="G2526" t="n">
+        <v>0.541666666666667</v>
+      </c>
+      <c r="H2526" t="n">
+        <v>0.333333333333333</v>
+      </c>
+      <c r="I2526" t="n">
+        <v>0.133333333333333</v>
+      </c>
+      <c r="J2526" t="n">
+        <v>0</v>
+      </c>
+      <c r="K2526" t="n">
+        <v>0.571428571428571</v>
+      </c>
+    </row>
+    <row r="2527">
+      <c r="A2527" t="s">
+        <v>631</v>
+      </c>
+      <c r="B2527" s="1" t="n">
+        <v>46022</v>
+      </c>
+      <c r="C2527" s="1" t="n">
+        <v>45811</v>
+      </c>
+      <c r="D2527" t="s">
+        <v>944</v>
+      </c>
+      <c r="E2527" t="n">
+        <v>0.454545454545455</v>
+      </c>
+      <c r="F2527" t="n">
+        <v>0.606060606060606</v>
+      </c>
+      <c r="G2527" t="n">
+        <v>0.625</v>
+      </c>
+      <c r="H2527" t="n">
+        <v>0.571428571428571</v>
+      </c>
+      <c r="I2527" t="n">
+        <v>0.133333333333333</v>
+      </c>
+      <c r="J2527" t="n">
+        <v>0</v>
+      </c>
+      <c r="K2527" t="n">
+        <v>0.285714285714286</v>
+      </c>
+    </row>
+    <row r="2528">
+      <c r="A2528" t="s">
+        <v>945</v>
+      </c>
+      <c r="B2528" s="1" t="n">
+        <v>46022</v>
+      </c>
+      <c r="C2528" s="1" t="n">
+        <v>45863</v>
+      </c>
+      <c r="D2528" t="s">
+        <v>946</v>
+      </c>
+      <c r="E2528" t="n">
+        <v>0.606060606060606</v>
+      </c>
+      <c r="F2528" t="n">
+        <v>0.727272727272727</v>
+      </c>
+      <c r="G2528" t="n">
+        <v>0.625</v>
+      </c>
+      <c r="H2528" t="n">
+        <v>0.571428571428571</v>
+      </c>
+      <c r="I2528" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="J2528" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="K2528" t="n">
+        <v>0.285714285714286</v>
+      </c>
+    </row>
+    <row r="2529">
+      <c r="A2529" t="s">
+        <v>647</v>
+      </c>
+      <c r="B2529" s="1" t="n">
+        <v>46022</v>
+      </c>
+      <c r="C2529" s="1" t="n">
+        <v>45831</v>
+      </c>
+      <c r="D2529" t="s">
+        <v>648</v>
+      </c>
+      <c r="E2529" t="n">
+        <v>0.575757575757576</v>
+      </c>
+      <c r="F2529" t="n">
+        <v>0.545454545454545</v>
+      </c>
+      <c r="G2529" t="n">
+        <v>0.416666666666667</v>
+      </c>
+      <c r="H2529" t="n">
+        <v>0.476190476190476</v>
+      </c>
+      <c r="I2529" t="n">
+        <v>0.466666666666667</v>
+      </c>
+      <c r="J2529" t="n">
+        <v>0.133333333333333</v>
+      </c>
+      <c r="K2529" t="n">
+        <v>0.523809523809524</v>
+      </c>
+    </row>
+    <row r="2530">
+      <c r="A2530" t="s">
+        <v>810</v>
+      </c>
+      <c r="B2530" s="1" t="n">
+        <v>45716</v>
+      </c>
+      <c r="C2530" s="1" t="n">
+        <v>45565</v>
+      </c>
+      <c r="D2530" t="s">
+        <v>811</v>
+      </c>
+      <c r="E2530" t="n">
+        <v>0.666666666666667</v>
+      </c>
+      <c r="F2530" t="n">
+        <v>0.696969696969697</v>
+      </c>
+      <c r="G2530" t="n">
+        <v>0.583333333333333</v>
+      </c>
+      <c r="H2530" t="n">
+        <v>0.571428571428571</v>
+      </c>
+      <c r="I2530" t="n">
+        <v>0.266666666666667</v>
+      </c>
+      <c r="J2530" t="n">
+        <v>0</v>
+      </c>
+      <c r="K2530" t="n">
+        <v>0.571428571428571</v>
+      </c>
+    </row>
+    <row r="2531">
+      <c r="A2531" t="s">
+        <v>655</v>
+      </c>
+      <c r="B2531" s="1" t="n">
+        <v>46022</v>
+      </c>
+      <c r="C2531" s="1" t="n">
+        <v>45863</v>
+      </c>
+      <c r="D2531" t="s">
+        <v>656</v>
+      </c>
+      <c r="E2531" t="n">
+        <v>0.575757575757576</v>
+      </c>
+      <c r="F2531" t="n">
+        <v>0.636363636363636</v>
+      </c>
+      <c r="G2531" t="n">
+        <v>0.541666666666667</v>
+      </c>
+      <c r="H2531" t="n">
+        <v>0.571428571428571</v>
+      </c>
+      <c r="I2531" t="n">
+        <v>0.133333333333333</v>
+      </c>
+      <c r="J2531" t="n">
+        <v>0.466666666666667</v>
+      </c>
+      <c r="K2531" t="n">
+        <v>0.571428571428571</v>
+      </c>
+    </row>
+    <row r="2532">
+      <c r="A2532" t="s">
+        <v>217</v>
+      </c>
+      <c r="B2532" s="1" t="n">
+        <v>46022</v>
+      </c>
+      <c r="C2532" s="1" t="n">
+        <v>45856</v>
+      </c>
+      <c r="D2532" t="s">
+        <v>218</v>
+      </c>
+      <c r="E2532" t="n">
+        <v>0.606060606060606</v>
+      </c>
+      <c r="F2532" t="n">
+        <v>0.727272727272727</v>
+      </c>
+      <c r="G2532" t="n">
+        <v>0.583333333333333</v>
+      </c>
+      <c r="H2532" t="n">
+        <v>0.476190476190476</v>
+      </c>
+      <c r="I2532" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="J2532" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="K2532" t="n">
+        <v>0.571428571428571</v>
+      </c>
+    </row>
+    <row r="2533">
+      <c r="A2533" t="s">
+        <v>667</v>
+      </c>
+      <c r="B2533" s="1" t="n">
+        <v>46022</v>
+      </c>
+      <c r="C2533" s="1" t="n">
+        <v>45832</v>
+      </c>
+      <c r="D2533" t="s">
+        <v>668</v>
+      </c>
+      <c r="E2533" t="n">
+        <v>0.727272727272727</v>
+      </c>
+      <c r="F2533" t="n">
+        <v>0.636363636363636</v>
+      </c>
+      <c r="G2533" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="H2533" t="n">
+        <v>0.571428571428571</v>
+      </c>
+      <c r="I2533" t="n">
+        <v>0.533333333333333</v>
+      </c>
+      <c r="J2533" t="n">
+        <v>0</v>
+      </c>
+      <c r="K2533" t="n">
+        <v>0.571428571428571</v>
+      </c>
+    </row>
+    <row r="2534">
+      <c r="A2534" t="s">
+        <v>669</v>
+      </c>
+      <c r="B2534" s="1" t="n">
+        <v>46022</v>
+      </c>
+      <c r="C2534" s="1" t="n">
+        <v>45852</v>
+      </c>
+      <c r="D2534" t="s">
+        <v>670</v>
+      </c>
+      <c r="E2534" t="n">
+        <v>0.454545454545455</v>
+      </c>
+      <c r="F2534" t="n">
+        <v>0.545454545454545</v>
+      </c>
+      <c r="G2534" t="n">
+        <v>0.541666666666667</v>
+      </c>
+      <c r="H2534" t="n">
+        <v>0.380952380952381</v>
+      </c>
+      <c r="I2534" t="n">
+        <v>0.133333333333333</v>
+      </c>
+      <c r="J2534" t="n">
+        <v>0.133333333333333</v>
+      </c>
+      <c r="K2534" t="n">
+        <v>0.571428571428571</v>
+      </c>
+    </row>
+    <row r="2535">
+      <c r="A2535" t="s">
+        <v>671</v>
+      </c>
+      <c r="B2535" s="1" t="n">
+        <v>46022</v>
+      </c>
+      <c r="C2535" s="1" t="n">
+        <v>45862</v>
+      </c>
+      <c r="D2535" t="s">
+        <v>672</v>
+      </c>
+      <c r="E2535" t="n">
+        <v>0.424242424242424</v>
+      </c>
+      <c r="F2535" t="n">
+        <v>0.545454545454545</v>
+      </c>
+      <c r="G2535" t="n">
+        <v>0.458333333333333</v>
+      </c>
+      <c r="H2535" t="n">
+        <v>0.428571428571429</v>
+      </c>
+      <c r="I2535" t="n">
+        <v>0.133333333333333</v>
+      </c>
+      <c r="J2535" t="n">
+        <v>0</v>
+      </c>
+      <c r="K2535" t="n">
+        <v>0.428571428571429</v>
+      </c>
+    </row>
+    <row r="2536">
+      <c r="A2536" t="s">
+        <v>675</v>
+      </c>
+      <c r="B2536" s="1" t="n">
+        <v>46022</v>
+      </c>
+      <c r="C2536" s="1" t="n">
+        <v>45825</v>
+      </c>
+      <c r="D2536" t="s">
+        <v>676</v>
+      </c>
+      <c r="E2536" t="n">
+        <v>0.484848484848485</v>
+      </c>
+      <c r="F2536" t="n">
+        <v>0.484848484848485</v>
+      </c>
+      <c r="G2536" t="n">
+        <v>0.458333333333333</v>
+      </c>
+      <c r="H2536" t="n">
+        <v>0.476190476190476</v>
+      </c>
+      <c r="I2536" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="J2536" t="n">
+        <v>0.133333333333333</v>
+      </c>
+      <c r="K2536" t="n">
+        <v>0.523809523809524</v>
+      </c>
+    </row>
+    <row r="2537">
+      <c r="A2537" t="s">
+        <v>679</v>
+      </c>
+      <c r="B2537" s="1" t="n">
+        <v>46022</v>
+      </c>
+      <c r="C2537" s="1" t="n">
+        <v>45840</v>
+      </c>
+      <c r="D2537" t="s">
+        <v>680</v>
+      </c>
+      <c r="E2537" t="n">
+        <v>0.636363636363636</v>
+      </c>
+      <c r="F2537" t="n">
+        <v>0.636363636363636</v>
+      </c>
+      <c r="G2537" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="H2537" t="n">
+        <v>0.571428571428571</v>
+      </c>
+      <c r="I2537" t="n">
+        <v>0.666666666666667</v>
+      </c>
+      <c r="J2537" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="K2537" t="n">
+        <v>0.619047619047619</v>
+      </c>
+    </row>
+    <row r="2538">
+      <c r="A2538" t="s">
+        <v>689</v>
+      </c>
+      <c r="B2538" s="1" t="n">
+        <v>46022</v>
+      </c>
+      <c r="C2538" s="1" t="n">
+        <v>45848</v>
+      </c>
+      <c r="D2538" t="s">
+        <v>690</v>
+      </c>
+      <c r="E2538" t="n">
+        <v>0.454545454545455</v>
+      </c>
+      <c r="F2538" t="n">
+        <v>0.454545454545455</v>
+      </c>
+      <c r="G2538" t="n">
+        <v>0.333333333333333</v>
+      </c>
+      <c r="H2538" t="n">
+        <v>0.571428571428571</v>
+      </c>
+      <c r="I2538" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="J2538" t="n">
+        <v>0.266666666666667</v>
+      </c>
+      <c r="K2538" t="n">
+        <v>0.666666666666667</v>
+      </c>
+    </row>
+    <row r="2539">
+      <c r="A2539" t="s">
+        <v>701</v>
+      </c>
+      <c r="B2539" s="1" t="n">
+        <v>46022</v>
+      </c>
+      <c r="C2539" s="1" t="n">
+        <v>45863</v>
+      </c>
+      <c r="D2539" t="s">
+        <v>702</v>
+      </c>
+      <c r="E2539" t="n">
+        <v>0.575757575757576</v>
+      </c>
+      <c r="F2539" t="n">
+        <v>0.666666666666667</v>
+      </c>
+      <c r="G2539" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="H2539" t="n">
+        <v>0.619047619047619</v>
+      </c>
+      <c r="I2539" t="n">
+        <v>0.133333333333333</v>
+      </c>
+      <c r="J2539" t="n">
+        <v>0</v>
+      </c>
+      <c r="K2539" t="n">
+        <v>0.428571428571429</v>
+      </c>
+    </row>
+    <row r="2540">
+      <c r="A2540" t="s">
+        <v>812</v>
+      </c>
+      <c r="B2540" s="1" t="n">
         <v>45838</v>
       </c>
-      <c r="D2500" t="s">
+      <c r="C2540" s="1" t="n">
+        <v>45681</v>
+      </c>
+      <c r="D2540" t="s">
+        <v>813</v>
+      </c>
+      <c r="E2540" t="n">
+        <v>0.454545454545455</v>
+      </c>
+      <c r="F2540" t="n">
+        <v>0.575757575757576</v>
+      </c>
+      <c r="G2540" t="n">
+        <v>0.541666666666667</v>
+      </c>
+      <c r="H2540" t="n">
+        <v>0.571428571428571</v>
+      </c>
+      <c r="I2540" t="n">
+        <v>0.333333333333333</v>
+      </c>
+      <c r="J2540" t="n">
+        <v>0.133333333333333</v>
+      </c>
+      <c r="K2540" t="n">
+        <v>0.619047619047619</v>
+      </c>
+    </row>
+    <row r="2541">
+      <c r="A2541" t="s">
+        <v>721</v>
+      </c>
+      <c r="B2541" s="1" t="n">
+        <v>46022</v>
+      </c>
+      <c r="C2541" s="1" t="n">
+        <v>45834</v>
+      </c>
+      <c r="D2541" t="s">
+        <v>722</v>
+      </c>
+      <c r="E2541" t="n">
+        <v>0.484848484848485</v>
+      </c>
+      <c r="F2541" t="n">
+        <v>0.515151515151515</v>
+      </c>
+      <c r="G2541" t="n">
+        <v>0.458333333333333</v>
+      </c>
+      <c r="H2541" t="n">
+        <v>0.476190476190476</v>
+      </c>
+      <c r="I2541" t="n">
+        <v>0.133333333333333</v>
+      </c>
+      <c r="J2541" t="n">
+        <v>0.133333333333333</v>
+      </c>
+      <c r="K2541" t="n">
+        <v>0.666666666666667</v>
+      </c>
+    </row>
+    <row r="2542">
+      <c r="A2542" t="s">
+        <v>725</v>
+      </c>
+      <c r="B2542" s="1" t="n">
+        <v>46022</v>
+      </c>
+      <c r="C2542" s="1" t="n">
+        <v>45859</v>
+      </c>
+      <c r="D2542" t="s">
+        <v>726</v>
+      </c>
+      <c r="E2542" t="n">
+        <v>0.454545454545455</v>
+      </c>
+      <c r="F2542" t="n">
+        <v>0.454545454545455</v>
+      </c>
+      <c r="G2542" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="H2542" t="n">
+        <v>0.571428571428571</v>
+      </c>
+      <c r="I2542" t="n">
+        <v>0.266666666666667</v>
+      </c>
+      <c r="J2542" t="n">
+        <v>0.333333333333333</v>
+      </c>
+      <c r="K2542" t="n">
+        <v>0.571428571428571</v>
+      </c>
+    </row>
+    <row r="2543">
+      <c r="A2543" t="s">
+        <v>237</v>
+      </c>
+      <c r="B2543" s="1" t="n">
+        <v>46022</v>
+      </c>
+      <c r="C2543" s="1" t="n">
+        <v>45855</v>
+      </c>
+      <c r="D2543" t="s">
+        <v>238</v>
+      </c>
+      <c r="E2543" t="n">
+        <v>0.636363636363636</v>
+      </c>
+      <c r="F2543" t="n">
+        <v>0.636363636363636</v>
+      </c>
+      <c r="G2543" t="n">
+        <v>0.583333333333333</v>
+      </c>
+      <c r="H2543" t="n">
+        <v>0.571428571428571</v>
+      </c>
+      <c r="I2543" t="n">
+        <v>0.666666666666667</v>
+      </c>
+      <c r="J2543" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="K2543" t="n">
+        <v>0.571428571428571</v>
+      </c>
+    </row>
+    <row r="2544">
+      <c r="A2544" t="s">
+        <v>729</v>
+      </c>
+      <c r="B2544" s="1" t="n">
+        <v>46022</v>
+      </c>
+      <c r="C2544" s="1" t="n">
+        <v>45863</v>
+      </c>
+      <c r="D2544" t="s">
+        <v>730</v>
+      </c>
+      <c r="E2544" t="n">
+        <v>0.636363636363636</v>
+      </c>
+      <c r="F2544" t="n">
+        <v>0.545454545454545</v>
+      </c>
+      <c r="G2544" t="n">
+        <v>0.458333333333333</v>
+      </c>
+      <c r="H2544" t="n">
+        <v>0.619047619047619</v>
+      </c>
+      <c r="I2544" t="n">
+        <v>0.133333333333333</v>
+      </c>
+      <c r="J2544" t="n">
+        <v>0.133333333333333</v>
+      </c>
+      <c r="K2544" t="n">
+        <v>0.476190476190476</v>
+      </c>
+    </row>
+    <row r="2545">
+      <c r="A2545" t="s">
+        <v>737</v>
+      </c>
+      <c r="B2545" s="1" t="n">
+        <v>46022</v>
+      </c>
+      <c r="C2545" s="1" t="n">
+        <v>45859</v>
+      </c>
+      <c r="D2545" t="s">
+        <v>738</v>
+      </c>
+      <c r="E2545" t="n">
+        <v>0.484848484848485</v>
+      </c>
+      <c r="F2545" t="n">
+        <v>0.575757575757576</v>
+      </c>
+      <c r="G2545" t="n">
+        <v>0.583333333333333</v>
+      </c>
+      <c r="H2545" t="n">
+        <v>0.619047619047619</v>
+      </c>
+      <c r="I2545" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="J2545" t="n">
+        <v>0.0666666666666667</v>
+      </c>
+      <c r="K2545" t="n">
+        <v>0.428571428571429</v>
+      </c>
+    </row>
+    <row r="2546">
+      <c r="A2546" t="s">
+        <v>815</v>
+      </c>
+      <c r="B2546" s="1" t="n">
+        <v>46022</v>
+      </c>
+      <c r="C2546" s="1" t="n">
+        <v>45838</v>
+      </c>
+      <c r="D2546" t="s">
         <v>816</v>
       </c>
-      <c r="E2500" t="n">
-        <v>0.666666666666667</v>
-      </c>
-      <c r="F2500" t="n">
+      <c r="E2546" t="n">
+        <v>0.666666666666667</v>
+      </c>
+      <c r="F2546" t="n">
         <v>0.636363636363636</v>
       </c>
-      <c r="G2500" t="n">
+      <c r="G2546" t="n">
         <v>0.541666666666667</v>
       </c>
-      <c r="H2500" t="n">
-        <v>0.571428571428571</v>
-      </c>
-      <c r="I2500" t="n">
-        <v>0.133333333333333</v>
-      </c>
-      <c r="J2500" t="n">
-        <v>0</v>
-      </c>
-      <c r="K2500" t="n">
+      <c r="H2546" t="n">
+        <v>0.571428571428571</v>
+      </c>
+      <c r="I2546" t="n">
+        <v>0.133333333333333</v>
+      </c>
+      <c r="J2546" t="n">
+        <v>0</v>
+      </c>
+      <c r="K2546" t="n">
         <v>0.571428571428571</v>
       </c>
     </row>

</xml_diff>